<commit_message>
add test_voucher to case\interface\inland
</commit_message>
<xml_diff>
--- a/case/src/http/inland.xlsx
+++ b/case/src/http/inland.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22320" windowHeight="9825" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="28080" windowHeight="13065" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="simplepay_recharge_spend" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200">
   <si>
     <t>Test suite名称</t>
   </si>
@@ -802,6 +802,9 @@
     <t>消费折扣券，ratio&lt;1</t>
   </si>
   <si>
+    <t>\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\</t>
+  </si>
+  <si>
     <t>会员红包券</t>
   </si>
 </sst>
@@ -810,11 +813,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -871,22 +874,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -899,8 +895,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -908,7 +905,21 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -930,7 +941,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -938,38 +949,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -983,9 +963,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -998,9 +978,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1046,7 +1049,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1058,31 +1103,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,19 +1115,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1118,13 +1127,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1142,31 +1145,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1178,43 +1211,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1243,26 +1246,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1278,39 +1266,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1340,6 +1295,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1348,10 +1351,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="2">
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -1360,133 +1363,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="23" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="18" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="34" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -3489,7 +3492,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3640,19 +3643,20 @@
         <v>193</v>
       </c>
       <c r="C8" s="17">
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>2</v>
       </c>
       <c r="D8" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <f ca="1">RANDBETWEEN(1,9998)</f>
+        <v>2427</v>
       </c>
       <c r="E8" s="17">
-        <f ca="1" t="shared" ref="E8:E12" si="0">RANDBETWEEN(D8,10)</f>
-        <v>9</v>
+        <f ca="1">RANDBETWEEN(D8,9999)</f>
+        <v>5014</v>
       </c>
       <c r="F8" s="17">
-        <f ca="1" t="shared" ref="F8:F12" si="1">ROUND(RAND(),2)</f>
-        <v>0.57</v>
+        <f ca="1" t="shared" ref="F8:F12" si="0">ROUND(RAND(),2)</f>
+        <v>0.02</v>
       </c>
       <c r="G8" s="18"/>
       <c r="H8" s="17"/>
@@ -3661,7 +3665,7 @@
       <c r="K8" s="17"/>
       <c r="L8" s="17">
         <f ca="1">RANDBETWEEN(0,1)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" s="17"/>
       <c r="N8" t="s">
@@ -3676,19 +3680,20 @@
         <v>194</v>
       </c>
       <c r="C9" s="17">
-        <v>1</v>
-      </c>
-      <c r="D9" s="17">
         <f ca="1">RANDBETWEEN(1,10)</f>
         <v>8</v>
       </c>
+      <c r="D9" s="17">
+        <f ca="1">RANDBETWEEN(1,9998)</f>
+        <v>2464</v>
+      </c>
       <c r="E9" s="17">
-        <f ca="1">RANDBETWEEN(D9+0.01,10)</f>
-        <v>9</v>
+        <f ca="1">RANDBETWEEN(D9,9999)</f>
+        <v>4432</v>
       </c>
       <c r="F9" s="17">
-        <f ca="1" t="shared" si="1"/>
-        <v>0.86</v>
+        <f ca="1" t="shared" si="0"/>
+        <v>0.25</v>
       </c>
       <c r="G9" s="17"/>
       <c r="H9" s="17"/>
@@ -3696,8 +3701,8 @@
       <c r="J9" s="17"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17">
-        <f ca="1" t="shared" ref="L8:L12" si="2">RANDBETWEEN(0,1)</f>
-        <v>0</v>
+        <f ca="1" t="shared" ref="L8:L12" si="1">RANDBETWEEN(0,1)</f>
+        <v>1</v>
       </c>
       <c r="M9" s="17"/>
       <c r="N9" t="s">
@@ -3712,19 +3717,20 @@
         <v>195</v>
       </c>
       <c r="C10" s="17">
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>9</v>
       </c>
       <c r="D10" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>3</v>
+        <f ca="1">RANDBETWEEN(1,9998)</f>
+        <v>7954</v>
       </c>
       <c r="E10" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>5</v>
+        <f ca="1">RANDBETWEEN(D10,9999)</f>
+        <v>9049</v>
       </c>
       <c r="F10" s="17">
-        <f ca="1" t="shared" si="1"/>
-        <v>0.42</v>
+        <f ca="1" t="shared" si="0"/>
+        <v>0.97</v>
       </c>
       <c r="G10" s="17"/>
       <c r="H10" s="17"/>
@@ -3732,7 +3738,7 @@
       <c r="J10" s="17"/>
       <c r="K10" s="17"/>
       <c r="L10" s="17">
-        <f ca="1" t="shared" si="2"/>
+        <f ca="1" t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="M10" s="17"/>
@@ -3748,19 +3754,20 @@
         <v>196</v>
       </c>
       <c r="C11" s="17">
-        <v>1</v>
+        <f ca="1">RANDBETWEEN(1,10)</f>
+        <v>3</v>
       </c>
       <c r="D11" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>10</v>
+        <f ca="1">RANDBETWEEN(1,9998)</f>
+        <v>4520</v>
       </c>
       <c r="E11" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>8</v>
+        <f ca="1">RANDBETWEEN(D11,9999)</f>
+        <v>4953</v>
       </c>
       <c r="F11" s="17">
-        <f ca="1" t="shared" si="1"/>
-        <v>0.38</v>
+        <f ca="1" t="shared" si="0"/>
+        <v>0.81</v>
       </c>
       <c r="G11" s="17"/>
       <c r="H11" s="17"/>
@@ -3768,8 +3775,8 @@
       <c r="J11" s="17"/>
       <c r="K11" s="17"/>
       <c r="L11" s="17">
-        <f ca="1" t="shared" si="2"/>
-        <v>1</v>
+        <f ca="1" t="shared" si="1"/>
+        <v>0</v>
       </c>
       <c r="M11" s="17"/>
       <c r="N11" t="s">
@@ -3780,21 +3787,24 @@
       <c r="A12" s="16">
         <v>8</v>
       </c>
-      <c r="B12"/>
+      <c r="B12" t="s">
+        <v>198</v>
+      </c>
       <c r="C12" s="17">
+        <f ca="1">RANDBETWEEN(1,10)</f>
         <v>1</v>
       </c>
       <c r="D12" s="17">
-        <f ca="1">RANDBETWEEN(1,10)</f>
-        <v>7</v>
+        <f ca="1">RANDBETWEEN(1,9998)</f>
+        <v>5659</v>
       </c>
       <c r="E12" s="17">
+        <f ca="1">RANDBETWEEN(D12,9999)</f>
+        <v>5827</v>
+      </c>
+      <c r="F12" s="17">
         <f ca="1" t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="F12" s="17">
-        <f ca="1" t="shared" si="1"/>
-        <v>0.89</v>
+        <v>0.84</v>
       </c>
       <c r="G12" s="17"/>
       <c r="H12" s="17"/>
@@ -3802,12 +3812,12 @@
       <c r="J12" s="17"/>
       <c r="K12" s="17"/>
       <c r="L12" s="17">
-        <f ca="1" t="shared" si="2"/>
-        <v>0</v>
+        <f ca="1" t="shared" si="1"/>
+        <v>1</v>
       </c>
       <c r="M12" s="17"/>
       <c r="N12" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add assert to new interface
</commit_message>
<xml_diff>
--- a/case/src/http/inland.xlsx
+++ b/case/src/http/inland.xlsx
@@ -100,29 +100,7 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
       <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -144,13 +122,6 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
       <color rgb="FF9C0006"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -158,8 +129,15 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
+      <color theme="0"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <b val="1"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -174,15 +152,7 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -213,7 +183,30 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
       <color rgb="FF3F3F76"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -228,17 +221,24 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FF800080"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
       <sz val="11"/>
-      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -263,6 +263,96 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -275,97 +365,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -377,49 +383,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,13 +407,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -472,21 +472,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -498,24 +483,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,20 +509,24 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -569,6 +545,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -577,10 +577,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -589,137 +589,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="19" borderId="6" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="28" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="29" borderId="7" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="6" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="8" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="9" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="8" borderId="9" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="8" borderId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -763,6 +763,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -1345,7 +1354,7 @@
 </t>
         </is>
       </c>
-      <c r="E8" s="24" t="inlineStr">
+      <c r="E8" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -1435,7 +1444,7 @@
 </t>
         </is>
       </c>
-      <c r="E11" s="24" t="inlineStr">
+      <c r="E11" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -1478,7 +1487,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "szfpay","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E12" s="24" t="inlineStr">
+      <c r="E12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: ""
@@ -1521,7 +1530,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "tenpay","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E13" s="24" t="inlineStr">
+      <c r="E13" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: ""
@@ -1564,7 +1573,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "xiaoyao","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E14" s="24" t="inlineStr">
+      <c r="E14" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "5003"
@@ -1607,7 +1616,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "-0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E15" s="24" t="inlineStr">
+      <c r="E15" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -1650,7 +1659,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E16" s="25" t="inlineStr">
+      <c r="E16" s="28" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "13"
@@ -1693,7 +1702,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "/xiaoyaoisasunshileman1997","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E17" s="24" t="inlineStr">
+      <c r="E17" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -1736,7 +1745,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E18" s="24" t="inlineStr">
+      <c r="E18" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "5003"
@@ -1807,7 +1816,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D20" s="23" t="inlineStr">
+      <c r="D20" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common","screenInfo":"FULL"}</t>
         </is>
@@ -1840,7 +1849,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D21" s="23" t="inlineStr">
+      <c r="D21" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common","screenInfo":"HALF"}</t>
         </is>
@@ -1873,7 +1882,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D22" s="23" t="inlineStr">
+      <c r="D22" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "d446ee8ac87b478eb3cec6e2d609c705","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "1","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
@@ -1944,7 +1953,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "-1","oriAmount": "-1","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "0","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E24" s="24" t="inlineStr">
+      <c r="E24" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "5003"
@@ -2217,7 +2226,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.query.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E32" s="24" t="inlineStr">
+      <c r="E32" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "W001"
@@ -2260,7 +2269,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.sign.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E33" s="24" t="inlineStr">
+      <c r="E33" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2303,7 +2312,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.unsign.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E34" s="24" t="inlineStr">
+      <c r="E34" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "5003"
@@ -2346,7 +2355,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E35" s="24" t="inlineStr">
+      <c r="E35" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2389,7 +2398,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.sign.first.and.pay.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E36" s="24" t="inlineStr">
+      <c r="E36" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2432,7 +2441,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.query.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E37" s="24" t="inlineStr">
+      <c r="E37" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "A001"
@@ -2475,7 +2484,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.judge.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E38" s="24" t="inlineStr">
+      <c r="E38" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: ""
@@ -2518,7 +2527,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.sign.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E39" s="24" t="inlineStr">
+      <c r="E39" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2561,7 +2570,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.unsign.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E40" s="24" t="inlineStr">
+      <c r="E40" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "1100"
@@ -2604,7 +2613,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E41" s="24" t="inlineStr">
+      <c r="E41" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2647,7 +2656,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.sign.first.and.pay.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E42" s="24" t="inlineStr">
+      <c r="E42" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2690,7 +2699,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "alipay","amount": "45.1","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "1","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"expendRequest": {"header": {"version": "5.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"price": 10000,"count": 1,"productname": "支付Demo测试商品","productdesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnerid": "2031","callBackUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","partnerOrder": "","channelId": "demo","ver": "3.1.5","source": "支付demo","attach": "","sign": "","appKey": "1234","voucherId": 52029740,"voucherType": 2,"voucherCount": 999,"order": "","factor": "sjh"}}</t>
         </is>
       </c>
-      <c r="E43" s="24" t="inlineStr">
+      <c r="E43" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2778,7 +2787,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGN","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "0.0","oriAmount": "0.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "0","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E45" s="24" t="inlineStr">
+      <c r="E45" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -2910,7 +2919,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "100.0","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "0","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E48" s="24" t="inlineStr">
+      <c r="E48" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3020,7 +3029,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "100.0","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "1","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E51" s="24" t="inlineStr">
+      <c r="E51" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "1200"
@@ -3259,7 +3268,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.query.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E7" s="24" t="inlineStr">
+      <c r="E7" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "W001"
@@ -3302,7 +3311,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.sign.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E8" s="24" t="inlineStr">
+      <c r="E8" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3345,7 +3354,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.unsign.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E9" s="24" t="inlineStr">
+      <c r="E9" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "5003"
@@ -3388,7 +3397,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E10" s="24" t="inlineStr">
+      <c r="E10" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3431,7 +3440,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "0.06","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "wxpay.avoid.sign.first.and.pay.server","isNeedExpend": "0","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E11" s="24" t="inlineStr">
+      <c r="E11" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3474,7 +3483,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.query.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E12" s="24" t="inlineStr">
+      <c r="E12" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "A001"
@@ -3517,7 +3526,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.judge.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E13" s="24" t="inlineStr">
+      <c r="E13" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: ""
@@ -3560,7 +3569,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.sign.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E14" s="24" t="inlineStr">
+      <c r="E14" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3603,7 +3612,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.unsign.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E15" s="24" t="inlineStr">
+      <c r="E15" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "1100"
@@ -3646,7 +3655,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E16" s="24" t="inlineStr">
+      <c r="E16" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3689,7 +3698,7 @@
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.coloros.cloud","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.06","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "00040001","notifyurl": "http://pay.album.ocloud-test.wanyol.com/pay/v2/payNotify.json","productName": "OPPO 云服务","productDesc": "OPPO 云服务","partnercode": "231810428","appversion": "210","currencyName": "人民币","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.199","ext1": "alipay.avoid.sign.first.and.pay.server","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
       </c>
-      <c r="E17" s="24" t="inlineStr">
+      <c r="E17" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3732,7 +3741,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "alipay","amount": "45.1","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "1","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"expendRequest": {"header": {"version": "5.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"price": 10000,"count": 1,"productname": "支付Demo测试商品","productdesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnerid": "2031","callBackUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","partnerOrder": "","channelId": "demo","ver": "3.1.5","source": "支付demo","attach": "","sign": "","appKey": "1234","voucherId": 52029740,"voucherType": 2,"voucherCount": 999,"order": "","factor": "sjh"}}</t>
         </is>
       </c>
-      <c r="E18" s="24" t="inlineStr">
+      <c r="E18" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3820,7 +3829,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGN","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "0.0","oriAmount": "0.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "0","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E20" s="24" t="inlineStr">
+      <c r="E20" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -3952,7 +3961,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "100.0","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "0","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E23" s="24" t="inlineStr">
+      <c r="E23" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "0000"
@@ -4062,7 +4071,7 @@
           <t>{"header": {"version": "1.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"transType": "SIGNANDPAY","renewProductCode": "20310001","signPartnerOrder": "","type": "wxpay","amount": "100.0","oriAmount": "100.0","ip": "113.102.136.208","sign": "","signAgreementNotifyUrl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","appId": "","isNeedExpend": "1","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "209","currencyName": "CNY","rate": 1.0,"partnerorder": ""}}</t>
         </is>
       </c>
-      <c r="E26" s="24" t="inlineStr">
+      <c r="E26" s="27" t="inlineStr">
         <is>
           <t xml:space="preserve">baseresult': {
   code: "1200"
@@ -4297,7 +4306,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D7" s="23" t="inlineStr">
+      <c r="D7" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
@@ -4338,7 +4347,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D8" s="23" t="inlineStr">
+      <c r="D8" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.136.248","isNeedExpend":"0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
@@ -4379,7 +4388,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D9" s="23" t="inlineStr">
+      <c r="D9" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "qqwallet","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
@@ -4420,7 +4429,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D10" s="23" t="inlineStr">
+      <c r="D10" s="26" t="inlineStr">
         <is>
           <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "qqwallet","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
         </is>
@@ -4747,7 +4756,7 @@
           <t>Test suite名称</t>
         </is>
       </c>
-      <c r="B1" s="17" t="inlineStr">
+      <c r="B1" s="20" t="inlineStr">
         <is>
           <t>批量发放优惠券测试用例集</t>
         </is>
@@ -4759,7 +4768,7 @@
           <t>URL</t>
         </is>
       </c>
-      <c r="B2" s="17" t="inlineStr">
+      <c r="B2" s="20" t="inlineStr">
         <is>
           <t>/voucher/grantMultiVoucher</t>
         </is>
@@ -4771,7 +4780,7 @@
           <t>HTTP请求方式</t>
         </is>
       </c>
-      <c r="B3" s="17" t="inlineStr">
+      <c r="B3" s="20" t="inlineStr">
         <is>
           <t>POST</t>
         </is>
@@ -4783,7 +4792,7 @@
           <t>前置条件</t>
         </is>
       </c>
-      <c r="B4" s="18" t="n"/>
+      <c r="B4" s="21" t="n"/>
     </row>
     <row r="5" ht="21" customHeight="1" s="1">
       <c r="A5" s="2" t="inlineStr">
@@ -4791,7 +4800,7 @@
           <t>环境恢复</t>
         </is>
       </c>
-      <c r="B5" s="18" t="n"/>
+      <c r="B5" s="21" t="n"/>
     </row>
     <row r="6" ht="20" customHeight="1" s="1">
       <c r="A6" s="6" t="inlineStr">
@@ -4866,67 +4875,67 @@
       </c>
     </row>
     <row r="7" ht="15.6" customHeight="1" s="1">
-      <c r="A7" s="19" t="inlineStr">
+      <c r="A7" s="22" t="inlineStr">
         <is>
           <t>vouType</t>
         </is>
       </c>
-      <c r="B7" s="19" t="inlineStr">
+      <c r="B7" s="22" t="inlineStr">
         <is>
           <t>vouName</t>
         </is>
       </c>
-      <c r="C7" s="19" t="inlineStr">
+      <c r="C7" s="22" t="inlineStr">
         <is>
           <t>grantCount</t>
         </is>
       </c>
-      <c r="D7" s="19" t="inlineStr">
+      <c r="D7" s="22" t="inlineStr">
         <is>
           <t>amount</t>
         </is>
       </c>
-      <c r="E7" s="19" t="inlineStr">
+      <c r="E7" s="22" t="inlineStr">
         <is>
           <t>maxAmount</t>
         </is>
       </c>
-      <c r="F7" s="19" t="inlineStr">
+      <c r="F7" s="22" t="inlineStr">
         <is>
           <t>ratio</t>
         </is>
       </c>
-      <c r="G7" s="19" t="inlineStr">
+      <c r="G7" s="22" t="inlineStr">
         <is>
           <t>beginTime</t>
         </is>
       </c>
-      <c r="H7" s="19" t="inlineStr">
+      <c r="H7" s="22" t="inlineStr">
         <is>
           <t>expireTime</t>
         </is>
       </c>
-      <c r="I7" s="19" t="inlineStr">
+      <c r="I7" s="22" t="inlineStr">
         <is>
           <t>scopeId</t>
         </is>
       </c>
-      <c r="J7" s="19" t="inlineStr">
+      <c r="J7" s="22" t="inlineStr">
         <is>
           <t>subScopeId</t>
         </is>
       </c>
-      <c r="K7" s="19" t="inlineStr">
+      <c r="K7" s="22" t="inlineStr">
         <is>
           <t>blackScopeId</t>
         </is>
       </c>
-      <c r="L7" s="19" t="inlineStr">
+      <c r="L7" s="22" t="inlineStr">
         <is>
           <t>settleType</t>
         </is>
       </c>
-      <c r="M7" s="19" t="inlineStr">
+      <c r="M7" s="22" t="inlineStr">
         <is>
           <t>configId</t>
         </is>
@@ -4938,7 +4947,7 @@
       </c>
     </row>
     <row r="8" ht="15.6" customHeight="1" s="1">
-      <c r="A8" s="20" t="n">
+      <c r="A8" s="23" t="n">
         <v>1</v>
       </c>
       <c r="B8" s="0" t="inlineStr">
@@ -4946,31 +4955,31 @@
           <t>消费券</t>
         </is>
       </c>
-      <c r="C8" s="21" t="n">
+      <c r="C8" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="24">
         <f>RANDBETWEEN(1,10)</f>
         <v/>
       </c>
-      <c r="E8" s="21">
+      <c r="E8" s="24">
         <f>RANDBETWEEN(D8,9999)</f>
         <v/>
       </c>
-      <c r="F8" s="21">
+      <c r="F8" s="24">
         <f>ROUND(RAND(),2)</f>
         <v/>
       </c>
-      <c r="G8" s="26" t="n"/>
-      <c r="H8" s="21" t="n"/>
-      <c r="I8" s="21" t="n"/>
-      <c r="J8" s="21" t="n"/>
-      <c r="K8" s="21" t="n"/>
-      <c r="L8" s="21">
+      <c r="G8" s="29" t="n"/>
+      <c r="H8" s="24" t="n"/>
+      <c r="I8" s="24" t="n"/>
+      <c r="J8" s="24" t="n"/>
+      <c r="K8" s="24" t="n"/>
+      <c r="L8" s="24">
         <f>RANDBETWEEN(0,1)</f>
         <v/>
       </c>
-      <c r="M8" s="21" t="n"/>
+      <c r="M8" s="24" t="n"/>
       <c r="N8" s="0" t="inlineStr">
         <is>
           <t>消费券</t>
@@ -4978,7 +4987,7 @@
       </c>
     </row>
     <row r="9" ht="15.6" customHeight="1" s="1">
-      <c r="A9" s="20" t="n">
+      <c r="A9" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B9" s="0" t="inlineStr">
@@ -4986,31 +4995,31 @@
           <t>抵扣券(满maxAmount，减amount)</t>
         </is>
       </c>
-      <c r="C9" s="21" t="n">
+      <c r="C9" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="24">
         <f>RANDBETWEEN(1,10)</f>
         <v/>
       </c>
-      <c r="E9" s="21">
+      <c r="E9" s="24">
         <f>RANDBETWEEN(D9,20)</f>
         <v/>
       </c>
-      <c r="F9" s="21">
+      <c r="F9" s="24">
         <f>ROUND(RAND(),2)</f>
         <v/>
       </c>
-      <c r="G9" s="21" t="n"/>
-      <c r="H9" s="21" t="n"/>
-      <c r="I9" s="21" t="n"/>
-      <c r="J9" s="21" t="n"/>
-      <c r="K9" s="21" t="n"/>
-      <c r="L9" s="21">
+      <c r="G9" s="24" t="n"/>
+      <c r="H9" s="24" t="n"/>
+      <c r="I9" s="24" t="n"/>
+      <c r="J9" s="24" t="n"/>
+      <c r="K9" s="24" t="n"/>
+      <c r="L9" s="24">
         <f>RANDBETWEEN(0,1)</f>
         <v/>
       </c>
-      <c r="M9" s="21" t="n"/>
+      <c r="M9" s="24" t="n"/>
       <c r="N9" s="0" t="inlineStr">
         <is>
           <t>抵扣券(满maxAmount，减amount)</t>
@@ -5018,7 +5027,7 @@
       </c>
     </row>
     <row r="10" ht="15.6" customHeight="1" s="1">
-      <c r="A10" s="20" t="n">
+      <c r="A10" s="23" t="n">
         <v>5</v>
       </c>
       <c r="B10" s="0" t="inlineStr">
@@ -5026,31 +5035,31 @@
           <t>折扣券（最低消费amount，单笔最高减maxAmount）</t>
         </is>
       </c>
-      <c r="C10" s="21" t="n">
+      <c r="C10" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="24">
         <f>RANDBETWEEN(1,10)</f>
         <v/>
       </c>
-      <c r="E10" s="21">
+      <c r="E10" s="24">
         <f>RANDBETWEEN(D10,9999)</f>
         <v/>
       </c>
-      <c r="F10" s="21">
+      <c r="F10" s="24">
         <f>ROUND(RAND(),2)</f>
         <v/>
       </c>
-      <c r="G10" s="21" t="n"/>
-      <c r="H10" s="21" t="n"/>
-      <c r="I10" s="21" t="n"/>
-      <c r="J10" s="21" t="n"/>
-      <c r="K10" s="21" t="n"/>
-      <c r="L10" s="21">
+      <c r="G10" s="24" t="n"/>
+      <c r="H10" s="24" t="n"/>
+      <c r="I10" s="24" t="n"/>
+      <c r="J10" s="24" t="n"/>
+      <c r="K10" s="24" t="n"/>
+      <c r="L10" s="24">
         <f>RANDBETWEEN(0,1)</f>
         <v/>
       </c>
-      <c r="M10" s="21" t="n"/>
+      <c r="M10" s="24" t="n"/>
       <c r="N10" s="0" t="inlineStr">
         <is>
           <t>折扣券（最低消费amount，单笔最高减maxAmount）</t>
@@ -5058,7 +5067,7 @@
       </c>
     </row>
     <row r="11" ht="15.6" customHeight="1" s="1">
-      <c r="A11" s="20" t="n">
+      <c r="A11" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B11" s="0" t="inlineStr">
@@ -5066,31 +5075,31 @@
           <t>消费折扣券</t>
         </is>
       </c>
-      <c r="C11" s="21" t="n">
+      <c r="C11" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D11" s="21">
+      <c r="D11" s="24">
         <f>RANDBETWEEN(1,10)</f>
         <v/>
       </c>
-      <c r="E11" s="21">
+      <c r="E11" s="24">
         <f>RANDBETWEEN(D11,9999)</f>
         <v/>
       </c>
-      <c r="F11" s="21">
+      <c r="F11" s="24">
         <f>ROUND(RAND(),2)</f>
         <v/>
       </c>
-      <c r="G11" s="21" t="n"/>
-      <c r="H11" s="21" t="n"/>
-      <c r="I11" s="21" t="n"/>
-      <c r="J11" s="21" t="n"/>
-      <c r="K11" s="21" t="n"/>
-      <c r="L11" s="21">
+      <c r="G11" s="24" t="n"/>
+      <c r="H11" s="24" t="n"/>
+      <c r="I11" s="24" t="n"/>
+      <c r="J11" s="24" t="n"/>
+      <c r="K11" s="24" t="n"/>
+      <c r="L11" s="24">
         <f>RANDBETWEEN(0,1)</f>
         <v/>
       </c>
-      <c r="M11" s="21" t="n"/>
+      <c r="M11" s="24" t="n"/>
       <c r="N11" s="0" t="inlineStr">
         <is>
           <t>消费折扣券，ratio&lt;1</t>
@@ -5098,7 +5107,7 @@
       </c>
     </row>
     <row r="12" ht="15.6" customHeight="1" s="1">
-      <c r="A12" s="20" t="n">
+      <c r="A12" s="23" t="n">
         <v>8</v>
       </c>
       <c r="B12" s="0" t="inlineStr">
@@ -5106,31 +5115,31 @@
           <t>\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\\用户红包券\</t>
         </is>
       </c>
-      <c r="C12" s="21" t="n">
+      <c r="C12" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="D12" s="21">
+      <c r="D12" s="24">
         <f>RANDBETWEEN(1,10)</f>
         <v/>
       </c>
-      <c r="E12" s="21">
+      <c r="E12" s="24">
         <f>RANDBETWEEN(D12,9999)</f>
         <v/>
       </c>
-      <c r="F12" s="21">
+      <c r="F12" s="24">
         <f>ROUND(RAND(),2)</f>
         <v/>
       </c>
-      <c r="G12" s="21" t="n"/>
-      <c r="H12" s="21" t="n"/>
-      <c r="I12" s="21" t="n"/>
-      <c r="J12" s="21" t="n"/>
-      <c r="K12" s="21" t="n"/>
-      <c r="L12" s="21">
+      <c r="G12" s="24" t="n"/>
+      <c r="H12" s="24" t="n"/>
+      <c r="I12" s="24" t="n"/>
+      <c r="J12" s="24" t="n"/>
+      <c r="K12" s="24" t="n"/>
+      <c r="L12" s="24">
         <f>RANDBETWEEN(0,1)</f>
         <v/>
       </c>
-      <c r="M12" s="21" t="n"/>
+      <c r="M12" s="24" t="n"/>
       <c r="N12" s="0" t="inlineStr">
         <is>
           <t>会员红包券</t>
@@ -5151,7 +5160,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
@@ -5173,7 +5182,7 @@
           <t>Test suite名称</t>
         </is>
       </c>
-      <c r="B1" s="16" t="inlineStr">
+      <c r="B1" s="19" t="inlineStr">
         <is>
           <t>营销信息-获取跳转链接信息</t>
         </is>
@@ -5282,7 +5291,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="D7" s="17" t="inlineStr">
         <is>
           <t>{"partnerId": "5456925"}</t>
         </is>
@@ -5323,7 +5332,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="17" t="inlineStr">
         <is>
           <t>{"partnerId": "888888"}</t>
         </is>
@@ -5346,6 +5355,7 @@
           <t>passed</t>
         </is>
       </c>
+      <c r="I8" s="11" t="n"/>
     </row>
     <row r="9" ht="27" customHeight="1" s="1">
       <c r="A9" s="7" t="inlineStr">
@@ -5363,7 +5373,7 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D9" s="15" t="inlineStr">
+      <c r="D9" s="17" t="inlineStr">
         <is>
           <t>{"partnerId": ""}</t>
         </is>
@@ -5386,6 +5396,7 @@
           <t>passed</t>
         </is>
       </c>
+      <c r="I9" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
@@ -5401,13 +5412,13 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
     <col width="25.875" customWidth="1" style="1" min="1" max="1"/>
-    <col width="33" customWidth="1" style="1" min="2" max="2"/>
+    <col width="18.25" customWidth="1" style="1" min="2" max="2"/>
     <col width="13.4416666666667" customWidth="1" style="1" min="3" max="3"/>
     <col width="54.1083333333333" customWidth="1" style="1" min="4" max="4"/>
     <col width="45.6666666666667" customWidth="1" style="1" min="5" max="5"/>
@@ -5516,13 +5527,13 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="27" customHeight="1" s="1">
+    <row r="7" ht="50" customHeight="1" s="1">
       <c r="A7" s="7" t="inlineStr">
         <is>
           <t>正常拉取会员加购位</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -5532,12 +5543,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D7" s="15" t="inlineStr">
+      <c r="D7" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "","partnerId": "5456925","orderAmount": "100", "factor": ""}</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="E7" s="16" t="inlineStr">
         <is>
           <t>{"data": {"buyPlaceList": []}, "success": true}</t>
         </is>
@@ -5545,21 +5556,25 @@
       <c r="F7" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="G7" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"True"}</t>
+        </is>
+      </c>
+      <c r="H7" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I7" s="11" t="n"/>
     </row>
-    <row r="8" ht="27" customHeight="1" s="1">
+    <row r="8" ht="50" customHeight="1" s="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>金额传入负数</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -5569,12 +5584,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D8" s="15" t="inlineStr">
+      <c r="D8" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "","partnerId": "5456925","orderAmount": "-100", "factor": ""}</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="E8" s="16" t="inlineStr">
         <is>
           <t>{"data": {"buyPlaceList": []}, "success": true}</t>
         </is>
@@ -5582,21 +5597,25 @@
       <c r="F8" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="7" t="inlineStr">
+      <c r="G8" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"True"}</t>
+        </is>
+      </c>
+      <c r="H8" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I8" s="7" t="n"/>
     </row>
-    <row r="9" ht="27" customHeight="1" s="1">
+    <row r="9" ht="50" customHeight="1" s="1">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>金额传入-</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -5606,12 +5625,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D9" s="15" t="inlineStr">
+      <c r="D9" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "","partnerId": "5456925","orderAmount": "0", "factor": ""}</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
+      <c r="E9" s="16" t="inlineStr">
         <is>
           <t>{"data": {"buyPlaceList": []}, "success": true}</t>
         </is>
@@ -5619,21 +5638,25 @@
       <c r="F9" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="7" t="inlineStr">
+      <c r="G9" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"True"}</t>
+        </is>
+      </c>
+      <c r="H9" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I9" s="7" t="n"/>
     </row>
-    <row r="10" ht="27" customHeight="1" s="1">
+    <row r="10" ht="50" customHeight="1" s="1">
       <c r="A10" s="7" t="inlineStr">
         <is>
           <t>passToken不正确</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -5643,12 +5666,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D10" s="15" t="inlineStr">
+      <c r="D10" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "error_token","partnerId": "5456925","orderAmount": "100", "factor": ""}</t>
         </is>
       </c>
-      <c r="E10" s="7" t="inlineStr">
+      <c r="E10" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "20004", "message": "娴佺▼鍑瘉澶辨晥"}, "success": false}</t>
         </is>
@@ -5656,21 +5679,25 @@
       <c r="F10" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="7" t="inlineStr">
+      <c r="G10" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"False"}</t>
+        </is>
+      </c>
+      <c r="H10" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I10" s="7" t="n"/>
     </row>
-    <row r="11" ht="27" customHeight="1" s="1">
+    <row r="11" ht="50" customHeight="1" s="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>业务线不传</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -5680,12 +5707,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D11" s="15" t="inlineStr">
+      <c r="D11" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "","partnerId": "","orderAmount": "100", "factor": ""}</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
+      <c r="E11" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "101", "message": "partnerId must not be empty"}, "success": false}</t>
         </is>
@@ -5693,21 +5720,25 @@
       <c r="F11" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="7" t="inlineStr">
+      <c r="G11" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"False"}</t>
+        </is>
+      </c>
+      <c r="H11" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I11" s="7" t="n"/>
     </row>
-    <row r="12" ht="27" customHeight="1" s="1">
+    <row r="12" ht="50" customHeight="1" s="1">
       <c r="A12" s="7" t="inlineStr">
         <is>
           <t>传入不支持的业务线</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -5717,12 +5748,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D12" s="15" t="inlineStr">
+      <c r="D12" s="16" t="inlineStr">
         <is>
           <t>{"processToken": "","partnerId": "99999","orderAmount": "", "factor": ""}</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr">
+      <c r="E12" s="16" t="inlineStr">
         <is>
           <t>{"data": {"buyPlaceList": []}, "success": true}</t>
         </is>
@@ -5730,8 +5761,12 @@
       <c r="F12" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="7" t="inlineStr">
+      <c r="G12" s="7" t="inlineStr">
+        <is>
+          <t>{"success":"True"}</t>
+        </is>
+      </c>
+      <c r="H12" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
@@ -5752,18 +5787,18 @@
   <dimension ref="A1:I14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
   <cols>
     <col width="20.5" customWidth="1" style="1" min="1" max="1"/>
-    <col width="33" customWidth="1" style="1" min="2" max="2"/>
+    <col width="19" customWidth="1" style="1" min="2" max="2"/>
     <col width="13.4416666666667" customWidth="1" style="1" min="3" max="3"/>
-    <col width="54.1083333333333" customWidth="1" style="1" min="4" max="4"/>
+    <col width="50" customWidth="1" style="1" min="4" max="4"/>
     <col width="45.6666666666667" customWidth="1" style="1" min="5" max="5"/>
     <col width="13.775" customWidth="1" style="1" min="6" max="6"/>
-    <col width="24.775" customWidth="1" style="1" min="7" max="7"/>
+    <col width="33.625" customWidth="1" style="1" min="7" max="7"/>
     <col width="15.6666666666667" customWidth="1" style="1" min="8" max="8"/>
     <col width="21.1083333333333" customWidth="1" style="1" min="9" max="9"/>
   </cols>
@@ -5867,13 +5902,13 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="40.5" customHeight="1" s="1">
+    <row r="7" ht="50" customHeight="1" s="1">
       <c r="A7" s="7" t="inlineStr">
         <is>
           <t>支付apk获取凭证</t>
         </is>
       </c>
-      <c r="B7" s="4" t="inlineStr">
+      <c r="B7" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -5888,29 +5923,33 @@
           <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1621241493314, "processToken": "Qe4aS3p5Z9KZVyGap8Roax"}, "success": true}</t>
+      <c r="E7" s="16" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1621243514755, "processToken": "2nzYJhTZ6aQ3pC2b5xMUJm"}, "success": true}</t>
         </is>
       </c>
       <c r="F7" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="G7" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H7" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I7" s="11" t="n"/>
     </row>
-    <row r="8" ht="40.5" customHeight="1" s="1">
+    <row r="8" ht="50" customHeight="1" s="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>msp获取凭证</t>
         </is>
       </c>
-      <c r="B8" s="4" t="inlineStr">
+      <c r="B8" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -5925,29 +5964,33 @@
           <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1621241493430, "processToken": "4pE5JFvy9vdtznPhjo39MW"}, "success": true}</t>
+      <c r="E8" s="16" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1621243514887, "processToken": "CeLec6zAuJwa6TtuhYwUw1"}, "success": true}</t>
         </is>
       </c>
       <c r="F8" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="11" t="inlineStr">
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H8" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I8" s="11" t="n"/>
     </row>
-    <row r="9" ht="40.5" customHeight="1" s="1">
+    <row r="9" ht="50" customHeight="1" s="1">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>apk无账号获取凭证</t>
         </is>
       </c>
-      <c r="B9" s="4" t="inlineStr">
+      <c r="B9" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -5962,29 +6005,33 @@
           <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1621241493759, "processToken": "Tqi6sz97eRojqRp9H2c1ws"}, "success": true}</t>
+      <c r="E9" s="16" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1621243515005, "processToken": "B3vBN2z8LXyM22fiwCqbEf"}, "success": true}</t>
         </is>
       </c>
       <c r="F9" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="G9" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H9" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I9" s="11" t="n"/>
     </row>
-    <row r="10" ht="40.5" customHeight="1" s="1">
+    <row r="10" ht="50" customHeight="1" s="1">
       <c r="A10" s="7" t="inlineStr">
         <is>
           <t>msp无账号获取凭证</t>
         </is>
       </c>
-      <c r="B10" s="4" t="inlineStr">
+      <c r="B10" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -5999,29 +6046,33 @@
           <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
         </is>
       </c>
-      <c r="E10" s="7" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1621241493878, "processToken": "6Ni2tMy9qDjQCjj6PkNLme"}, "success": true}</t>
+      <c r="E10" s="16" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1621243515122, "processToken": "8vuWJ1kgwcnM1cuq75bfM9"}, "success": true}</t>
         </is>
       </c>
       <c r="F10" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="11" t="inlineStr">
+      <c r="G10" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H10" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I10" s="11" t="n"/>
     </row>
-    <row r="11" ht="40.5" customHeight="1" s="1">
+    <row r="11" ht="50" customHeight="1" s="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>msp获取凭证不传appId</t>
         </is>
       </c>
-      <c r="B11" s="4" t="inlineStr">
+      <c r="B11" s="14" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
@@ -6036,29 +6087,33 @@
           <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1621241493994, "processToken": "74atS5NUk8F9PSHm15vVRF"}, "success": true}</t>
+      <c r="E11" s="16" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1621243515238, "processToken": "HabxCfQrgYtuYFeEKTAAJz"}, "success": true}</t>
         </is>
       </c>
       <c r="F11" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="G11" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H11" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I11" s="11" t="n"/>
     </row>
-    <row r="12" ht="40.5" customHeight="1" s="1">
+    <row r="12" ht="50" customHeight="1" s="1">
       <c r="A12" s="7" t="inlineStr">
         <is>
           <t>token传入不正确</t>
         </is>
       </c>
-      <c r="B12" s="4" t="inlineStr">
+      <c r="B12" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -6073,7 +6128,7 @@
           <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr">
+      <c r="E12" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "20000", "message": "閴存潈澶辫触"}, "success": false}</t>
         </is>
@@ -6081,21 +6136,25 @@
       <c r="F12" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="G12" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "False"}</t>
+        </is>
+      </c>
+      <c r="H12" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I12" s="11" t="n"/>
     </row>
-    <row r="13" ht="40.5" customHeight="1" s="1">
+    <row r="13" ht="50" customHeight="1" s="1">
       <c r="A13" s="7" t="inlineStr">
         <is>
           <t>partnerCode不传</t>
         </is>
       </c>
-      <c r="B13" s="4" t="inlineStr">
+      <c r="B13" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -6110,7 +6169,7 @@
           <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
+      <c r="E13" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "101", "message": "must not be blank"}, "success": false}</t>
         </is>
@@ -6118,21 +6177,25 @@
       <c r="F13" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="G13" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "False"}</t>
+        </is>
+      </c>
+      <c r="H13" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
     </row>
-    <row r="14" ht="27" customHeight="1" s="1">
+    <row r="14" ht="50" customHeight="1" s="1">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>appPackage不传</t>
         </is>
       </c>
-      <c r="B14" s="4" t="inlineStr">
+      <c r="B14" s="14" t="inlineStr">
         <is>
           <t>full</t>
         </is>
@@ -6142,12 +6205,12 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D14" s="15" t="inlineStr">
+      <c r="D14" s="16" t="inlineStr">
         <is>
           <t>{"token": "","appId": "","appPackage": "", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E14" s="7" t="inlineStr">
+      <c r="E14" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "101", "message": "must not be blank"}, "success": false}</t>
         </is>
@@ -6155,8 +6218,12 @@
       <c r="F14" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="11" t="inlineStr">
+      <c r="G14" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "False"}</t>
+        </is>
+      </c>
+      <c r="H14" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
@@ -6177,7 +6244,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="0"/>
@@ -6292,7 +6359,7 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="40" customHeight="1" s="1">
+    <row r="7" ht="50" customHeight="1" s="1">
       <c r="A7" s="7" t="inlineStr">
         <is>
           <t>有账号+自动续费+全屏</t>
@@ -6314,7 +6381,7 @@
 "renewal": "Y", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E7" s="7" t="inlineStr">
+      <c r="E7" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鏀粯瀹濆鎵樹唬鎵�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "寰俊濮旀墭浠ｆ墸", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "11", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "wxpay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6322,15 +6389,19 @@
       <c r="F7" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G7" s="7" t="n"/>
-      <c r="H7" s="11" t="inlineStr">
+      <c r="G7" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H7" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I7" s="11" t="n"/>
     </row>
-    <row r="8" ht="40" customHeight="1" s="1">
+    <row r="8" ht="50" customHeight="1" s="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
           <t>有账号+自动续费+横屏(目前不支持)</t>
@@ -6353,7 +6424,7 @@
 "renewal": "Y", "acrossScreen": "Y"}</t>
         </is>
       </c>
-      <c r="E8" s="7" t="inlineStr">
+      <c r="E8" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": []}, "success": true}</t>
         </is>
@@ -6361,15 +6432,19 @@
       <c r="F8" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G8" s="7" t="n"/>
-      <c r="H8" s="11" t="inlineStr">
+      <c r="G8" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H8" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I8" s="11" t="n"/>
     </row>
-    <row r="9" ht="40" customHeight="1" s="1">
+    <row r="9" ht="50" customHeight="1" s="1">
       <c r="A9" s="7" t="inlineStr">
         <is>
           <t>有账号+普通支付+全屏</t>
@@ -6392,7 +6467,7 @@
 "renewal": "N", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E9" s="7" t="inlineStr">
+      <c r="E9" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "10", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "绉嬭礉濂藉垎鏈焅t", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/finzpay_icon.png", "index": "0", "lastPayType": "N", "payType": "finzpay", "prompt": "finzpay", "smallIcon": "", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "9", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "0", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "8", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "7", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "3", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6400,15 +6475,19 @@
       <c r="F9" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G9" s="7" t="n"/>
-      <c r="H9" s="11" t="inlineStr">
+      <c r="G9" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H9" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I9" s="11" t="n"/>
     </row>
-    <row r="10" ht="40" customHeight="1" s="1">
+    <row r="10" ht="50" customHeight="1" s="1">
       <c r="A10" s="7" t="inlineStr">
         <is>
           <t>有账号+普通支付+横屏</t>
@@ -6431,7 +6510,7 @@
 "renewal": "N", "acrossScreen": "Y"}</t>
         </is>
       </c>
-      <c r="E10" s="7" t="inlineStr">
+      <c r="E10" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6439,15 +6518,19 @@
       <c r="F10" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G10" s="7" t="n"/>
-      <c r="H10" s="11" t="inlineStr">
+      <c r="G10" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H10" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I10" s="11" t="n"/>
     </row>
-    <row r="11" ht="40" customHeight="1" s="1">
+    <row r="11" ht="50" customHeight="1" s="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
           <t>无账号+普通支付+全屏</t>
@@ -6470,7 +6553,7 @@
 "renewal": "N", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E11" s="7" t="inlineStr">
+      <c r="E11" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "10", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "绉嬭礉濂藉垎鏈焅t", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/finzpay_icon.png", "index": "0", "lastPayType": "N", "payType": "finzpay", "prompt": "finzpay", "smallIcon": "", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "9", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "0", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "8", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "7", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "3", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6478,15 +6561,19 @@
       <c r="F11" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G11" s="7" t="n"/>
-      <c r="H11" s="11" t="inlineStr">
+      <c r="G11" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H11" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I11" s="11" t="n"/>
     </row>
-    <row r="12" ht="40" customHeight="1" s="1">
+    <row r="12" ht="50" customHeight="1" s="1">
       <c r="A12" s="7" t="inlineStr">
         <is>
           <t>无账号+普通支付+横屏(目前不支持)</t>
@@ -6509,7 +6596,7 @@
 "renewal": "N", "acrossScreen": "Y"}</t>
         </is>
       </c>
-      <c r="E12" s="7" t="inlineStr">
+      <c r="E12" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6517,15 +6604,19 @@
       <c r="F12" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G12" s="7" t="n"/>
-      <c r="H12" s="11" t="inlineStr">
+      <c r="G12" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H12" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I12" s="11" t="n"/>
     </row>
-    <row r="13" ht="40" customHeight="1" s="1">
+    <row r="13" ht="50" customHeight="1" s="1">
       <c r="A13" s="7" t="inlineStr">
         <is>
           <t>无账号+自动续费+全屏(目前不支持)</t>
@@ -6548,7 +6639,7 @@
 "renewal": "Y", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E13" s="7" t="inlineStr">
+      <c r="E13" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鏀粯瀹濆鎵樹唬鎵�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "寰俊濮旀墭浠ｆ墸", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "11", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "wxpay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
         </is>
@@ -6556,15 +6647,19 @@
       <c r="F13" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G13" s="7" t="n"/>
-      <c r="H13" s="11" t="inlineStr">
+      <c r="G13" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H13" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I13" s="11" t="n"/>
     </row>
-    <row r="14" ht="40" customHeight="1" s="1">
+    <row r="14" ht="50" customHeight="1" s="1">
       <c r="A14" s="7" t="inlineStr">
         <is>
           <t>无账号+自动续费+横屏(目前不支持)</t>
@@ -6587,7 +6682,7 @@
 "renewal": "Y", "acrossScreen": "Y"}</t>
         </is>
       </c>
-      <c r="E14" s="7" t="inlineStr">
+      <c r="E14" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": []}, "success": true}</t>
         </is>
@@ -6595,15 +6690,19 @@
       <c r="F14" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G14" s="7" t="n"/>
-      <c r="H14" s="7" t="inlineStr">
+      <c r="G14" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H14" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I14" s="11" t="n"/>
     </row>
-    <row r="15" ht="40" customHeight="1" s="1">
+    <row r="15" ht="50" customHeight="1" s="1">
       <c r="A15" s="7" t="inlineStr">
         <is>
           <t>proceessToken传入不正确</t>
@@ -6626,7 +6725,7 @@
 "renewal": "Y", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E15" s="7" t="inlineStr">
+      <c r="E15" s="16" t="inlineStr">
         <is>
           <t>{"error": {"code": "20004", "message": "娴佺▼鍑瘉澶辨晥"}, "success": false}</t>
         </is>
@@ -6634,15 +6733,19 @@
       <c r="F15" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G15" s="7" t="n"/>
-      <c r="H15" s="11" t="inlineStr">
+      <c r="G15" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "False"}</t>
+        </is>
+      </c>
+      <c r="H15" s="18" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I15" s="11" t="n"/>
     </row>
-    <row r="16" ht="40" customHeight="1" s="1">
+    <row r="16" ht="50" customHeight="1" s="1">
       <c r="A16" s="7" t="inlineStr">
         <is>
           <t>partnerId不传</t>
@@ -6664,7 +6767,7 @@
 "renewal": "Y", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E16" s="7" t="inlineStr">
+      <c r="E16" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": []}, "success": true}</t>
         </is>
@@ -6672,15 +6775,19 @@
       <c r="F16" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G16" s="7" t="n"/>
-      <c r="H16" s="7" t="inlineStr">
+      <c r="G16" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H16" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
       <c r="I16" s="11" t="n"/>
     </row>
-    <row r="17" ht="40" customHeight="1" s="1">
+    <row r="17" ht="50" customHeight="1" s="1">
       <c r="A17" s="7" t="inlineStr">
         <is>
           <t>partnerId不存在</t>
@@ -6702,7 +6809,7 @@
 "renewal": "Y", "acrossScreen": "N"}</t>
         </is>
       </c>
-      <c r="E17" s="7" t="inlineStr">
+      <c r="E17" s="16" t="inlineStr">
         <is>
           <t>{"data": {"payTypeList": []}, "success": true}</t>
         </is>
@@ -6710,8 +6817,12 @@
       <c r="F17" s="10" t="n">
         <v>200</v>
       </c>
-      <c r="G17" s="7" t="n"/>
-      <c r="H17" s="7" t="inlineStr">
+      <c r="G17" s="17" t="inlineStr">
+        <is>
+          <t>{"success": "True"}</t>
+        </is>
+      </c>
+      <c r="H17" s="10" t="inlineStr">
         <is>
           <t>passed</t>
         </is>

</xml_diff>

<commit_message>
delete encjson fixture in case/interface/inland/http/test_pb2json.py
</commit_message>
<xml_diff>
--- a/case/src/http/inland.xlsx
+++ b/case/src/http/inland.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28080" windowHeight="13065" activeTab="1"/>
+    <workbookView windowWidth="28080" windowHeight="13065" tabRatio="973" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="simplepay_recharge_spend" sheetId="1" r:id="rId1"/>
@@ -12,21 +12,26 @@
     <sheet name="simplepay_recharge" sheetId="3" r:id="rId3"/>
     <sheet name="simplepay_no_login" sheetId="4" r:id="rId4"/>
     <sheet name="grant_multi_vouchers" sheetId="5" r:id="rId5"/>
-    <sheet name="simplepay_autosign" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="get_link_info" sheetId="6" r:id="rId6"/>
+    <sheet name="get_marketing_info" sheetId="7" r:id="rId7"/>
+    <sheet name="process_token" sheetId="8" r:id="rId8"/>
+    <sheet name="list_pay_types" sheetId="9" r:id="rId9"/>
+    <sheet name="get_pay_result_activity" sheetId="11" r:id="rId10"/>
+    <sheet name="simplepay_autosign" sheetId="10" state="hidden" r:id="rId11"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">simplepay_recharge_spend!$A$6:$I$53</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">simplepay_direct!$A$6:$I$10</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">simplepay_recharge!$A$6:$I$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">simplepay_no_login!$A$6:$I$6</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">simplepay_autosign!$A$6:$I$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">simplepay_autosign!$A$6:$I$28</definedName>
   </definedNames>
   <calcPr calcId="144525" concurrentCalc="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282">
   <si>
     <t>Test suite名称</t>
   </si>
@@ -649,7 +654,7 @@
     <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "alipay","amount": "0.01","cardno": "","cardpwd":"","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "112.97.217.16","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
   </si>
   <si>
-    <t>{"baseresult": {"code": "0000", "msg": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22RM202105081607362086780423436812%22%26subject%3D%22%E6%94%AF%E4%BB%98Demo%E6%B5%8B%E8%AF%95%E5%95%86%E5%93%81%22%26body%3D%22%E6%94%AF%E4%BB%98Demo%E6%B5%8B%E8%AF%95%E5%95%86%E5%93%81%22%26total_fee%3D%220.01%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22rQPTrh%252B%252B9Ek6k9ymEvo%252FRsMAjmHzq5GvUxeASYa5D7NNvi6OGys%252Be7bPy26BFDP7Nu49SBIlqw48RvZoe3bTXOepQ2BENbQ8Bs57g8h43s5YtG%252Fr7BHDHVzFLJrBQFSW%252B%252Bt6PfrLp05fyjvxnGeeMSE283FIksXKuEu%252BKoR1YDc%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"RM202105081607362086780423436812\"}"}, "payrequestid": "RM202105081607362086780423436812"}</t>
+    <t>{"baseresult": {"code": "0000", "msg": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22RM202105141531282086776969068242%22%26subject%3D%22%E6%94%AF%E4%BB%98Demo%E6%B5%8B%E8%AF%95%E5%95%86%E5%93%81%22%26body%3D%22%E6%94%AF%E4%BB%98Demo%E6%B5%8B%E8%AF%95%E5%95%86%E5%93%81%22%26total_fee%3D%220.01%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22nESxQM0%252B68z4OmiH6MQQWcFyMKYRLu4xh740y84YtFhZVFn2A5%252FpBj3GKS4WfNu17h8wpY5HZQL5rU%252BhZHA%252BezzqF3J2qFFS7K9uym2ZXqazmAN1uFVi9hlkbBaaGkhRJhnSM4q7FPtSFPFDXxW60pzy0bSFsimLmPq3CjhA%252FK4%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"RM202105141531282086776969068242\"}"}, "payrequestid": "RM202105141531282086776969068242"}</t>
   </si>
   <si>
     <t>passed</t>
@@ -661,7 +666,7 @@
     <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "wxpay","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.136.248","isNeedExpend":"0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
   </si>
   <si>
-    <t>{"baseresult": {"code": "0000", "msg": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"ce0add29b2a94ae7b93d13638787e409\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx081607375399685afa268f43ae53720000\",\"sign\":\"BDA76E2B716CBB2B26B8B7C5B619FCB0\",\"timestamp\":\"1620461257\"}"}, "payrequestid": "RM202105081607372086780423628842"}</t>
+    <t>{"baseresult": {"code": "0000", "msg": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"63f958f023d5452ab147ca71f9fc1956\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx1415312879265359873312883b68b10000\",\"sign\":\"9835400DEAAE9D3AE88C3EB0354417ED\",\"timestamp\":\"1620977488\"}"}, "payrequestid": "RM202105141531282086776969810772"}</t>
   </si>
   <si>
     <t>直扣-qq钱包</t>
@@ -670,13 +675,13 @@
     <t>{"header": {"version": "12.0","t_p": "","imei": "","model": "PBDM00","apntype": "1","package": "com.example.pay_demo","r_v": "","ext": "","sdkVer": 209,"country": "CN","currency": "CNY","brandType": "OPPO","mobileos": "11"},"type": "qqwallet","amount": "100.0","cardno": "","cardpwd": "","ext": "","basepay": {"channelId": "demo","notifyurl": "http://pay.pay-test.wanyol.com/notify/notify/receiver","productName": "支付Demo测试商品","productDesc": "垚姦鱻羴犇猋麤骉毳蠱掱赑","partnercode": "2031","appversion": "3.1.5","currencyName": "CNY","rate": 1.0,"partnerorder": ""},"sign": "","ip": "113.102.137.193","isNeedExpend": "0","appId": "","payTypeRMBType": "1","tradeType": "common"}</t>
   </si>
   <si>
-    <t>{"baseresult": {"code": "0000", "msg": "{\"appId\":\"1104946420\",\"bargainorId\":\"1282256301\",\"nonce\":\"802c2e989cf93c6cb52b808a3e1c9cee\",\"pubAcc\":\"\",\"sig\":\"K5vmwVnY+DE/2Gd5mlVe25PqFZs=\",\"tokenId\":\"6M3c58144a48c43a1abcc93ae86a8936\"}"}, "payrequestid": "RM202105081607372086780423777302"}</t>
+    <t>{"baseresult": {"code": "0000", "msg": "{\"appId\":\"1104946420\",\"bargainorId\":\"1282256301\",\"nonce\":\"b70742479bbac554e07deda9d6194a68\",\"pubAcc\":\"\",\"sig\":\"++adfJ3ye5dpyNKbAHqrU/hPWZc=\",\"tokenId\":\"6M0d34dfb700b5d569977bbacbf17c66\"}"}, "payrequestid": "RM202105141531292086776969762372"}</t>
   </si>
   <si>
     <t>直扣-oppopay</t>
   </si>
   <si>
-    <t>{"baseresult": {"code": "0000", "msg": "{\"appId\":\"1104946420\",\"bargainorId\":\"1282256301\",\"nonce\":\"61e26fc612d46bb584a9c25c66d9476d\",\"pubAcc\":\"\",\"sig\":\"BdDlDdRw4oKq+Wu44omG/BaE+pQ=\",\"tokenId\":\"6M85ad9556285189a83d07e6e3bd2f73\"}"}, "payrequestid": "RM202105081607392086780423207652"}</t>
+    <t>{"baseresult": {"code": "0000", "msg": "{\"appId\":\"1104946420\",\"bargainorId\":\"1282256301\",\"nonce\":\"b70742479bbac554e07deda9d6194a68\",\"pubAcc\":\"\",\"sig\":\"Md1/ptuPZcwHXLXm3wONcb/+n/M=\",\"tokenId\":\"6M5efc6a6619cb9dc9a29f35c522f2aa\"}"}, "payrequestid": "RM202105141531292086776969441052"}</t>
   </si>
   <si>
     <t>批量发放优惠券测试用例集</t>
@@ -785,6 +790,268 @@
   </si>
   <si>
     <t>会员红包券</t>
+  </si>
+  <si>
+    <t>营销信息-获取跳转链接信息</t>
+  </si>
+  <si>
+    <t>/api/marketing/v290/get-link-info</t>
+  </si>
+  <si>
+    <t>配置信息有加购位</t>
+  </si>
+  <si>
+    <t>{"partnerId": "5456925"}</t>
+  </si>
+  <si>
+    <t>{"data": {"vipRights": [{"description": "鏇村鍙竵鍒�", "imgUrl": "https://fast-wallet-test.wanyol.com/file/pay/20201120/0031cf18-8223-40ae-b130-154a939cbe9e.jpg", "name": "蹇幓棰嗗彇鏇村鍙竵鍒�", "redirectUrl": "uc://platform.usercenter.com/innerbrowser?min_version=523&amp;url=https%3A%2F%2Fuc3-h5-test.wanyol.com%2Fvip%2fvip_gamePrivilege.html%3fisGradualToolbar%3dtrue%26isTranslucentBar%3dtrue%26LoadInCurrentPage%3dfalse%26source%3dusercenter_message_link_zz"}]}, "success": true}</t>
+  </si>
+  <si>
+    <t>{"success":"True"}</t>
+  </si>
+  <si>
+    <t>配置信息无加购位</t>
+  </si>
+  <si>
+    <t>{"partnerId": "888888"}</t>
+  </si>
+  <si>
+    <t>{"data": {"vipRights": []}, "success": true}</t>
+  </si>
+  <si>
+    <t>partnerId不传</t>
+  </si>
+  <si>
+    <t>{"partnerId": ""}</t>
+  </si>
+  <si>
+    <t>{"error": {"code": "101", "message": "partnerId must not be empty"}, "success": false}</t>
+  </si>
+  <si>
+    <t>{"success":"False"}</t>
+  </si>
+  <si>
+    <t>营销信息-获取营销信息</t>
+  </si>
+  <si>
+    <t>/api/marketing/v290/get-marketing-info</t>
+  </si>
+  <si>
+    <t>正常拉取会员加购位</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "5456925","orderAmount": "100", "factor": ""}</t>
+  </si>
+  <si>
+    <t>{"data": {"buyPlaceList": []}, "success": true}</t>
+  </si>
+  <si>
+    <t>金额传入负数</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "5456925","orderAmount": "-100", "factor": ""}</t>
+  </si>
+  <si>
+    <t>金额传入-</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "5456925","orderAmount": "0", "factor": ""}</t>
+  </si>
+  <si>
+    <t>passToken不正确</t>
+  </si>
+  <si>
+    <t>{"processToken": "error_token","partnerId": "5456925","orderAmount": "100", "factor": ""}</t>
+  </si>
+  <si>
+    <t>{"error": {"code": "20004", "message": "娴佺▼鍑瘉澶辨晥"}, "success": false}</t>
+  </si>
+  <si>
+    <t>业务线不传</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "","orderAmount": "100", "factor": ""}</t>
+  </si>
+  <si>
+    <t>传入不支持的业务线</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "99999","orderAmount": "", "factor": ""}</t>
+  </si>
+  <si>
+    <t>支付流程-获取流程凭证</t>
+  </si>
+  <si>
+    <t>/api/api/pay-flow/v290/get-process-token</t>
+  </si>
+  <si>
+    <t>支付apk获取凭证</t>
+  </si>
+  <si>
+    <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
+  </si>
+  <si>
+    <t>{"data": {"expireTime": 1621243514755, "processToken": "2nzYJhTZ6aQ3pC2b5xMUJm"}, "success": true}</t>
+  </si>
+  <si>
+    <t>{"success": "True"}</t>
+  </si>
+  <si>
+    <t>msp获取凭证</t>
+  </si>
+  <si>
+    <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
+  </si>
+  <si>
+    <t>{"data": {"expireTime": 1621243514887, "processToken": "CeLec6zAuJwa6TtuhYwUw1"}, "success": true}</t>
+  </si>
+  <si>
+    <t>apk无账号获取凭证</t>
+  </si>
+  <si>
+    <t>{"data": {"expireTime": 1621243515005, "processToken": "B3vBN2z8LXyM22fiwCqbEf"}, "success": true}</t>
+  </si>
+  <si>
+    <t>msp无账号获取凭证</t>
+  </si>
+  <si>
+    <t>{"data": {"expireTime": 1621243515122, "processToken": "8vuWJ1kgwcnM1cuq75bfM9"}, "success": true}</t>
+  </si>
+  <si>
+    <t>msp获取凭证不传appId</t>
+  </si>
+  <si>
+    <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
+  </si>
+  <si>
+    <t>{"data": {"expireTime": 1621243515238, "processToken": "HabxCfQrgYtuYFeEKTAAJz"}, "success": true}</t>
+  </si>
+  <si>
+    <t>token传入不正确</t>
+  </si>
+  <si>
+    <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
+  </si>
+  <si>
+    <t>{"error": {"code": "20000", "message": "閴存潈澶辫触"}, "success": false}</t>
+  </si>
+  <si>
+    <t>{"success": "False"}</t>
+  </si>
+  <si>
+    <t>partnerCode不传</t>
+  </si>
+  <si>
+    <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "","platform": "ATLAS"}</t>
+  </si>
+  <si>
+    <t>{"error": {"code": "101", "message": "must not be blank"}, "success": false}</t>
+  </si>
+  <si>
+    <t>appPackage不传</t>
+  </si>
+  <si>
+    <t>{"token": "","appId": "","appPackage": "", "partnerCode": "2031","platform": "ATLAS"}</t>
+  </si>
+  <si>
+    <t>支付流程-获取支付渠道列表</t>
+  </si>
+  <si>
+    <t>/api/pay-flow/v290/list-pay-types</t>
+  </si>
+  <si>
+    <t>有账号+自动续费+全屏</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "2031","accountExist": "Y",
+"renewal": "Y", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鏀粯瀹濆鎵樹唬鎵�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "寰俊濮旀墭浠ｆ墸", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "11", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "wxpay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "alipay", "smallIcon": "", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
+  </si>
+  <si>
+    <t>有账号+自动续费+横屏(目前不支持)</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "Y",
+"renewal": "Y", "acrossScreen": "Y"}</t>
+  </si>
+  <si>
+    <t>{"data": {"payTypeList": []}, "success": true}</t>
+  </si>
+  <si>
+    <t>有账号+普通支付+全屏</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "Y",
+"renewal": "N", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>{"data": {"payTypeList": [{"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "10", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "绉嬭礉濂藉垎鏈焅t", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/finzpay_icon.png", "index": "0", "lastPayType": "N", "payType": "finzpay", "prompt": "finzpay", "smallIcon": "", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "9", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "0", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "4", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "7", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "8", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "6", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "1", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "3", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "2", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鑺卞憲鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/huabei.png", "index": "7", "lastPayType": "N", "payType": "alipay_hb", "prompt": "alipay_hb", "smallIcon": "", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "20", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "閾惰鍗�", "icon": "https://opayfs.nearme.com.cn/insidepay/images/near-me-y-v3.png", "index": "3", "lastPayType": "N", "payType": "bankplatform", "prompt": "鎺ㄨ崘鍌ㄨ搫鍗°�佷俊鐢ㄥ崱鎸佹湁鑰呬娇鐢�", "subscripts": []}, {"frontName": "娓告垙鐐瑰崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_game_default.png", "index": "5", "lastPayType": "N", "payType": "heepay", "prompt": "鏀寔楠忕綉涓�鍗￠�氥�佸彲甯佸崱", "subscripts": []}, {"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鎵嬫満鍏呭�煎崱", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_charge.png", "index": "4", "lastPayType": "N", "payType": "szfpay", "prompt": "鏀寔绉诲姩銆佽仈閫氥�佺數淇＄殑鍏呭�煎崱", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}]}, "success": true}</t>
+  </si>
+  <si>
+    <t>有账号+普通支付+横屏</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "Y",
+"renewal": "N", "acrossScreen": "Y"}</t>
+  </si>
+  <si>
+    <t>{"data": {"payTypeList": [{"frontName": "OPPO Pay 锛堟帹鑽愶級", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/oppopay.png", "index": "6", "lastPayType": "N", "payType": "oppopay", "prompt": "OPPO Pay", "smallIcon": "https://opayfs.nearme.com.cn/images/insidepay/images/union-small.png", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "寰俊鏀粯", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/icon_nowpay.png", "index": "1", "lastPayType": "N", "payType": "wxpay", "prompt": "鎺ㄨ崘寰俊缁戝崱鐢ㄦ埛浣跨敤", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "QQ閽卞寘", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/qqwallet_icon.png", "index": "2", "lastPayType": "N", "payType": "qqwallet", "prompt": "鎺ㄨ崘鏈夎储浠橀�氳处鍙枫�丵Q璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}, {"frontName": "鏀粯瀹�", "icon": "https://opayfs.nearme.com.cn/images/insidepay/images/alipay2.png", "index": "0", "lastPayType": "N", "payType": "alipay", "prompt": "鎺ㄨ崘鏈夋敮浠樺疂璐﹀彿鐨勭敤鎴蜂娇鐢�", "subscripts": []}]}, "success": true}</t>
+  </si>
+  <si>
+    <t>无账号+普通支付+全屏</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "N",
+"renewal": "N", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>无账号+普通支付+横屏(目前不支持)</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "N",
+"renewal": "N", "acrossScreen": "Y"}</t>
+  </si>
+  <si>
+    <t>无账号+自动续费+全屏(目前不支持)</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "N",
+"renewal": "Y", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>无账号+自动续费+横屏(目前不支持)</t>
+  </si>
+  <si>
+    <t>{"processToken": "",
+"partnerId": "2031","accountExist": "N",
+"renewal": "Y", "acrossScreen": "Y"}</t>
+  </si>
+  <si>
+    <t>proceessToken传入不正确</t>
+  </si>
+  <si>
+    <t>{"processToken": "ERROR_TOKEN",
+"partnerId": "2031","accountExist": "Y",
+"renewal": "Y", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "","accountExist": "Y",
+"renewal": "Y", "acrossScreen": "N"}</t>
+  </si>
+  <si>
+    <t>partnerId不存在</t>
+  </si>
+  <si>
+    <t>{"processToken": "","partnerId": "88888888888888","accountExist": "Y",
+"renewal": "Y", "acrossScreen": "N"}</t>
   </si>
 </sst>
 </file>
@@ -792,13 +1059,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="h:mm\ AM/PM"/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -838,6 +1105,18 @@
       <charset val="134"/>
     </font>
     <font>
+      <sz val="9.75"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="微软雅黑"/>
@@ -848,13 +1127,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -873,21 +1145,50 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
@@ -919,58 +1220,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -987,9 +1236,39 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1016,7 +1295,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1028,55 +1355,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1094,7 +1385,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1106,73 +1463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1184,19 +1475,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1243,15 +1522,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
@@ -1262,7 +1532,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1297,6 +1567,26 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1311,17 +1601,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -1330,10 +1609,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="7">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="6">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0">
@@ -1342,137 +1621,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="0">
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="6">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="5">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="8">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="7">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="9">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="5">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="25" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="4">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="9">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="6">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="2">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="8">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="19" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1508,10 +1787,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1963,7 +2263,7 @@
       <c r="D8" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E8" s="20" t="s">
+      <c r="E8" s="27" t="s">
         <v>22</v>
       </c>
       <c r="F8" s="10">
@@ -2022,7 +2322,7 @@
       <c r="D11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="E11" s="20" t="s">
+      <c r="E11" s="27" t="s">
         <v>29</v>
       </c>
       <c r="F11" s="10">
@@ -2047,7 +2347,7 @@
       <c r="D12" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="27" t="s">
         <v>33</v>
       </c>
       <c r="F12" s="10">
@@ -2072,7 +2372,7 @@
       <c r="D13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="27" t="s">
         <v>33</v>
       </c>
       <c r="F13" s="10">
@@ -2097,7 +2397,7 @@
       <c r="D14" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="20" t="s">
+      <c r="E14" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F14" s="10">
@@ -2122,7 +2422,7 @@
       <c r="D15" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="27" t="s">
         <v>44</v>
       </c>
       <c r="F15" s="10">
@@ -2147,7 +2447,7 @@
       <c r="D16" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="28" t="s">
         <v>47</v>
       </c>
       <c r="F16" s="10">
@@ -2172,7 +2472,7 @@
       <c r="D17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="27" t="s">
         <v>50</v>
       </c>
       <c r="F17" s="10">
@@ -2197,7 +2497,7 @@
       <c r="D18" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="27" t="s">
         <v>40</v>
       </c>
       <c r="F18" s="10">
@@ -2244,7 +2544,7 @@
       <c r="C20" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="26" t="s">
         <v>58</v>
       </c>
       <c r="E20" s="5"/>
@@ -2267,7 +2567,7 @@
       <c r="C21" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="26" t="s">
         <v>61</v>
       </c>
       <c r="E21" s="5"/>
@@ -2290,7 +2590,7 @@
       <c r="C22" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D22" s="19" t="s">
+      <c r="D22" s="26" t="s">
         <v>63</v>
       </c>
       <c r="E22" s="5"/>
@@ -2341,7 +2641,7 @@
       <c r="D24" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="E24" s="20" t="s">
+      <c r="E24" s="27" t="s">
         <v>69</v>
       </c>
       <c r="F24" s="10">
@@ -2537,7 +2837,7 @@
       <c r="D32" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E32" s="20" t="s">
+      <c r="E32" s="27" t="s">
         <v>87</v>
       </c>
       <c r="F32" s="10">
@@ -2562,7 +2862,7 @@
       <c r="D33" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="E33" s="20" t="s">
+      <c r="E33" s="27" t="s">
         <v>91</v>
       </c>
       <c r="F33" s="10">
@@ -2587,7 +2887,7 @@
       <c r="D34" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="27" t="s">
         <v>94</v>
       </c>
       <c r="F34" s="10">
@@ -2612,7 +2912,7 @@
       <c r="D35" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="20" t="s">
+      <c r="E35" s="27" t="s">
         <v>97</v>
       </c>
       <c r="F35" s="10">
@@ -2637,7 +2937,7 @@
       <c r="D36" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E36" s="27" t="s">
         <v>101</v>
       </c>
       <c r="F36" s="10">
@@ -2662,7 +2962,7 @@
       <c r="D37" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="E37" s="20" t="s">
+      <c r="E37" s="27" t="s">
         <v>104</v>
       </c>
       <c r="F37" s="10">
@@ -2687,7 +2987,7 @@
       <c r="D38" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E38" s="27" t="s">
         <v>33</v>
       </c>
       <c r="F38" s="10">
@@ -2712,7 +3012,7 @@
       <c r="D39" s="9" t="s">
         <v>109</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E39" s="27" t="s">
         <v>110</v>
       </c>
       <c r="F39" s="10">
@@ -2737,7 +3037,7 @@
       <c r="D40" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="20" t="s">
+      <c r="E40" s="27" t="s">
         <v>113</v>
       </c>
       <c r="F40" s="10">
@@ -2762,7 +3062,7 @@
       <c r="D41" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E41" s="20" t="s">
+      <c r="E41" s="27" t="s">
         <v>116</v>
       </c>
       <c r="F41" s="10">
@@ -2787,7 +3087,7 @@
       <c r="D42" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="E42" s="20" t="s">
+      <c r="E42" s="27" t="s">
         <v>119</v>
       </c>
       <c r="F42" s="10">
@@ -2812,7 +3112,7 @@
       <c r="D43" s="9" t="s">
         <v>121</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E43" s="27" t="s">
         <v>122</v>
       </c>
       <c r="F43" s="10">
@@ -2862,7 +3162,7 @@
       <c r="D45" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E45" s="20" t="s">
+      <c r="E45" s="27" t="s">
         <v>130</v>
       </c>
       <c r="F45" s="10">
@@ -2937,7 +3237,7 @@
       <c r="D48" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="E48" s="20" t="s">
+      <c r="E48" s="27" t="s">
         <v>141</v>
       </c>
       <c r="F48" s="10">
@@ -3012,7 +3312,7 @@
       <c r="D51" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="E51" s="20" t="s">
+      <c r="E51" s="27" t="s">
         <v>148</v>
       </c>
       <c r="F51" s="10">
@@ -3072,6 +3372,663 @@
     </row>
   </sheetData>
   <autoFilter ref="A6:I53"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I28"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A7" sqref="$A7:$XFD28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="49.1583333333333" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4416666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.1083333333333" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.775" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.775" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1083333333333" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.8916666666667" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="22" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" ht="22" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" ht="22" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="22" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" ht="22" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" ht="22" customHeight="1" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="E7" s="27" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="10">
+        <v>200</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="10">
+        <v>200</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A9" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="F9" s="10">
+        <v>200</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="11"/>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A10" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F10" s="10">
+        <v>200</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="10">
+        <v>200</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A12" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="F12" s="10">
+        <v>200</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="H12" s="11"/>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A13" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="F13" s="10">
+        <v>200</v>
+      </c>
+      <c r="G13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="H13" s="11"/>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A14" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="10">
+        <v>200</v>
+      </c>
+      <c r="G14" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H14" s="11"/>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="F15" s="10">
+        <v>200</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="H15" s="11"/>
+      <c r="I15" s="11"/>
+    </row>
+    <row r="16" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A16" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="E16" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" s="10">
+        <v>200</v>
+      </c>
+      <c r="G16" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+    </row>
+    <row r="17" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A17" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="E17" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="10">
+        <v>200</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="H17" s="11"/>
+      <c r="I17" s="11"/>
+    </row>
+    <row r="18" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A18" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E18" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="F18" s="10">
+        <v>200</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+    </row>
+    <row r="19" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A19" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="F19" s="10">
+        <v>200</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="H19" s="11"/>
+      <c r="I19" s="11"/>
+    </row>
+    <row r="20" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A20" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="10">
+        <v>200</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="11"/>
+      <c r="I20" s="11"/>
+    </row>
+    <row r="21" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A21" s="12" t="s">
+        <v>132</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F21" s="10">
+        <v>200</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>135</v>
+      </c>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11"/>
+    </row>
+    <row r="22" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A22" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="F22" s="10">
+        <v>200</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+    </row>
+    <row r="23" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A23" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" s="10">
+        <v>200</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="11"/>
+      <c r="I23" s="11"/>
+    </row>
+    <row r="24" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A24" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F24" s="10">
+        <v>500</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="11"/>
+      <c r="I24" s="11"/>
+    </row>
+    <row r="25" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A25" s="12" t="s">
+        <v>144</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="E25" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25" s="10">
+        <v>500</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" s="11"/>
+      <c r="I25" s="11"/>
+    </row>
+    <row r="26" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A26" s="12" t="s">
+        <v>146</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>148</v>
+      </c>
+      <c r="F26" s="10">
+        <v>200</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H26" s="11"/>
+      <c r="I26" s="11"/>
+    </row>
+    <row r="27" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A27" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="9"/>
+      <c r="F27" s="10">
+        <v>200</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H27" s="11"/>
+      <c r="I27" s="11"/>
+    </row>
+    <row r="28" ht="15.75" customHeight="1" spans="1:9">
+      <c r="A28" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E28" s="9"/>
+      <c r="F28" s="10">
+        <v>200</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A6:I28"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -3082,8 +4039,8 @@
   <sheetPr/>
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
@@ -3176,7 +4133,7 @@
       <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="19" t="s">
+      <c r="D7" s="26" t="s">
         <v>154</v>
       </c>
       <c r="E7" s="7" t="s">
@@ -3203,7 +4160,7 @@
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="19" t="s">
+      <c r="D8" s="26" t="s">
         <v>158</v>
       </c>
       <c r="E8" s="7" t="s">
@@ -3230,7 +4187,7 @@
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="26" t="s">
         <v>161</v>
       </c>
       <c r="E9" s="7" t="s">
@@ -3257,7 +4214,7 @@
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="19" t="s">
+      <c r="D10" s="26" t="s">
         <v>161</v>
       </c>
       <c r="E10" s="7" t="s">
@@ -3287,7 +4244,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5" outlineLevelRow="5"/>
@@ -3477,7 +4434,7 @@
   <dimension ref="A1:N12"/>
   <sheetViews>
     <sheetView zoomScale="95" zoomScaleNormal="95" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3500,7 +4457,7 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="20" t="s">
         <v>165</v>
       </c>
     </row>
@@ -3508,7 +4465,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="20" t="s">
         <v>166</v>
       </c>
     </row>
@@ -3516,7 +4473,7 @@
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="13" t="s">
+      <c r="B3" s="20" t="s">
         <v>5</v>
       </c>
     </row>
@@ -3524,13 +4481,13 @@
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="14"/>
+      <c r="B4" s="21"/>
     </row>
     <row r="5" ht="21" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="14"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" ht="20" customHeight="1" spans="1:14">
       <c r="A6" s="6" t="s">
@@ -3577,43 +4534,43 @@
       </c>
     </row>
     <row r="7" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="22" t="s">
         <v>180</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="22" t="s">
         <v>182</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>184</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="22" t="s">
         <v>185</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="22" t="s">
         <v>186</v>
       </c>
-      <c r="H7" s="15" t="s">
+      <c r="H7" s="22" t="s">
         <v>187</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="J7" s="15" t="s">
+      <c r="J7" s="22" t="s">
         <v>189</v>
       </c>
-      <c r="K7" s="15" t="s">
+      <c r="K7" s="22" t="s">
         <v>190</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="22" t="s">
         <v>191</v>
       </c>
-      <c r="M7" s="15" t="s">
+      <c r="M7" s="22" t="s">
         <v>192</v>
       </c>
       <c r="N7" t="s">
@@ -3621,181 +4578,181 @@
       </c>
     </row>
     <row r="8" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A8" s="16">
+      <c r="A8" s="23">
         <v>1</v>
       </c>
       <c r="B8" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="24">
         <v>1</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="24">
         <f ca="1" t="shared" ref="D8:D12" si="0">RANDBETWEEN(1,10)</f>
-        <v>3</v>
-      </c>
-      <c r="E8" s="17">
+        <v>7</v>
+      </c>
+      <c r="E8" s="24">
         <f ca="1" t="shared" ref="E8:E12" si="1">RANDBETWEEN(D8,9999)</f>
-        <v>1231</v>
-      </c>
-      <c r="F8" s="17">
+        <v>4233</v>
+      </c>
+      <c r="F8" s="24">
         <f ca="1" t="shared" ref="F8:F12" si="2">ROUND(RAND(),2)</f>
-        <v>0.16</v>
-      </c>
-      <c r="G8" s="18"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="17"/>
-      <c r="L8" s="17">
+        <v>0.26</v>
+      </c>
+      <c r="G8" s="25"/>
+      <c r="H8" s="24"/>
+      <c r="I8" s="24"/>
+      <c r="J8" s="24"/>
+      <c r="K8" s="24"/>
+      <c r="L8" s="24">
         <f ca="1" t="shared" ref="L8:L12" si="3">RANDBETWEEN(0,1)</f>
         <v>1</v>
       </c>
-      <c r="M8" s="17"/>
+      <c r="M8" s="24"/>
       <c r="N8" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="9" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A9" s="16">
+      <c r="A9" s="23">
         <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>195</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="24">
         <v>1</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="24">
         <f ca="1" t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="E9" s="17">
+        <v>8</v>
+      </c>
+      <c r="E9" s="24">
         <f ca="1">RANDBETWEEN(D9,20)</f>
-        <v>7</v>
-      </c>
-      <c r="F9" s="17">
+        <v>12</v>
+      </c>
+      <c r="F9" s="24">
         <f ca="1" t="shared" si="2"/>
-        <v>0.6</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="17"/>
-      <c r="J9" s="17"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17">
+        <v>0.26</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24">
         <f ca="1" t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M9" s="17"/>
+      <c r="M9" s="24"/>
       <c r="N9" t="s">
         <v>195</v>
       </c>
     </row>
     <row r="10" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A10" s="16">
+      <c r="A10" s="23">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>196</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="24">
         <v>1</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="24">
         <f ca="1" t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="E10" s="17">
+        <v>4</v>
+      </c>
+      <c r="E10" s="24">
         <f ca="1" t="shared" si="1"/>
-        <v>9550</v>
-      </c>
-      <c r="F10" s="17">
+        <v>8523</v>
+      </c>
+      <c r="F10" s="24">
         <f ca="1" t="shared" si="2"/>
-        <v>0.82</v>
-      </c>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="17"/>
-      <c r="J10" s="17"/>
-      <c r="K10" s="17"/>
-      <c r="L10" s="17">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="24"/>
+      <c r="H10" s="24"/>
+      <c r="I10" s="24"/>
+      <c r="J10" s="24"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24">
+        <f ca="1" t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="M10" s="24"/>
+      <c r="N10" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="11" ht="15.6" customHeight="1" spans="1:14">
+      <c r="A11" s="23">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="24">
+        <v>1</v>
+      </c>
+      <c r="D11" s="24">
+        <f ca="1" t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E11" s="24">
+        <f ca="1" t="shared" si="1"/>
+        <v>8593</v>
+      </c>
+      <c r="F11" s="24">
+        <f ca="1" t="shared" si="2"/>
+        <v>0.32</v>
+      </c>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+      <c r="K11" s="24"/>
+      <c r="L11" s="24">
         <f ca="1" t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M10" s="17"/>
-      <c r="N10" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="11" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A11" s="16">
+      <c r="M11" s="24"/>
+      <c r="N11" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" ht="15.6" customHeight="1" spans="1:14">
+      <c r="A12" s="23">
+        <v>8</v>
+      </c>
+      <c r="B12" t="s">
+        <v>199</v>
+      </c>
+      <c r="C12" s="24">
+        <v>1</v>
+      </c>
+      <c r="D12" s="24">
+        <f ca="1" t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B11" t="s">
-        <v>197</v>
-      </c>
-      <c r="C11" s="17">
-        <v>1</v>
-      </c>
-      <c r="D11" s="17">
-        <f ca="1" t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E11" s="17">
+      <c r="E12" s="24">
         <f ca="1" t="shared" si="1"/>
-        <v>5214</v>
-      </c>
-      <c r="F11" s="17">
+        <v>1895</v>
+      </c>
+      <c r="F12" s="24">
         <f ca="1" t="shared" si="2"/>
-        <v>0.17</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="17"/>
-      <c r="J11" s="17"/>
-      <c r="K11" s="17"/>
-      <c r="L11" s="17">
+        <v>0.19</v>
+      </c>
+      <c r="G12" s="24"/>
+      <c r="H12" s="24"/>
+      <c r="I12" s="24"/>
+      <c r="J12" s="24"/>
+      <c r="K12" s="24"/>
+      <c r="L12" s="24">
         <f ca="1" t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="M11" s="17"/>
-      <c r="N11" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="12" ht="15.6" customHeight="1" spans="1:14">
-      <c r="A12" s="16">
-        <v>8</v>
-      </c>
-      <c r="B12" t="s">
-        <v>199</v>
-      </c>
-      <c r="C12" s="17">
-        <v>1</v>
-      </c>
-      <c r="D12" s="17">
-        <f ca="1" t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="E12" s="17">
-        <f ca="1" t="shared" si="1"/>
-        <v>2710</v>
-      </c>
-      <c r="F12" s="17">
-        <f ca="1" t="shared" si="2"/>
-        <v>0.4</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="17"/>
-      <c r="J12" s="17"/>
-      <c r="K12" s="17"/>
-      <c r="L12" s="17">
-        <f ca="1" t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="M12" s="17"/>
+      <c r="M12" s="24"/>
       <c r="N12" t="s">
         <v>200</v>
       </c>
@@ -3809,16 +4766,190 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="A7" sqref="$A7:$XFD28"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.89166666666667" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="49.1583333333333" style="1" customWidth="1"/>
-    <col min="2" max="2" width="29.5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="26.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="27.625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4416666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.775" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.775" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1083333333333" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" ht="18" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="27" customHeight="1" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="F7" s="10">
+        <v>200</v>
+      </c>
+      <c r="G7" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" ht="27" customHeight="1" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="17" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="F8" s="10">
+        <v>200</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" ht="27" customHeight="1" spans="1:9">
+      <c r="A9" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="F9" s="10">
+        <v>200</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="25.875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.4416666666667" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.1083333333333" style="1" customWidth="1"/>
     <col min="5" max="5" width="45.6666666666667" style="1" customWidth="1"/>
@@ -3826,26 +4957,25 @@
     <col min="7" max="7" width="24.775" style="1" customWidth="1"/>
     <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
     <col min="9" max="9" width="21.1083333333333" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.8916666666667" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="22" customHeight="1" spans="1:2">
+    <row r="1" ht="18" customHeight="1" spans="1:2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" ht="22" customHeight="1" spans="1:2">
+      <c r="B1" s="13" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:2">
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" ht="22" customHeight="1" spans="1:2">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1" spans="1:2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -3853,19 +4983,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" ht="22" customHeight="1" spans="1:2">
+    <row r="4" ht="18" customHeight="1" spans="1:2">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" ht="22" customHeight="1" spans="1:2">
+    <row r="5" ht="18" customHeight="1" spans="1:2">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" ht="22" customHeight="1" spans="1:9">
+    <row r="6" ht="18" customHeight="1" spans="1:9">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
@@ -3894,554 +5024,868 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" ht="15.75" customHeight="1" spans="1:9">
+    <row r="7" ht="50" customHeight="1" spans="1:9">
       <c r="A7" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>27</v>
+        <v>216</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="E7" s="20" t="s">
-        <v>87</v>
+      <c r="D7" s="16" t="s">
+        <v>217</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="F7" s="10">
         <v>200</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>88</v>
-      </c>
-      <c r="H7" s="11"/>
+        <v>206</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I7" s="11"/>
     </row>
-    <row r="8" ht="15.75" customHeight="1" spans="1:9">
+    <row r="8" ht="50" customHeight="1" spans="1:9">
       <c r="A8" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="B8" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="B8" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="E8" s="20" t="s">
-        <v>91</v>
+      <c r="D8" s="16" t="s">
+        <v>220</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>218</v>
       </c>
       <c r="F8" s="10">
         <v>200</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H8" s="11"/>
+        <v>206</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="7"/>
+    </row>
+    <row r="9" ht="50" customHeight="1" spans="1:9">
+      <c r="A9" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F9" s="10">
+        <v>200</v>
+      </c>
+      <c r="G9" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="7"/>
+    </row>
+    <row r="10" ht="50" customHeight="1" spans="1:9">
+      <c r="A10" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>224</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>225</v>
+      </c>
+      <c r="F10" s="10">
+        <v>200</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="7"/>
+    </row>
+    <row r="11" ht="50" customHeight="1" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>227</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>212</v>
+      </c>
+      <c r="F11" s="10">
+        <v>200</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I11" s="7"/>
+    </row>
+    <row r="12" ht="50" customHeight="1" spans="1:9">
+      <c r="A12" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>218</v>
+      </c>
+      <c r="F12" s="10">
+        <v>200</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="H12" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="7"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4416666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="50" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.775" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1083333333333" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" ht="18" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="50" customHeight="1" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="F7" s="10">
+        <v>200</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" ht="50" customHeight="1" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="F8" s="10">
+        <v>200</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I8" s="11"/>
     </row>
-    <row r="9" ht="15.75" customHeight="1" spans="1:9">
+    <row r="9" ht="50" customHeight="1" spans="1:9">
       <c r="A9" s="7" t="s">
-        <v>92</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>239</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>94</v>
+      <c r="D9" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>240</v>
       </c>
       <c r="F9" s="10">
         <v>200</v>
       </c>
-      <c r="G9" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H9" s="11"/>
+      <c r="G9" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I9" s="11"/>
     </row>
-    <row r="10" ht="15.75" customHeight="1" spans="1:9">
+    <row r="10" ht="50" customHeight="1" spans="1:9">
       <c r="A10" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>27</v>
+        <v>241</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E10" s="20" t="s">
-        <v>97</v>
+      <c r="D10" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>242</v>
       </c>
       <c r="F10" s="10">
         <v>200</v>
       </c>
-      <c r="G10" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H10" s="11"/>
+      <c r="G10" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I10" s="11"/>
     </row>
-    <row r="11" ht="15.75" customHeight="1" spans="1:9">
+    <row r="11" ht="50" customHeight="1" spans="1:9">
       <c r="A11" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>27</v>
+        <v>243</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
       </c>
       <c r="C11" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="9" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11" s="20" t="s">
-        <v>101</v>
+      <c r="D11" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>245</v>
       </c>
       <c r="F11" s="10">
         <v>200</v>
       </c>
-      <c r="G11" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H11" s="11"/>
+      <c r="G11" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I11" s="11"/>
     </row>
-    <row r="12" ht="15.75" customHeight="1" spans="1:9">
+    <row r="12" ht="50" customHeight="1" spans="1:9">
       <c r="A12" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="B12" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="B12" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="E12" s="20" t="s">
-        <v>104</v>
+      <c r="D12" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>248</v>
       </c>
       <c r="F12" s="10">
         <v>200</v>
       </c>
-      <c r="G12" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H12" s="11"/>
+      <c r="G12" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I12" s="11"/>
     </row>
-    <row r="13" ht="15.75" customHeight="1" spans="1:9">
+    <row r="13" ht="50" customHeight="1" spans="1:9">
       <c r="A13" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B13" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="B13" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>33</v>
+      <c r="D13" s="15" t="s">
+        <v>251</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="F13" s="10">
         <v>200</v>
       </c>
-      <c r="G13" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H13" s="11"/>
+      <c r="G13" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" ht="15.75" customHeight="1" spans="1:9">
+    <row r="14" ht="50" customHeight="1" spans="1:9">
       <c r="A14" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B14" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="B14" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="9" t="s">
-        <v>109</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>110</v>
+      <c r="D14" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>252</v>
       </c>
       <c r="F14" s="10">
         <v>200</v>
       </c>
-      <c r="G14" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="11"/>
+      <c r="G14" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I14" s="11"/>
     </row>
-    <row r="15" ht="15.75" customHeight="1" spans="1:9">
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <cols>
+    <col min="1" max="1" width="32.25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.4416666666667" style="1" customWidth="1"/>
+    <col min="4" max="4" width="48.375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="45.6666666666667" style="1" customWidth="1"/>
+    <col min="6" max="6" width="13.775" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.775" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6666666666667" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.1083333333333" style="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="18" customHeight="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="2" ht="18" customHeight="1" spans="1:2">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" ht="18" customHeight="1" spans="1:2">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" ht="18" customHeight="1" spans="1:2">
+      <c r="A4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="5"/>
+    </row>
+    <row r="5" ht="18" customHeight="1" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" ht="18" customHeight="1" spans="1:9">
+      <c r="A6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" ht="24" customHeight="1" spans="1:9">
+      <c r="A7" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="10">
+        <v>200</v>
+      </c>
+      <c r="G7" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H7" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I7" s="11"/>
+    </row>
+    <row r="8" ht="24" customHeight="1" spans="1:9">
+      <c r="A8" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E8" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F8" s="10">
+        <v>200</v>
+      </c>
+      <c r="G8" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H8" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I8" s="11"/>
+    </row>
+    <row r="9" ht="24" customHeight="1" spans="1:9">
+      <c r="A9" s="7" t="s">
+        <v>263</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="E9" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F9" s="10">
+        <v>200</v>
+      </c>
+      <c r="G9" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I9" s="11"/>
+    </row>
+    <row r="10" ht="24" customHeight="1" spans="1:9">
+      <c r="A10" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="10">
+        <v>200</v>
+      </c>
+      <c r="G10" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H10" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I10" s="11"/>
+    </row>
+    <row r="11" ht="24" customHeight="1" spans="1:9">
+      <c r="A11" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>265</v>
+      </c>
+      <c r="F11" s="10">
+        <v>200</v>
+      </c>
+      <c r="G11" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H11" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I11" s="11"/>
+    </row>
+    <row r="12" ht="24" customHeight="1" spans="1:9">
+      <c r="A12" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="B12" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>272</v>
+      </c>
+      <c r="E12" s="16" t="s">
+        <v>268</v>
+      </c>
+      <c r="F12" s="10">
+        <v>200</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H12" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I12" s="11"/>
+    </row>
+    <row r="13" ht="24" customHeight="1" spans="1:9">
+      <c r="A13" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>274</v>
+      </c>
+      <c r="E13" s="16" t="s">
+        <v>259</v>
+      </c>
+      <c r="F13" s="10">
+        <v>200</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="I13" s="11"/>
+    </row>
+    <row r="14" ht="24" customHeight="1" spans="1:9">
+      <c r="A14" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="E14" s="16" t="s">
+        <v>262</v>
+      </c>
+      <c r="F14" s="10">
+        <v>200</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H14" s="10" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="11"/>
+    </row>
+    <row r="15" ht="24" customHeight="1" spans="1:9">
       <c r="A15" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="B15" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="9" t="s">
-        <v>112</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>113</v>
+      <c r="D15" s="15" t="s">
+        <v>278</v>
+      </c>
+      <c r="E15" s="16" t="s">
+        <v>225</v>
       </c>
       <c r="F15" s="10">
         <v>200</v>
       </c>
-      <c r="G15" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="11"/>
+      <c r="G15" s="17" t="s">
+        <v>249</v>
+      </c>
+      <c r="H15" s="18" t="s">
+        <v>156</v>
+      </c>
       <c r="I15" s="11"/>
     </row>
-    <row r="16" ht="15.75" customHeight="1" spans="1:9">
+    <row r="16" ht="24" customHeight="1" spans="1:9">
       <c r="A16" s="7" t="s">
-        <v>114</v>
-      </c>
-      <c r="B16" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>116</v>
+      <c r="D16" s="15" t="s">
+        <v>279</v>
+      </c>
+      <c r="E16" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="F16" s="10">
         <v>200</v>
       </c>
-      <c r="G16" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H16" s="11"/>
+      <c r="G16" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H16" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="I16" s="11"/>
     </row>
-    <row r="17" ht="15.75" customHeight="1" spans="1:9">
+    <row r="17" ht="24" customHeight="1" spans="1:9">
       <c r="A17" s="7" t="s">
-        <v>117</v>
-      </c>
-      <c r="B17" s="4" t="s">
+        <v>280</v>
+      </c>
+      <c r="B17" s="14" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>118</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>119</v>
+      <c r="D17" s="15" t="s">
+        <v>281</v>
+      </c>
+      <c r="E17" s="16" t="s">
+        <v>262</v>
       </c>
       <c r="F17" s="10">
         <v>200</v>
       </c>
-      <c r="G17" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="11"/>
+      <c r="G17" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>156</v>
+      </c>
       <c r="I17" s="11"/>
     </row>
-    <row r="18" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A18" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C18" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="E18" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="F18" s="10">
-        <v>200</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-    </row>
-    <row r="19" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A19" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C19" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="F19" s="10">
-        <v>200</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-    </row>
-    <row r="20" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A20" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>130</v>
-      </c>
-      <c r="F20" s="10">
-        <v>200</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>131</v>
-      </c>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-    </row>
-    <row r="21" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A21" s="12" t="s">
-        <v>132</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>133</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F21" s="10">
-        <v>200</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>135</v>
-      </c>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-    </row>
-    <row r="22" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A22" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>137</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>138</v>
-      </c>
-      <c r="F22" s="10">
-        <v>200</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-    </row>
-    <row r="23" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A23" s="5" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="E23" s="20" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" s="10">
-        <v>200</v>
-      </c>
-      <c r="G23" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-    </row>
-    <row r="24" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A24" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>143</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F24" s="10">
-        <v>500</v>
-      </c>
-      <c r="G24" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-    </row>
-    <row r="25" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A25" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>145</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="F25" s="10">
-        <v>500</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-    </row>
-    <row r="26" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A26" s="12" t="s">
-        <v>146</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="E26" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="F26" s="10">
-        <v>200</v>
-      </c>
-      <c r="G26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-    </row>
-    <row r="27" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A27" s="12" t="s">
-        <v>149</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="E27" s="9"/>
-      <c r="F27" s="10">
-        <v>200</v>
-      </c>
-      <c r="G27" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-    </row>
-    <row r="28" ht="15.75" customHeight="1" spans="1:9">
-      <c r="A28" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="E28" s="9"/>
-      <c r="F28" s="10">
-        <v>200</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A6:I28"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>

<commit_message>
fix refactor testcase bug
</commit_message>
<xml_diff>
--- a/case/src/http/inland.xlsx
+++ b/case/src/http/inland.xlsx
@@ -123,14 +123,6 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
       <color rgb="FF0000FF"/>
       <sz val="11"/>
       <u val="single"/>
@@ -139,7 +131,7 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -153,16 +145,16 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
+      <charset val="0"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -189,48 +181,10 @@
     </font>
     <font>
       <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
       <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -250,9 +204,55 @@
     </font>
     <font>
       <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFA7D00"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="15"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
       <charset val="0"/>
       <b val="1"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F3F"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -260,7 +260,7 @@
       <name val="宋体"/>
       <charset val="0"/>
       <b val="1"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -286,13 +286,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -304,13 +310,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -328,13 +340,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,13 +370,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -370,25 +388,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -400,19 +400,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -430,13 +430,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -448,25 +454,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -491,24 +491,6 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,18 +544,16 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -592,6 +572,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -600,10 +600,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -612,133 +612,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="11" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="9" borderId="9" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="21" borderId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4358,7 +4358,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4491,12 +4491,12 @@
       </c>
       <c r="D7" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "SWngK5Xd2Fv98jKt6sdBuN", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "PTsvpZ19BHF6ozS4mCWilRxE70gjd2nf", "amount": 1, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "2069d49e01f9aadc611f8bb80bd249f5", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "GTysNSPeKBAV2tRk9Enr5X4lOHa8bgu3", "amount": 1, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "a72ba1d3f1c036a3d4d0811d42f48b12", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"242f25b311b942ae87af5f0420378097\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211534428058e915a0599b17b5c10000\",\"sign\":\"05E9B1060897A84414E0E7AC77DFF40B\",\"timestamp\":\"1625577334\"}", "payRequestId": "RM20210706211534208677696912422t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"0a6fdbae25f14a24b008f0239eacb377\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx071453501846390efb906757bf73190000\",\"sign\":\"CD8D9229B9D79F9BDAF68547113E48EA\",\"timestamp\":\"1625640830\"}", "payRequestId": "RM20210707145349208677696982538t"}, "success": true}</t>
         </is>
       </c>
       <c r="F7" s="10" t="n">
@@ -4512,8 +4512,10 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I7" s="11" t="n">
-        <v>1</v>
+      <c r="I7" s="11" t="inlineStr">
+        <is>
+          <t>1，currencySystem直扣必须填CASH</t>
+        </is>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1" s="1">
@@ -4534,12 +4536,12 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "GaGG6Ga8Mxt6X6Pcz8xioU", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "LXIQS6EqFROVciKpDBo1ZeawrAMst3Wn", "amount": 9999999, "productName": "test", "productDesc": "test paydirect pay-alipay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 9999999, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "b7ac1958ea82a14add8e01dfbe81a1c0", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "mpJU6YIu2kn8OqrNEHDobBtGjhyMse7w", "amount": 9999999, "productName": "test", "productDesc": "test paydirect pay-alipay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 9999999, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "f21a267af9854ea0ce6d246a7f8f63f8", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22RM20210706211534208677696910047t%22%26subject%3D%22test%22%26body%3D%22test+paydirect+pay-alipay%22%26total_fee%3D%2299999.99%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22rXPG7jH0ePg0FzX7uih%252Bil31JXiKa58H%252BAnOB4AZrdEgDGe%252FD9CeX1c3ZVHciDEFE3eZbA%252BnDLDRWUuaw8%252FOCxbzqAa2kkLWOxDsPtOr1FeUOAOkd0WUGbftMfZurwDOcuTTM%252Fbf9h44CPFGbmaTV0%252FTsR2crXYe%252FtJ0MrxcXIw%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"RM20210706211534208677696910047t\"}", "payRequestId": "RM20210706211534208677696910047t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22RM20210707145350208677696963552t%22%26subject%3D%22test%22%26body%3D%22test+paydirect+pay-alipay%22%26total_fee%3D%2299999.99%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22F%252BoNACBeZ9TxuGTuMVNcnAgkQ5abBC7j1HjOgm8tyiHTROZM02%252BCHJfL4uYyobzIxsPBzqw0tSikuieLc4xjytNwTBJTdwqo6uF3e44dcwlzXrFbRv9q3TciBigQJWTVHF7Bb0M4iwe%252FprxSBWU%252Fizr9nRCB5ddOJ8%252Br04kTTuc%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"RM20210707145350208677696963552t\"}", "payRequestId": "RM20210707145350208677696963552t"}, "success": true}</t>
         </is>
       </c>
       <c r="F8" s="10" t="n">
@@ -4555,8 +4557,10 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I8" s="11" t="n">
-        <v>9999999</v>
+      <c r="I8" s="11" t="inlineStr">
+        <is>
+          <t>9999999，currencySystem直扣必须填CASH</t>
+        </is>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1" s="1">
@@ -4577,7 +4581,7 @@
       </c>
       <c r="D9" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "PCbBVVDkGc6n4hhXGXLALp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "hpUf8rkQI97Z0JOmoTldaPB5xu1svtAX", "amount": 0, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 0, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "786bb0d9d0b8e48e5802b7652e6cdcab", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "r8a54YBOEmbwjDUC6KStsAfXIGF0TuJy", "amount": 0, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 0, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "926f50f42f8c4fa9e8a7f9e47dfef360", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
@@ -4598,8 +4602,10 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I9" s="11" t="n">
-        <v>0</v>
+      <c r="I9" s="11" t="inlineStr">
+        <is>
+          <t>0，currencySystem直扣必须填CASH</t>
+        </is>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1" s="1">
@@ -4620,7 +4626,7 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "Sb6cfXdH9D7Hj6BYFSsT8T", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "biHNJs1dXjpDro6EFWvCOl8KRcSwz3BL", "amount": 1.2, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1.2, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "bccfc7158746ef73c61afeb74e1b61df", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "mGUxjv2s0e7hyocLW3DrIPHJ6AVMXZpF", "amount": 1.2, "productName": "test", "productDesc": "test paydirect pay-wxpay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1.2, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "d969070794e9d76792a2f250e0ad064a", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
@@ -4641,14 +4647,16 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I10" s="11" t="n">
-        <v>1.2</v>
+      <c r="I10" s="11" t="inlineStr">
+        <is>
+          <t>1.2，currencySystem直扣必须填CASH</t>
+        </is>
       </c>
     </row>
     <row r="11" ht="15.75" customHeight="1" s="1">
       <c r="A11" s="7" t="inlineStr">
         <is>
-          <t>直扣-支付宝，currencySystem=COCOIN_ALLOWED</t>
+          <t>直扣-微信，携带消费券</t>
         </is>
       </c>
       <c r="B11" s="4" t="inlineStr">
@@ -4658,17 +4666,17 @@
       </c>
       <c r="C11" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "CAj71XS1qB13Bc3DfG9VZC", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "zIS49DstoYvObG5flJ02RHrunhe3yTCj", "amount": 1, "productName": "test", "productDesc": "test paydirect pay-alipay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "appKey": "2033", "sign": "5ca40d8a7612268206017d71b8830028", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "YNaRdW4VCp2J5Ffue9OAKq6sZmrtvXoD", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "1e932cd1a6656754bbc79a78cf11bc5a", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"payRequestId": "KB20210706211534208677696900883t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}, "success": false}</t>
         </is>
       </c>
       <c r="F11" s="10" t="n">
@@ -4676,7 +4684,7 @@
       </c>
       <c r="G11" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "RM20"}</t>
+          <t>{"success": false, "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}</t>
         </is>
       </c>
       <c r="H11" s="11" t="inlineStr">
@@ -4686,14 +4694,14 @@
       </c>
       <c r="I11" s="11" t="inlineStr">
         <is>
-          <t>1，标志是否允许用可币，不用也可以</t>
+          <t>1，currencySystem直扣必须填CASH</t>
         </is>
       </c>
     </row>
     <row r="12" ht="15.75" customHeight="1" s="1">
       <c r="A12" s="7" t="inlineStr">
         <is>
-          <t>直扣-微信，携带消费券</t>
+          <t>直扣-支付宝，携带可币券+可币</t>
         </is>
       </c>
       <c r="B12" s="4" t="inlineStr">
@@ -4708,7 +4716,7 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "2CKNFRGhNsoN4J9SdrjntM", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "HLph3GtQRVmr5B1bqnSZiwYux9gDTIaO", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "08a093ce128638ad78264b3cb03bf0b9", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "gkh9OMorvtlWD1cQXmA27biTzBd0uJ3y", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935506", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "1959a1d8ee7aef875d4886f8cb22dad8", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E12" s="7" t="inlineStr">
@@ -4721,7 +4729,7 @@
       </c>
       <c r="G12" s="11" t="inlineStr">
         <is>
-          <t>{"success": false, "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}</t>
+          <t>{"message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�","success":false}</t>
         </is>
       </c>
       <c r="H12" s="11" t="inlineStr">
@@ -4729,34 +4737,36 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I12" s="11" t="n">
-        <v>1</v>
+      <c r="I12" s="11" t="inlineStr">
+        <is>
+          <t>101，currencySystem直扣必须填CASH</t>
+        </is>
       </c>
     </row>
     <row r="13" ht="15.75" customHeight="1" s="1">
       <c r="A13" s="7" t="inlineStr">
         <is>
-          <t>直扣-支付宝，携带可币券+可币</t>
+          <t>纯可币</t>
         </is>
       </c>
       <c r="B13" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C13" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D13" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "GCh3JjD6djTsztwNZ4eri8", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "hQNKpsPVSz7l3W4a1EGjRkyAgfr0ib2m", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935540", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "270eabd792ebae5dcdaadebeb0e9c75e", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "ri25Y3VGqlbpj4Hu0R7OBmP8yFLNXkfa", "amount": 1, "productName": "test", "productDesc": "test pay only cocoin spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "a89589b684c530b29afc20dda5383917", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}, "success": false}</t>
+          <t>{"data": {"payRequestId": "KB20210707145350208677696925606t"}, "success": true}</t>
         </is>
       </c>
       <c r="F13" s="10" t="n">
@@ -4764,7 +4774,7 @@
       </c>
       <c r="G13" s="11" t="inlineStr">
         <is>
-          <t>{"message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�","success":false}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H13" s="11" t="inlineStr">
@@ -4773,13 +4783,13 @@
         </is>
       </c>
       <c r="I13" s="11" t="n">
-        <v>101</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" ht="15.75" customHeight="1" s="1">
       <c r="A14" s="7" t="inlineStr">
         <is>
-          <t>纯可币</t>
+          <t>纯可币券</t>
         </is>
       </c>
       <c r="B14" s="4" t="inlineStr">
@@ -4794,12 +4804,12 @@
       </c>
       <c r="D14" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "W7bBvvff8SDUQJnXky7hUZ", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "SerYW3TxlQZuyCgB9EI2UPjVcRdJLXmp", "amount": 1, "productName": "test", "productDesc": "test pay only cocoin spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "cd5dd11dc01be6e7c5dcdb2d8c5a7e08", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "N1Zpfnr4Sckx37lXgbuqyJOtMAe28C0m", "amount": 1, "productName": "test", "productDesc": "test pay only voucher spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "99181b1daa8eea028b6cacc442ef35aa", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"payRequestId": "KB20210706211535208677696945544t"}, "success": true}</t>
+          <t>{"data": {"payRequestId": "KB20210707145351208677696977435t"}, "success": true}</t>
         </is>
       </c>
       <c r="F14" s="10" t="n">
@@ -4822,7 +4832,7 @@
     <row r="15" ht="15.75" customHeight="1" s="1">
       <c r="A15" s="7" t="inlineStr">
         <is>
-          <t>纯可币券</t>
+          <t>纯可币+可币券</t>
         </is>
       </c>
       <c r="B15" s="4" t="inlineStr">
@@ -4837,12 +4847,12 @@
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "FiyjHMjwra4Zy3iyLT7rUs", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "el5iNnZ6m3czC2HAEyd1waIxGsvD8BqS", "amount": 1, "productName": "test", "productDesc": "test pay only voucher spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "20647782e8b8abdbd8e7e5811e40c492", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "sVjT3UM6bEF47HDp9SqmhfOo0gJZ8LKQ", "amount": 100, "productName": "test", "productDesc": "test pay only cocoin+voucher spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 100, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "45e412fa8fb9a0f76baf739d9abcf91b", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"payRequestId": "KB20210706211535208677696912625t"}, "success": true}</t>
+          <t>{"data": {"payRequestId": "KB20210707145351208677696953176t"}, "success": true}</t>
         </is>
       </c>
       <c r="F15" s="10" t="n">
@@ -4859,13 +4869,13 @@
         </is>
       </c>
       <c r="I15" s="11" t="n">
-        <v>1</v>
+        <v>100</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1" s="1">
       <c r="A16" s="7" t="inlineStr">
         <is>
-          <t>纯可币+可币券</t>
+          <t>可币+微信</t>
         </is>
       </c>
       <c r="B16" s="4" t="inlineStr">
@@ -4880,12 +4890,12 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "Eq73psPtibtN8MgHuTNvJH", "payType": "VIRTUAL_ASSETS", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "MufN1oJ4chXPi0wYergjSTIpmElBzHVR", "amount": 100, "productName": "test", "productDesc": "test pay only cocoin+voucher spend", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 100, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "36c0e92f9006205c335d7773110fb089", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "LiTkeGJx0mAbpotV6cQaBu8XjdDzZWvO", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 2, "cocoinDeductAmount": 2, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "967affcead901356cd50d092f2c4b9cc", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E16" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "222", "message": "鏀粯鏂瑰紡涓嶆敮鎸�:VIRTUAL_ASSETS"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"2c994dfa437143ce9bda0e4291bc6fed\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0714535190956452444a78b6396b1c0000\",\"sign\":\"77EB961CACEDB5E55A1EC1E70455DA2D\",\"timestamp\":\"1625640831\"}", "payRequestId": "KB20210707145351208677696926420t"}, "success": true}</t>
         </is>
       </c>
       <c r="F16" s="10" t="n">
@@ -4893,7 +4903,7 @@
       </c>
       <c r="G16" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": true, "appid": "wx93eea96ecc33f168"}</t>
         </is>
       </c>
       <c r="H16" s="11" t="inlineStr">
@@ -4902,13 +4912,13 @@
         </is>
       </c>
       <c r="I16" s="11" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" ht="15.75" customHeight="1" s="1">
       <c r="A17" s="7" t="inlineStr">
         <is>
-          <t>可币+微信</t>
+          <t>消费券+微信</t>
         </is>
       </c>
       <c r="B17" s="4" t="inlineStr">
@@ -4921,14 +4931,14 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D17" s="13" t="inlineStr">
-        <is>
-          <t>{"processToken": "WkH8JVrMwY7ZaZcJ8xJaSG", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "ltaOmRfUrxXyweqYC83iL2p4ASo9ZnPJ", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 2, "cocoinDeductAmount": 2, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "e5eecb0bc84b7af70fc59751868b7a08", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+      <c r="D17" s="0" t="inlineStr">
+        <is>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "UOn7teAZKgJGwIF1Nr5CBV9WLy8mxsMv", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 5, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "bf5ad984a92cfe706b71cee0e6995c20", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"318057d409be48068967196667914b3a\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211535756856c06fbfc17bec2f050000\",\"sign\":\"5600C2EA4B3CC751213902E672E31A6D\",\"timestamp\":\"1625577335\"}", "payRequestId": "KB20210706211535208677696903861t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"ca6997809c1a4421b80280e518c00372\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145352694464cea7f1dd1a16753b0000\",\"sign\":\"296267CB77285DD2C0DFEA3CA7B99FCC\",\"timestamp\":\"1625640832\"}", "payRequestId": "KB20210707145352208677696904628t"}, "success": true}</t>
         </is>
       </c>
       <c r="F17" s="10" t="n">
@@ -4936,7 +4946,7 @@
       </c>
       <c r="G17" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "appid": "wx93eea96ecc33f168"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H17" s="11" t="inlineStr">
@@ -4951,7 +4961,7 @@
     <row r="18" ht="15.75" customHeight="1" s="1">
       <c r="A18" s="7" t="inlineStr">
         <is>
-          <t>消费券+微信</t>
+          <t>抵扣券+支付宝</t>
         </is>
       </c>
       <c r="B18" s="4" t="inlineStr">
@@ -4964,14 +4974,14 @@
           <t>+</t>
         </is>
       </c>
-      <c r="D18" s="0" t="inlineStr">
-        <is>
-          <t>{"processToken": "Ef38eiaBwLPq4kuhGtZv97", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "YKfnEDsvdCF2bzSgT1Lhm30HOai7uZ69", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 5, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "a891979ff555cb62596c20d8df42459f", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+      <c r="D18" s="13" t="inlineStr">
+        <is>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "gJ3zjKvxN5MrZInXskmT9hWalO6qVFPL", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935519", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "8eb7f432847f79c9e2992116e13dc59b", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"de9eadb2e8564c02b2e49c963f6621ab\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211536166251890a465b80e93d260000\",\"sign\":\"F650C2F058B745EA56A58EED85481CEA\",\"timestamp\":\"1625577336\"}", "payRequestId": "KB20210706211535208677696930522t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145352208677696910178t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22Ct5h%252BrRKkdMW4XztfuY%252BUAEvpN7TdBYXxyF%252BsBc5WIMcXQLKx6ZI7dL71U2KE84KdSZZQpZLPL%252BUsVMbUXDvb8ZNhyn96lfPeA1%252BnYHuI9GjzaPIzAOiCv0bYb2BuXXFfiGC0vj3bi0UfG7P7QnlsStIFtW0sASFF5lV0BOGKbk%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145352208677696910178t\"}", "payRequestId": "KB20210707145352208677696910178t"}, "success": true}</t>
         </is>
       </c>
       <c r="F18" s="10" t="n">
@@ -4988,33 +4998,33 @@
         </is>
       </c>
       <c r="I18" s="11" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1" s="1">
       <c r="A19" s="7" t="inlineStr">
         <is>
-          <t>抵扣券+支付宝</t>
+          <t>抵扣券+支付宝，未达到条件金额</t>
         </is>
       </c>
       <c r="B19" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C19" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D19" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "3iJEmS84epThwsbv9E1hZw", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "Sfk1inxyU6NIGzOFCbPLeYsHTural3Qm", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935549", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "9e243a5ed635a5c7e2b3406bc75b80aa", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "0QfhZ1E4CW5lUmdTHAD2e9JjYvXVtOxI", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935519", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "61d8cc0645e462eeafc5f8dd9da3aa0f", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210706211536208677696947833t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22RcyonKKCn5n%252BAV7L5gBsJq7dr0%252BNf23IrIPOGO3fdDafRWXI%252BZ%252BSNpoCcuNzJX2seJCygykWoAOdGa7Z3BN5XDNNVVfD6PEeBP9IqzON%252BGnfryvT93K0N2qVc5%252FifzmaGagopCzDhwsskvysiFe1XPxtUynfvZDR8bUJmCE5PSA%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210706211536208677696947833t\"}", "payRequestId": "KB20210706211536208677696947833t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
         </is>
       </c>
       <c r="F19" s="10" t="n">
@@ -5022,7 +5032,7 @@
       </c>
       <c r="G19" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
         </is>
       </c>
       <c r="H19" s="11" t="inlineStr">
@@ -5031,33 +5041,33 @@
         </is>
       </c>
       <c r="I19" s="11" t="n">
-        <v>101</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20" ht="15.75" customHeight="1" s="1">
       <c r="A20" s="7" t="inlineStr">
         <is>
-          <t>抵扣券+支付宝，未达到条件金额</t>
+          <t>折扣券+微信</t>
         </is>
       </c>
       <c r="B20" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C20" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "UxjgdSo2sRfazutNyEv5qE", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "fIBWa2dDHCJ1wsmkRp3X9luQg4N6ZYjS", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935519", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "99e33f200ea4a0781c8b16ea9f244939", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "B9EZVDMYeEWaFAHuyu7gzg", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "qFkx1woWSn7jhftAKaTpvcO6Eb0d5XCL", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "20d700b919204e334fdd67ad61851131", "timestamp": "1625640747576", "nonce": "AUjqM0EK", "country": "CN"}</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"37961f37fa49427abbf869c8b309281a\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145234521433b4dc43aa4210e9170000\",\"sign\":\"9DB109A6041484729D19DF6CE8C09D96\",\"timestamp\":\"1625640754\"}", "payRequestId": "KB20210707145234208677696901665t"}, "success": true}</t>
         </is>
       </c>
       <c r="F20" s="10" t="n">
@@ -5065,7 +5075,7 @@
       </c>
       <c r="G20" s="11" t="inlineStr">
         <is>
-          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H20" s="11" t="inlineStr">
@@ -5074,33 +5084,33 @@
         </is>
       </c>
       <c r="I20" s="11" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="21" ht="15.75" customHeight="1" s="1">
       <c r="A21" s="7" t="inlineStr">
         <is>
-          <t>折扣券+微信</t>
+          <t>折扣券+微信，未达到条件金额</t>
         </is>
       </c>
       <c r="B21" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C21" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D21" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "146F2KETm8HWxoUA5F3b8X", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "BTQzv3UYjOGcoRlkJI7nbxZq8sE4wmgr", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "9ecee89aee3993a501eadc43794e5bad", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "B9EZVDMYeEWaFAHuyu7gzg", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "Pvyogi4bhjWEf2FxU7HsYmMLR0qKn6De", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 9, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "d065f516be615579ab95da38b7bae6cc", "timestamp": "1625640747576", "nonce": "AUjqM0EK", "country": "CN"}</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"679b3c802a5e4540959b92119d524a63\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx062115366900959fc845a5dc925fd50000\",\"sign\":\"5E3629AF56D440E67136DBF74FDF1012\",\"timestamp\":\"1625577336\"}", "payRequestId": "KB20210706211536208677696926731t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
         </is>
       </c>
       <c r="F21" s="10" t="n">
@@ -5108,7 +5118,7 @@
       </c>
       <c r="G21" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
         </is>
       </c>
       <c r="H21" s="11" t="inlineStr">
@@ -5117,33 +5127,33 @@
         </is>
       </c>
       <c r="I21" s="11" t="n">
-        <v>101</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" ht="15.75" customHeight="1" s="1">
       <c r="A22" s="7" t="inlineStr">
         <is>
-          <t>折扣券+微信，未达到条件金额</t>
+          <t>消费折扣券+支付宝</t>
         </is>
       </c>
       <c r="B22" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C22" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "bLRcEeJpEcJKUF9Vyngbt", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "HsS8aoIhCNLfykMZ6JU9bvPQxdTm1cB5", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935550", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 9, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "e4a998d199d6f1ab4e15cf4796bae24b", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "Fro9c846vdYIQuyhw5j7k0WpSKbHgNOn", "amount": 100, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 100, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935562", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "77107dd357454f608bc8db2da7b03599", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E22" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145353208677696984131t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.01%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22pe98gfLq%252FB29WAgbuNvi%252FeFohbzvVjqoxzpRM12spjqNcTnN1sj174jidxSP%252BAD0VoAoMY9zaeqMOkUnDg0JVsZ8TAM5O1lwHm3NqcFd7T%252BWgyqm61BttKnGkv7Az6KkGGF0Xru2b8asugmPPL22p0stbvAfV73%252BwQ%252FE7CbS61E%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145353208677696984131t\"}", "payRequestId": "KB20210707145353208677696984131t"}, "success": true}</t>
         </is>
       </c>
       <c r="F22" s="10" t="n">
@@ -5151,7 +5161,7 @@
       </c>
       <c r="G22" s="11" t="inlineStr">
         <is>
-          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H22" s="11" t="inlineStr">
@@ -5160,33 +5170,33 @@
         </is>
       </c>
       <c r="I22" s="11" t="n">
-        <v>10</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1" s="1">
       <c r="A23" s="7" t="inlineStr">
         <is>
-          <t>消费折扣券+支付宝</t>
+          <t>消费折扣券+支付宝，未达到条件金额</t>
         </is>
       </c>
       <c r="B23" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C23" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "LjHnC2PbeyDj4FLpk67bdp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "YsOxSMByNUw6WDJkPpc0LEHGh7vdVo2R", "amount": 100, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 100, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935542", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "f769392c4216f6e6246cf113cb413ea0", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "caY5KdESZb4gF6t9HQOxyP0rlhW8NJTn", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935493", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 9, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "7b08498c64ef16f797c4ea9be4c27506", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210706211536208677696934054t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.01%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22F%252BUEgfNx2p0oENwZvWgKeNoN%252F6G2k7T%252FPwll5dDKWm%252BSRHvycFd7gNEiuGM1wem%252F2ioOKQ00LzdLtSQ8OG8eM0LkNG3iovnwUZr0nqJWnRsOST7XPw8EqqwUQh%252FOP7lMY8hxTs0Lcn2cPvlciXZcoZMwAbjLS4313CynGHrXQ6M%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210706211536208677696934054t\"}", "payRequestId": "KB20210706211536208677696934054t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
         </is>
       </c>
       <c r="F23" s="10" t="n">
@@ -5194,7 +5204,7 @@
       </c>
       <c r="G23" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
         </is>
       </c>
       <c r="H23" s="11" t="inlineStr">
@@ -5203,33 +5213,33 @@
         </is>
       </c>
       <c r="I23" s="11" t="n">
-        <v>100</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" ht="15.75" customHeight="1" s="1">
       <c r="A24" s="7" t="inlineStr">
         <is>
-          <t>消费折扣券+支付宝，未达到条件金额</t>
+          <t>红包券+微信</t>
         </is>
       </c>
       <c r="B24" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C24" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D24" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "U7jFf1G2qaXGHJxv7PEhZ1", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "mSGJjUuD27cpABEfNH6nwykKi1dI9gzx", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935521", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 9, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "7d4a20d26855822dfdd5aa105c52ca8a", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "gohkQiRJrXb60wls4TaAEtM1CNzDPHO9", "amount": 2000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 2000, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 0, "cocoinDeductAmount": 0, "voucherId": "100935522", "voucherCount": 1, "voucherType": "8", "voucherDeductAmount": 1000, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "4d19cefc50ef705da0038b7e5cab7f16", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"4e1f242c7e5a4c2d87f1817a3ac7617c\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0714535415471083ae9ec1b7cbe8140000\",\"sign\":\"706A5DEEC2E16DA0FD6DEC4183366EA3\",\"timestamp\":\"1625640834\"}", "payRequestId": "KB20210707145353208677696962557t"}, "success": true}</t>
         </is>
       </c>
       <c r="F24" s="10" t="n">
@@ -5237,7 +5247,7 @@
       </c>
       <c r="G24" s="11" t="inlineStr">
         <is>
-          <t>{"success": false, "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H24" s="11" t="inlineStr">
@@ -5246,13 +5256,13 @@
         </is>
       </c>
       <c r="I24" s="11" t="n">
-        <v>10</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="25" ht="15.75" customHeight="1" s="1">
       <c r="A25" s="7" t="inlineStr">
         <is>
-          <t>红包券+微信</t>
+          <t>可币+消费券(单张)+微信</t>
         </is>
       </c>
       <c r="B25" s="4" t="inlineStr">
@@ -5267,12 +5277,12 @@
       </c>
       <c r="D25" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "Py7r8RgoyXZgJ6o1Zyg9Nu", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "mxdE1VU6rbWBsQ35A7DNKC8pkc2aIuzl", "amount": 2000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 2000, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 0, "cocoinDeductAmount": 0, "voucherId": "100935552", "voucherCount": 1, "voucherType": "8", "voucherDeductAmount": 1000, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "1ab3c05c774e5d0be531bfcce49c9843", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "fqSmJyGD4Nz37VI1xlLHjPRXedptYMOE", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "71839aa10a41add3ed5db64abe802a99", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E25" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"4573b91866494d4b8aa80a0acc8077a2\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx062115371918181a460bf28588e7130000\",\"sign\":\"D5E821F8797785A4846CD98334FE6C45\",\"timestamp\":\"1625577337\"}", "payRequestId": "KB20210706211536208677696918374t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"d2201d126a0543afa7d2a94ecb6cf0df\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0714535464310221a33790ac606d670000\",\"sign\":\"3CF52C0B5EC1914076FA26385FA752BC\",\"timestamp\":\"1625640834\"}", "payRequestId": "KB20210707145354208677696974665t"}, "success": true}</t>
         </is>
       </c>
       <c r="F25" s="10" t="n">
@@ -5289,18 +5299,18 @@
         </is>
       </c>
       <c r="I25" s="11" t="n">
-        <v>2000</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" ht="15.75" customHeight="1" s="1">
       <c r="A26" s="7" t="inlineStr">
         <is>
-          <t>可币+消费券(单张)+微信</t>
+          <t>可币+消费券(单张)+微信，券扣减金额大于券面额</t>
         </is>
       </c>
       <c r="B26" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C26" s="8" t="inlineStr">
@@ -5310,12 +5320,12 @@
       </c>
       <c r="D26" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "PACxG51WiJSNnM7U3Usw7g", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "fGm6uLN91riVDwg7cUvHTO5KRb2ZCW0I", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "0e1d6e2b1138e6ad240116705b148c5d", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "CLmdGqBipeDt9vHZK8Y746S2wVu3x50O", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "08634792a53d27acdead8c2e89ad3e13", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E26" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"3ad9fa099ce84eb69c03f0b4b06a55b1\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211537593932dcc18082243f34cb0000\",\"sign\":\"685AE1BA108297933F802A6E7E43064A\",\"timestamp\":\"1625577337\"}", "payRequestId": "KB20210706211537208677696968722t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"c900ba11eea449259eaebd909f682928\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145355261214649b79a91b8802810000\",\"sign\":\"44B8CD7D3A8FF3AB82EB24005E4DF1B3\",\"timestamp\":\"1625640835\"}", "payRequestId": "KB20210707145355208677696987176t"}, "success": true}</t>
         </is>
       </c>
       <c r="F26" s="10" t="n">
@@ -5331,19 +5341,21 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I26" s="11" t="n">
-        <v>10</v>
+      <c r="I26" s="11" t="inlineStr">
+        <is>
+          <t>10，券扣减金额字段会被服务端干掉</t>
+        </is>
       </c>
     </row>
     <row r="27" ht="15.75" customHeight="1" s="1">
       <c r="A27" s="7" t="inlineStr">
         <is>
-          <t>可币+消费券(单张)+微信，券扣减金额大于券面额</t>
+          <t>可币+消费券(多张)+微信</t>
         </is>
       </c>
       <c r="B27" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C27" s="8" t="inlineStr">
@@ -5353,12 +5365,12 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "WGvWFZZZWz2LK5jAMCTGJ6", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "7Shr8THtcxZMn6kXF9CYafEUlgs0Kuvo", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "4681e7e24b4dc75389e4d2970dffedba", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "UBjZHDn9t1O2uP8rXwfGJeyiWdIK6com", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 5, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "16a6e156dd2146aea8e51bf696e1f0dd", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"11b3e3ecd71b4cc5bbd81fc6ab9334c9\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0621153800922369755faee96f0b790000\",\"sign\":\"1C9FDA07DCD8A10C686633E8254A92AF\",\"timestamp\":\"1625577338\"}", "payRequestId": "KB20210706211537208677696963876t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"2e15f14cbbe9480d8946c335f3ff7c49\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145355741984770f6a88619b6a150000\",\"sign\":\"55F0A5AEA43C103D790CB1F2AAFEAD70\",\"timestamp\":\"1625640835\"}", "payRequestId": "KB20210707145355208677696982066t"}, "success": true}</t>
         </is>
       </c>
       <c r="F27" s="10" t="n">
@@ -5374,16 +5386,14 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I27" s="11" t="inlineStr">
-        <is>
-          <t>10，券扣减金额字段会被服务端干掉</t>
-        </is>
+      <c r="I27" s="11" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="28" ht="15.75" customHeight="1" s="1">
       <c r="A28" s="7" t="inlineStr">
         <is>
-          <t>可币+消费券(多张)+微信</t>
+          <t>可币+抵扣券+支付宝</t>
         </is>
       </c>
       <c r="B28" s="4" t="inlineStr">
@@ -5398,12 +5408,12 @@
       </c>
       <c r="D28" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "Q6Sh3TyjRXbU6ziXE6nSgj", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "YJzuAKl5sj3npfceBih7Fq0dHWMPV2mO", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "0", "voucherCount": 5, "voucherType": "1", "voucherDeductAmount": 2, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "d02be9ff382fc2037d1bfea864eeb4d9", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "3Y0tTvW4iO29qkQAKlCcZexM1IrbhSzm", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935560", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "314ab022df90d97658387132998622f7", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"593bc5d5381f436d89ac07cfae974a12\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211538384047cf7d6e3202158bb70000\",\"sign\":\"E487958CA3B0C15B9194FE4E8D720D7C\",\"timestamp\":\"1625577338\"}", "payRequestId": "KB20210706211538208677696930534t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145357208677696923218t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22CtB4%252FQvo6SYovDbUPF8LSOIF4rPamFswPfdcj2FAc9T%252BGB97HzBM%252BmTuspUjSpqV5rAoupVvIodceudlCr%252FnXFghqh9zOB6XQZQwWCkhICXHqnMzulWaY3FwynAxDMMlLh2tRMMjYmZoCUFXe9JEsZxmLK1g8bAEav9HarGRpIU%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145357208677696923218t\"}", "payRequestId": "KB20210707145357208677696923218t"}, "success": true}</t>
         </is>
       </c>
       <c r="F28" s="10" t="n">
@@ -5420,33 +5430,33 @@
         </is>
       </c>
       <c r="I28" s="11" t="n">
-        <v>10</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1" s="1">
       <c r="A29" s="7" t="inlineStr">
         <is>
-          <t>可币+抵扣券+支付宝</t>
+          <t>可币+抵扣券+微信，支付金额不能为负数</t>
         </is>
       </c>
       <c r="B29" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C29" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "3VWEn5heVPvUmLfeEsPwM5", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "DtSK6LICcJxhTF8Y3a9zM72fleopkwHj", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935549", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "9ce1c14e9bf970140918499d9f2f81c8", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "sKLlzS5pQgT83jtEhe9vdmMXiPOrq0HZ", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935519", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 10, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "3fe0edbd05d5e309ab582fdf3924af3f", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210706211538208677696948603t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22SLNtQvjRzienBJbyhJ%252BTrMDDiNy%252B4ZceTTxYDgzgvhYeQZOZBz4rtW7n8cXkRn0Z9%252FAU83sMDFyGxmfDkAC9ywt4g26%252BaM%252FIj95UFMFIdmRrY3orrvEwSi2ctRiL2f8q6jLiGgwb0anYQCJ6Qb5RDQt%252Bu%252B81Dyt9KcwMnKjxsfo%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210706211538208677696948603t\"}", "payRequestId": "KB20210706211538208677696948603t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}, "success": false}</t>
         </is>
       </c>
       <c r="F29" s="10" t="n">
@@ -5454,7 +5464,7 @@
       </c>
       <c r="G29" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": false}</t>
         </is>
       </c>
       <c r="H29" s="11" t="inlineStr">
@@ -5462,34 +5472,36 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I29" s="11" t="n">
-        <v>101</v>
+      <c r="I29" s="11" t="inlineStr">
+        <is>
+          <t>10，10-10-1=-1</t>
+        </is>
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1" s="1">
       <c r="A30" s="7" t="inlineStr">
         <is>
-          <t>可币+抵扣券+微信，支付金额不能为负数</t>
+          <t>可币+折扣券+支付宝</t>
         </is>
       </c>
       <c r="B30" s="4" t="inlineStr">
         <is>
-          <t>full</t>
+          <t>smoke</t>
         </is>
       </c>
       <c r="C30" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D30" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "2wUMpNWaNEmVmHtDGSLLBD", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "zBMC8x6jyb7lrs4FZdL9cGHKJaPpXVvS", "amount": 10, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 10, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935519", "voucherCount": 1, "voucherType": "2", "voucherDeductAmount": 10, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "2a2f10ac280747eed4b49af07fd840d3", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "B9EZVDMYeEWaFAHuyu7gzg", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "AJyXKgwPnVNZHF8DzvY3S46LihcCejGk", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "22c1d77681716249f4c647d2e3510800", "timestamp": "1625640747576", "nonce": "AUjqM0EK", "country": "CN"}</t>
         </is>
       </c>
       <c r="E30" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "鐩村啿涓嶈兘鏈変紭鎯犲埜鍜屽彲甯侀噾棰�"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145237208677696952533t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22s92Gf3T0TvqNubOLc5ZtC3S5RhLlGUZYS0KjyDqzIJtX4bsYiZGjFK1J8omDUpnPCH0Kj7l20KyaRNgNWBLMuSYwFz%252F%252FFAVYub2J84MG2Due6LQfjIFJb7lcRUrvFatpb9WjSlcNuPSPxDAAqPmONuuhz%252BAoOZJLOTpxOeCPlB4%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145237208677696952533t\"}", "payRequestId": "KB20210707145237208677696952533t"}, "success": true}</t>
         </is>
       </c>
       <c r="F30" s="10" t="n">
@@ -5497,7 +5509,7 @@
       </c>
       <c r="G30" s="11" t="inlineStr">
         <is>
-          <t>{"success": false}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H30" s="11" t="inlineStr">
@@ -5505,16 +5517,14 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I30" s="11" t="inlineStr">
-        <is>
-          <t>10，10-10-1=-1</t>
-        </is>
+      <c r="I30" s="11" t="n">
+        <v>101</v>
       </c>
     </row>
     <row r="31" ht="15.75" customHeight="1" s="1">
       <c r="A31" s="7" t="inlineStr">
         <is>
-          <t>可币+折扣券+支付宝</t>
+          <t>可币+消费折扣券+微信</t>
         </is>
       </c>
       <c r="B31" s="4" t="inlineStr">
@@ -5529,12 +5539,12 @@
       </c>
       <c r="D31" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "qMDEihNgGRPLgFuovDbuw", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "uryV0W8aKBzgGdSERpfi6v25CI7TPQjF", "amount": 101, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 101, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935507", "voucherCount": 1, "voucherType": "3", "voucherDeductAmount": 99, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "3870b1e57f4b3205dce416fadfe8194b", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "lez3ABDxKqLwOGMU0T1nZ6PHjigvNEFI", "amount": 1000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1000, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "100935493", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 990, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "9d863751e347c46e8b68ed2ad57e8b7c", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210706211538208677696983242t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%220.02%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22HSDMP5OheGGYCB8ruNQM3QLR%252Bs9UeE7AuDsKwKPf%252Fmo6UNdk0Z3b71yjrMMUE6XpNndjia9FhB%252FqYpet6Zdq8jqmqK%252BPkiQOZfqGH2KBQHzS5C66k4SkFPVBDMPh98T1ZIVnqCn1ZyjuNN9RDgs4taJtbGYVoWY%252F1cNzavMn%252FU8%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210706211538208677696983242t\"}", "payRequestId": "KB20210706211538208677696983242t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"6a26f606e7b640fa89a024cea64b23a3\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145358209303a8bef135aa7b861a0000\",\"sign\":\"1B4543D4AFE706137F5F39F601B58CF3\",\"timestamp\":\"1625640838\"}", "payRequestId": "KB20210707145357208677696925474t"}, "success": true}</t>
         </is>
       </c>
       <c r="F31" s="10" t="n">
@@ -5551,13 +5561,13 @@
         </is>
       </c>
       <c r="I31" s="11" t="n">
-        <v>101</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="32" ht="15.75" customHeight="1" s="1">
       <c r="A32" s="7" t="inlineStr">
         <is>
-          <t>可币+消费折扣券+微信</t>
+          <t>可币+红包券+支付宝</t>
         </is>
       </c>
       <c r="B32" s="4" t="inlineStr">
@@ -5572,12 +5582,12 @@
       </c>
       <c r="D32" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "VKUC3WijRphffxy1EGmGUX", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "AxnJ1CNdBhvOcQXjsHRkIE5og23uWLpG", "amount": 1000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1000, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 4, "cocoinDeductAmount": 4, "voucherId": "100935542", "voucherCount": 1, "voucherType": "4", "voucherDeductAmount": 990, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "814fd31d72041084c65874c72f56d555", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "dlyR6h21n59bIDEPJUBAGuTswM3H7X0S", "amount": 2000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 2000, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935509", "voucherCount": 1, "voucherType": "8", "voucherDeductAmount": 1000, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "a593a1a4c32d44d634c2b37d8d0e9b2e", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E32" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"054a0f84f63d45fca6f5d71a156b8708\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx062115390626526dacd7501a821aac0000\",\"sign\":\"B5010F7EE5D14A98CFF88C454570BA95\",\"timestamp\":\"1625577339\"}", "payRequestId": "KB20210706211538208677696970880t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"9f1736ed24d14db28663dc35ccba98f0\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145358642364cc944a30cb1768df0000\",\"sign\":\"7D35819D673A46032F46BBDB7BBDD234\",\"timestamp\":\"1625640838\"}", "payRequestId": "KB20210707145358208677696930417t"}, "success": true}</t>
         </is>
       </c>
       <c r="F32" s="10" t="n">
@@ -5594,13 +5604,13 @@
         </is>
       </c>
       <c r="I32" s="11" t="n">
-        <v>1000</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="33" ht="15.75" customHeight="1" s="1">
       <c r="A33" s="7" t="inlineStr">
         <is>
-          <t>可币+红包券+支付宝</t>
+          <t>纯充值-微信</t>
         </is>
       </c>
       <c r="B33" s="4" t="inlineStr">
@@ -5615,12 +5625,12 @@
       </c>
       <c r="D33" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "MSkTAaYJrgDymyFtqRLqhH", "payType": "wxpay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "YEGRd5NT6oCMxuU7Zs4ceJSw8PBVzt0g", "amount": 2000, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 2000, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "100935522", "voucherCount": 1, "voucherType": "8", "voucherDeductAmount": 1000, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "b95e7c81959cf59cdf2a7baa57d31cb2", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "9cf27658c997874228a50650895c6055", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E33" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"ec456abc46db4134be6146741e59e164\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0621153950728835f835cfbffeae830000\",\"sign\":\"28B504CAF6093975336005AD40543BD9\",\"timestamp\":\"1625577339\"}", "payRequestId": "KB20210706211539208677696932041t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"8c89c871fcb14b7b96204f1bf4b5f0e0\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx071453590065865111d62bec3e84e70000\",\"sign\":\"A98F5CB55C77F16C7DE351122108646C\",\"timestamp\":\"1625640839\"}", "payRequestId": "KB20210707145358208677696956536t"}, "success": true}</t>
         </is>
       </c>
       <c r="F33" s="10" t="n">
@@ -5628,7 +5638,7 @@
       </c>
       <c r="G33" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "KB20"}</t>
+          <t>{"success": true, "payRequestId": "RM20"}</t>
         </is>
       </c>
       <c r="H33" s="11" t="inlineStr">
@@ -5637,13 +5647,13 @@
         </is>
       </c>
       <c r="I33" s="11" t="n">
-        <v>2000</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" ht="15.75" customHeight="1" s="1">
       <c r="A34" s="7" t="inlineStr">
         <is>
-          <t>纯充值-微信</t>
+          <t>纯充值-支付宝</t>
         </is>
       </c>
       <c r="B34" s="4" t="inlineStr">
@@ -5658,12 +5668,12 @@
       </c>
       <c r="D34" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "DJ9Y8TZ7uVaTVBm2XoxQvF", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "999b4e2147e613b66e4ba046b7df52ed", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 999999999, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 999999999, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "58033fc2dcecfb06abb06b65701823d9", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E34" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"b7420f45d22e4ace9231e4b0f0d0e5cf\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx0621153983377663552a650cc108b30000\",\"sign\":\"CE5B7CAA39DEDBF4CD99B20058613711\",\"timestamp\":\"1625577339\"}", "payRequestId": "KB20210706211539208677696936718t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145359208677696944384t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%229999999.99%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22SGYw5KMCoK1SYtyiqIV7%252FXINl1duuHqt3xvgBgL3Fz2Mjntzu%252BLDRYkKhJLwq2Bv9NM%252F3tLOF%252B6fJLqvSBqOJTecZ0BvCMo0EJq8Tyht9PWtpmYJXO1tEmrqc%252FRUUMdy0%252Fk5Jis84ZqWEl%252F4qgbFiG%252BwaYER7WLDsiJk%252B5ofchQ%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145359208677696944384t\"}", "payRequestId": "KB20210707145359208677696944384t"}, "success": true}</t>
         </is>
       </c>
       <c r="F34" s="10" t="n">
@@ -5680,33 +5690,33 @@
         </is>
       </c>
       <c r="I34" s="11" t="n">
-        <v>1</v>
+        <v>999999999</v>
       </c>
     </row>
     <row r="35" ht="15.75" customHeight="1" s="1">
       <c r="A35" s="7" t="inlineStr">
         <is>
-          <t>纯充值-支付宝</t>
+          <t>纯充值-微信，携带可币券</t>
         </is>
       </c>
       <c r="B35" s="4" t="inlineStr">
         <is>
-          <t>smoke</t>
+          <t>full</t>
         </is>
       </c>
       <c r="C35" s="8" t="inlineStr">
         <is>
-          <t>+</t>
+          <t>-</t>
         </is>
       </c>
       <c r="D35" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "DJ9Y8TZ7uVaTVBm2XoxQvF", "payType": "alipay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 999999999, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 999999999, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "appKey": "2033", "sign": "cae8ebdfb903cd5e0621c6d06706c71e", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "7d8bc71ea04fa23d23742a43e793c3f4", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E35" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210706211539208677696901702t%22%26subject%3D%22test%22%26body%3D%22test+pay%22%26total_fee%3D%229999999.99%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22OmvDzFhnXssyvViASiu9uU5s53hoky5%252F%252BMVwZZACzNtyW7vHqjVPZCZUOIOAYq4k9yHKjfjFl6m4dfOHOEGp%252B65upHU%252F7Lg2qIyW17N%252B3wZy7qR5omllxqC8bYQqwk4x%252FgEyTECTJ8PqW%252F%252BQk9VDAJlOo57Ef0z8%252B35ANsqV2B0%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210706211539208677696901702t\"}", "payRequestId": "KB20210706211539208677696901702t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
         </is>
       </c>
       <c r="F35" s="10" t="n">
@@ -5714,7 +5724,7 @@
       </c>
       <c r="G35" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "RM20"}</t>
+          <t>{"success": false}</t>
         </is>
       </c>
       <c r="H35" s="11" t="inlineStr">
@@ -5723,13 +5733,13 @@
         </is>
       </c>
       <c r="I35" s="11" t="n">
-        <v>999999999</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" ht="15.75" customHeight="1" s="1">
       <c r="A36" s="7" t="inlineStr">
         <is>
-          <t>纯充值-微信，携带可币券</t>
+          <t>纯充值-支付宝，携带可币</t>
         </is>
       </c>
       <c r="B36" s="4" t="inlineStr">
@@ -5744,12 +5754,12 @@
       </c>
       <c r="D36" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "DJ9Y8TZ7uVaTVBm2XoxQvF", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "FULL", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.oppo.usercenter", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "0", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "f1724c3212012972f11ed81a6563c219", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "c772925bac153f403852c2a239f0e284", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E36" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"0cde86ce86a44f0c87abcc0bd96557d6\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx07145400972913a166a4e7695685400000\",\"sign\":\"911B6E916478E8F715E83211831B25AB\",\"timestamp\":\"1625640841\"}", "payRequestId": "KB20210707145400208677696936838t"}, "success": true}</t>
         </is>
       </c>
       <c r="F36" s="10" t="n">
@@ -5772,7 +5782,7 @@
     <row r="37" ht="15.75" customHeight="1" s="1">
       <c r="A37" s="7" t="inlineStr">
         <is>
-          <t>纯充值-支付宝，携带可币</t>
+          <t>纯充值-支付宝，currencySystem=COCOIN_ALLOWED</t>
         </is>
       </c>
       <c r="B37" s="4" t="inlineStr">
@@ -5787,12 +5797,12 @@
       </c>
       <c r="D37" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "DJ9Y8TZ7uVaTVBm2XoxQvF", "payType": "wxpay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "CASH", "virtualAssets": {"cocoinCount": 1, "cocoinDeductAmount": 1, "voucherId": "", "voucherCount": "", "voucherType": 0, "voucherDeductAmount": 0, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "5c17c21b4a91721db3800da6dbf87025", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935123", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "393c13d959730e2dd5600a99e184f35d", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E37" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"6be48af89a214386b76eacccaa975eef\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1559247341\",\"prepayid\":\"wx06211541302858c1a289b62d2d93ba0000\",\"sign\":\"34808CA618263054ADB989121692A635\",\"timestamp\":\"1625577341\"}", "payRequestId": "KB20210706211541208677696920676t"}, "success": true}</t>
+          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
         </is>
       </c>
       <c r="F37" s="10" t="n">
@@ -5815,7 +5825,7 @@
     <row r="38" ht="15.75" customHeight="1" s="1">
       <c r="A38" s="7" t="inlineStr">
         <is>
-          <t>纯充值-支付宝，currencySystem=COCOIN_ALLOWED</t>
+          <t>直扣-支付宝，currencySystem=COCOIN_ALLOWED，无可币</t>
         </is>
       </c>
       <c r="B38" s="4" t="inlineStr">
@@ -5825,17 +5835,17 @@
       </c>
       <c r="C38" s="8" t="inlineStr">
         <is>
-          <t>-</t>
+          <t>+</t>
         </is>
       </c>
       <c r="D38" s="13" t="inlineStr">
         <is>
-          <t>{"processToken": "DJ9Y8TZ7uVaTVBm2XoxQvF", "payType": "alipay", "goodsType": "COCOIN", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "", "amount": 1, "productName": "test", "productDesc": "test pay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "HALF", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "virtualAssets": {"cocoinCount": "", "cocoinDeductAmount": 0, "voucherId": "100935123", "voucherCount": 1, "voucherType": "1", "voucherDeductAmount": 1, "virtualVoucher": "", "creditCount": 0, "creditDeductAmount": 0}, "appKey": "2033", "sign": "1963cdba33d9a466b77d805283224a12", "timestamp": "1625577285745", "nonce": "cnEeiq0O", "country": "CN"}</t>
+          <t>{"processToken": "V4GGAWpDZQdRLxBogAk2Bp", "payType": "alipay", "goodsType": "COMMON", "platform": "ATLAS", "partnerCode": "2031", "partnerOrder": "r170G3Ajnakxb5EUzoFhmIBLQKlC9gwT", "amount": 1, "productName": "test", "productDesc": "test paydirect pay-alipay", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "clientCallbackUrl": "", "price": 1, "count": 1, "screenInfo": "ACROSS", "currencyCode": "CNY", "currencyName": "", "source": "", "appPackage": "com.example.pay_demo", "appVersion": "", "appId": "", "partnerSign": "", "channelId": "", "factor": "", "discountCode": "", "acqAddnData": "", "attach": "", "ext": "", "token": "", "currencySystem": "COCOIN_ALLOWED", "appKey": "2033", "sign": "dea4a83028dfbe1f24eacbae7eee4fb8", "timestamp": "1625640824336", "nonce": "W1cROCSA", "country": "CN"}</t>
         </is>
       </c>
       <c r="E38" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "浣跨敤浼樻儬鍒告椂, 浼樻儬閲戦涓嶈兘涓�0"}, "success": false}</t>
+          <t>{"data": {"channelData": "{\"payType\":\"AlipayPlugin\",\"mes\":\"partner%3D%222088311951685799%22%26seller_id%3D%22kekezhifu%40keke.cn%22%26out_trade_no%3D%22KB20210707145359208677696921456t%22%26subject%3D%22test%22%26body%3D%22test+paydirect+pay-alipay%22%26total_fee%3D%220.01%22%26notify_url%3D%22http%3A%2F%2Fopaycenter-secure-test3.wanyol.com%2Fopaycenter%2Fnotifypluginreader%22%26service%3D%22mobile.securitypay.pay%22%26payment_type%3D%221%22%26_input_charset%3D%22utf-8%22%26it_b_pay%3D%2230m%22%26sign%3D%22UnqnD3AXex7QeZsBZaZNfZh51nfrdGAteFPFFyyLidEbHabrci4X6J85jEdjeMCSDcVBl59LBYqWIJ%252FNXRFw5ITLWB%252BxDItd4wQY6lEXxyef9XxYnD0t3SvOgvUMDwVvFM%252FeAzTaXu05arz31%252BX1hqNZQzuzJl1YhzuyXcz4kIw%253D%22%26sign_type%3D%22RSA%22\",\"system_order\":\"KB20210707145359208677696921456t\"}", "payRequestId": "KB20210707145359208677696921456t"}, "success": true}</t>
         </is>
       </c>
       <c r="F38" s="10" t="n">
@@ -5843,7 +5853,7 @@
       </c>
       <c r="G38" s="11" t="inlineStr">
         <is>
-          <t>{"success": false}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H38" s="11" t="inlineStr">
@@ -5851,8 +5861,10 @@
           <t>passed</t>
         </is>
       </c>
-      <c r="I38" s="11" t="n">
-        <v>1</v>
+      <c r="I38" s="11" t="inlineStr">
+        <is>
+          <t>1，标志是否允许用可币，将扣除可币余额</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
refactor testcase pay and signpay
</commit_message>
<xml_diff>
--- a/case/src/http/inland.xlsx
+++ b/case/src/http/inland.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28080" windowHeight="13065" tabRatio="913" firstSheet="2" activeTab="13" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="28080" windowHeight="13065" tabRatio="913" firstSheet="2" activeTab="14" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="simplepay_recharge_spend" sheetId="1" state="visible" r:id="rId1"/>
@@ -123,15 +123,37 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <u val="single"/>
       <scheme val="minor"/>
     </font>
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FFFF0000"/>
+      <b val="1"/>
+      <color rgb="FFFFFFFF"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF9C0006"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF3F3F76"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -145,7 +167,47 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF800080"/>
+      <sz val="11"/>
+      <u val="single"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="18"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <b val="1"/>
+      <color theme="3"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <b val="1"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -160,7 +222,7 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -168,75 +230,7 @@
       <name val="宋体"/>
       <charset val="0"/>
       <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -251,8 +245,7 @@
     <font>
       <name val="宋体"/>
       <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF9C6500"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -261,6 +254,13 @@
       <charset val="0"/>
       <b val="1"/>
       <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <color rgb="FF006100"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -286,7 +286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -298,19 +298,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -322,19 +310,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -352,31 +346,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -388,7 +364,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -406,13 +388,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -442,13 +442,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -495,6 +495,30 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -525,26 +549,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -575,15 +584,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -600,10 +600,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyAlignment="1">
@@ -612,133 +612,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="8" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="17" borderId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="2" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="8" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="7" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="7" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="11" borderId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="9" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="4" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="22" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="9" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="19" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="29" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="30" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="29" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -4357,8 +4357,8 @@
   </sheetPr>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -4903,7 +4903,7 @@
       </c>
       <c r="G16" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "appid": "wx93eea96ecc33f168"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H16" s="11" t="inlineStr">
@@ -5638,7 +5638,7 @@
       </c>
       <c r="G33" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "RM20"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H33" s="11" t="inlineStr">
@@ -5681,7 +5681,7 @@
       </c>
       <c r="G34" s="11" t="inlineStr">
         <is>
-          <t>{"success": true, "payRequestId": "RM20"}</t>
+          <t>{"success": true, "payRequestId": "KB20"}</t>
         </is>
       </c>
       <c r="H34" s="11" t="inlineStr">
@@ -5880,8 +5880,8 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6014,12 +6014,12 @@
       </c>
       <c r="D7" s="0" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "TB5LBVoZ8Z3HMnnVi3LV4R", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "114cfc8da30a99b473252c8e1dd3b461", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "dsz7iPu2mOlHBEh0GNRx31WA6JogS5MI", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "GojHtWALFU1iDiVycUGdc6", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "cddfe74d7eb4ebdcdff270a8dd1f3818", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "NsMJDUYy80BgZbkW9VCaihXfFQpxcmv7"}</t>
         </is>
       </c>
       <c r="E7" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"d113713eec8c4f878ffb0d3118c0a440\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1259634601\",\"prepayid\":\"wx17101504578033ffe26fdcad24a9960000\",\"sign\":\"72752199DE9B9C5D3B09376F9773F87B\",\"timestamp\":\"1623896104\"}", "payRequestId": "RM20210617095156208677696917142t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"7e8cfb1101d24d798e523da8b4e25474\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1259634601\",\"prepayid\":\"wx07203648489071b330b53c1903be500000\",\"sign\":\"3997AFAC5806C947B65D131317CF738E\",\"timestamp\":\"1625661408\"}", "payRequestId": "RM20210707203648208677696951771t"}, "success": true}</t>
         </is>
       </c>
       <c r="F7" s="10" t="n">
@@ -6057,12 +6057,12 @@
       </c>
       <c r="D8" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "N3wawcWCZS1NokvqibHXch", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "b345218d9712eb0ceff02b914d8998f5", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "7Qusy0AeiU68vSR4mcYbktEIo5nxHJBD", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "Gdnj3fQn5K4Cw9vBs3Z1zL", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "5f098e37fc23766938c8a65c9a94486d", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "Oo7LFnmZDrzVtG2bJK1EBkA4ciWpd8as"}</t>
         </is>
       </c>
       <c r="E8" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202106171015041381633876730528%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210617095156208677696951284t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DYjnEfwbaGIpat7zPEKYUQUwfKLJjPBhOAsQ6%252BopUMbZiwOc95wDViI0vqgna5KaUtAqctnSQwkq4T6k50FWoTxMXN8BRMateNcUP3EjNrT%252BTHLhIbv8VVr%252Ff5S7q0kHIXularN8UsqteJUqkRuV5uvehibfUYXzgKPDyX%252FYeBL05LiNqieD2Us2dG8LkUsdQw3AY7%252BfRbzGqmFl%252FbO8wrWP7xmQITubJCRckcwdAGvg7GIsY4Ajp2kenMJEhtqDgDi%252Bzu1ZdhsynYYR02Cu8SbJWh%252FlWru56AHGPHhWMfEqVEcmqA6%252BNb3urFTV4eY8uTjXOEgVWgxBgxaB%252BE%252BCckQ%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A04%26version%3D1.0", "payRequestId": "RM20210617095156208677696951284t"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202107072036481326274008126254%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210707203648208677696905325t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DpkEfFWoyaAKYvd4p1sywGduTuk0kX1tmTKVHUP1Qnb6D%252FuNxSF%252B3%252B9q3GZdEVef1%252BfEYAzZNlvyQbYMkAoUSMhW407tBAK3RPFAQtLU23BdDZLMAQRGt6S5kSQFwgjuRs3sNPRGpu2Y0XUJIOTlB1Zx6cWWz4yGCeHYJni1AuXbG3PfOm9i7oJxQs9Fwe0nwivoluCzZTIsu%252BbO%252BbVY72hCZvgef2Eo%252FjEJOjL%252Fgtdw4mnnaCSHqsCdv9PxqTpqHN0syPMPbyPdTxPZ4xdz%252BsaxEtGjNKeudgfY0ak0h6EafmQL0AJkeGiac9ZMNQvVhztVu%252FrBz3ugJzzqQ2hhyfg%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A48%26version%3D1.0", "payRequestId": "RM20210707203648208677696905325t"}, "success": true}</t>
         </is>
       </c>
       <c r="F8" s="10" t="n">
@@ -6100,12 +6100,12 @@
       </c>
       <c r="D9" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "EwDh9akcBnAkcQHmAokeDT", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 99999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "bb28f5c8a8e50c14ea14583491a609d9", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "oWnblthfesrHE7FO5j6xQIRGDJaMVwAC", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "6nwy5BL1owFTAneVQdEdhu", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 99999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "4fd5e2c058c24e2129e858fe3df61f4a", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "k2uJBWl6P8s1frA4F5gMoQnGpUHNXqex"}</t>
         </is>
       </c>
       <c r="E9" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"177bde355050415aadd13756ac9d2b3c\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1259634601\",\"prepayid\":\"wx1710150501168770d6b5c4f3b9b9ec0000\",\"sign\":\"A10CAEAFBF9DAD8D1B63AF8D7EF9D5F8\",\"timestamp\":\"1623896105\"}", "payRequestId": "RM20210617101418208677696923552t"}, "success": true}</t>
+          <t>{"data": {"channelData": "{\"appid\":\"wx93eea96ecc33f168\",\"noncestr\":\"a16dbd275119427b878ce5134ba0d998\",\"packageNm\":\"Sign=WXPay\",\"partnerid\":\"1259634601\",\"prepayid\":\"wx07203649089276696b194a1de4854e0000\",\"sign\":\"7D407762BDA9C0682158D1777FE0667C\",\"timestamp\":\"1625661409\"}", "payRequestId": "RM20210707203648208677696977806t"}, "success": true}</t>
         </is>
       </c>
       <c r="F9" s="10" t="n">
@@ -6143,12 +6143,12 @@
       </c>
       <c r="D10" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "54zCYTtHnftRGdVEh1dYSW", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 999999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "7003aaf4ebd247dd32c2381295b4dcc8", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "ePsoyfLwAOMKQiD7rjgWkuUZc8bhaHmV", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "ToHCgSQ4tNAmfC6fjZqtcT", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 999999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "de467731f3c5be4f408c160bb04118c0", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "UJ50W49ly7j8HtkKpZA2zmhw31fDSM6n"}</t>
         </is>
       </c>
       <c r="E10" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202106171015056726718106782271%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210617095157208677696920006t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25229999999.99%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DeBqBWA%252B0Byf6cv3BC91uM%252FiYFVNON%252FbjRbP2X0k3%252FaUDAE4PL9bq0qrohaMmqqdEa3jgKa1YzM1mdK6%252FcN2PjZcGG7hOkEaNRHIz75wA%252BWBcxMryRKzcz7sy4FGq8NN%252BwOxaz5hIVv6BnN4cHO7vFFAFF2hSz9jpNuGatL0BvNZF4KnaVcwP%252FQpJ%252FN2lcYz8cPRChTgZxXzCXIIl0cHOlEUN%252FaR7%252BH6n0qH%252F%252FcyO6c1lem7jFtmAB4M0O9Esfp%252B7YrY7qZ3kI3mLL%252FpbJ2Bl3LwCY1j3XI44BG0Sl9foCiORUv2%252FNvOh9XOmGbuMJ1OjkPvs50jspOhUUZ%252F4TJ4hjg%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A05%26version%3D1.0", "payRequestId": "RM20210617095157208677696920006t"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202107072036492681454521883681%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210707203649208677696957738t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25229999999.99%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DMs9C76hgGhJVl2BOi6LlBAjK9KwjiTwF1T7fp9FGnoFuzJufnibuZ0g9R%252BYZ1K%252F9flRUObO99I8033XIjvzP6M%252B9xlb3DUEe6SSfSa10czYHGQsC1LW88jr8kw2%252BAGkZ4tCADNHadaF8J9CFeEoUvpqTZtjkM3dHp9dZZZa9l05Z9WpQTsSKp%252BnaJf6%252F2%252BEMLyT5sthn0p1V4VdZlqmP%252FJuBrXmmQXRg%252BYzpUdaObMz0VLvn96FAwbQ4BVClofQcdaRpJy82V6jC6UXvohqYYKV2AT5f4IyFB3ot%252B8hZQiZFm2G3z2PBb52YZ%252BQ%252FjDa692M2u7gsXzmslqm3PDnHzQ%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A49%26version%3D1.0", "payRequestId": "RM20210707203649208677696957738t"}, "success": true}</t>
         </is>
       </c>
       <c r="F10" s="10" t="n">
@@ -6186,7 +6186,7 @@
       </c>
       <c r="D11" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "EwDh9akcBnAkcQHmAokeDT", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 9999999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "6a5d717a82c697c8ce7d8f865372f046", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "zfRyW4UQBAc7lDPXmw9ohraGdVNEHKY2", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "9mgnxajoYqFDcBqxFt2kah", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 9999999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "9008e7035bb0c008702daa73bea60ece", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "Fn4o2kmUypgTq6Js0Pa1XcuBS3VRz9Ax"}</t>
         </is>
       </c>
       <c r="E11" s="7" t="inlineStr">
@@ -6231,12 +6231,12 @@
       </c>
       <c r="D12" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "HRrXS1dm5f6h4CgtPenLjDUMKAi0oYxl", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "EwDh9akcBnAkcQHmAokeDT", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 2147483647, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "6a5d717a82c697c8ce7d8f865372f046", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "70pbh26a1jdNLSFtYguzeyGJXmMr4qsK", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "7gQ2SnnfGXBabbE7SnMwb2", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 2147483647, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "cbfc6054b2408e33cd8d73db0dfe1352", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "hiE91otUAs8WDnpPBSJuqaVzRIg5fHMN"}</t>
         </is>
       </c>
       <c r="E12" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "100", "message": "SYSTEM_ERROR"}, "success": false}</t>
+          <t>{"data": {"channelData": "璇锋眰澶辫触,璇锋崲鍏朵粬鏀粯鏂瑰紡", "payRequestId": "RM20210707203647208677696967108t"}, "success": true}</t>
         </is>
       </c>
       <c r="F12" s="10" t="n">
@@ -6274,12 +6274,12 @@
       </c>
       <c r="D13" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "1yguL58RprMaYmzfJHESPsFiblw97kDX", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "9MdfqCU1bfkSa65C1aaCUE", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "df33ace2b27b541ae361846708428166", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "UeEKQbno2ZYwgdqA7jxa3R51PGpCvuiW", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "L5WAER6vfT2QZxQB2NTtvc", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "576d04808cf28754cd4ed4fb1d958d11", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "e1lR3fVF4WhgNbnaLSvI7ErzAx6jCoyK"}</t>
         </is>
       </c>
       <c r="E13" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "璇锋眰澶辫触,璇锋崲鍏朵粬鏀粯鏂瑰紡", "payRequestId": "RM20210617095352208677696902625t"}, "success": true}</t>
+          <t>{"data": {"channelData": "璇锋眰澶辫触,璇锋崲鍏朵粬鏀粯鏂瑰紡", "payRequestId": "RM20210707203651208677696974062t"}, "success": true}</t>
         </is>
       </c>
       <c r="F13" s="10" t="n">
@@ -6317,12 +6317,12 @@
       </c>
       <c r="D14" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "M12IxbL5ZGm3VBtKN098eac4QzAuElkq", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "wxpay", "processToken": "TWp7bmug8eQ8bLg6VA6HH7", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "dfe58eab629b526558800d552d5b89ed", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "L6slha09TAk5tKpyeNHQ12EBgvGJ7PrO", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "wxpay", "processToken": "F3CiwWb3ZusWFYXKgUBeor", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "614a410176d7f9eeb60b3fa435a521a7", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "rLMOV7RlQnYhXibpkdJPZcfqCTej1Ew6"}</t>
         </is>
       </c>
       <c r="E14" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "5b78394918f6940f0febc1f2c0270ac36c2f2a8d65104bb0b3bc03c6c3b712eb1623896105Qx5JCNU1JDs7IoN8x1E1aaTDp7tR9SP3", "payRequestId": "SN202106171015056314800726472770"}, "success": true}</t>
+          <t>{"data": {"channelData": "dbd5edafe410f34e7b027d43fca9d83e8007ea4e5ec5fc4b97c74e7a364d8c481625661409XFjKGCWp9Ni8GYnFBuGlZFmQl1kRLUAp", "payRequestId": "SN202107072036495405581016457805"}, "success": true}</t>
         </is>
       </c>
       <c r="F14" s="10" t="n">
@@ -6358,12 +6358,12 @@
       </c>
       <c r="D15" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "M12IxbL5ZGm3VBtKN098eac4QzAuElkq", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "alipay", "processToken": "5NNAC5ufFogMSRvwg1jLHu", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "0c1df6ecad5c55b1dcb58ee7ff8b276f", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "0PjZaYHVqgXT6dlchtzO5SRJ3rQLAIUm", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "alipay", "processToken": "CuYXrqLnkxVR5K6tKnCcEA", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "13dacb2333dd852978a45b6d860f94d2", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "d13aepFIsRChjiJDkwtXyNrcE8Bz92lu"}</t>
         </is>
       </c>
       <c r="E15" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=60000157&amp;appClearTop=false&amp;startMultApp=YES&amp;sign_params=alipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522access_params%2522%253A%257B%2522channel%2522%253A%2522ALIPAYAPP%2522%257D%252C%2522external_agreement_no%2522%253A%2522SN202106171015052123824386020105%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.user.agreement.page.sign%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidnotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DlxgA1bYg8vSFGdXtKRyE3og6zK6Upq3KUlAh42QRaEZoyx%252BwTpA71zbJXnzBQlZCikoupraA0v%252FvKsVM2H%252BTKVLe3B7x1QSNtwV6T%252Boso%252B5Bb%252F9qJ9%252BJ%252B5lNoWh4otIKhJk4vEP9H0wNutiyGIDII%252Bjbrg9vwLe5LksEnsazla1aiQzoMWcx0exwml%252ByHzI22peamn0o0zkSaRGDvj1XHDlBulF5fTyNe3Rgc%252Byh83CaZ%252B1czpB0yOEQm60SlT0IPBMkLmim7hcCl4kEwfrGSWl4qLNgd14DSeqPoJrELTsmvQoiEragNJuxWyH2y4gyeQAGP%252B5SsI2oGrIFO6R6Qw%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A05%26version%3D1.0", "payRequestId": "SN202106171015055807817251150378"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=60000157&amp;appClearTop=false&amp;startMultApp=YES&amp;sign_params=alipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522access_params%2522%253A%257B%2522channel%2522%253A%2522ALIPAYAPP%2522%257D%252C%2522external_agreement_no%2522%253A%2522SN202107072036493282238526380844%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.user.agreement.page.sign%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidnotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3Dh0Pk0F372Gl%252Fmwchl4IQu4M248jTFNfTEFwfb9YHmJfWD%252F1Gtc%252FqVQeCIQd9EgVP%252BmGG3tx6QE4Iw9jyJg9ilCvm5bVFgTExpDAuez1cOwYSMEc9BVU%252BSgCw7mQvabOOvQZ61aaj1cla31uCQC6CPNhFQLey791dDGZDy9e3RoMxFyvpF3P8XM5YKjsYy29oHwnYsuyoOdaZ3AVEmUdmVt9gXKB7ucTxkroEv0mLRAvTzlqnmVtf0nxOhJUINqku9bpe4QjK36g58qStVc7mMq6T1VnIqueouMBQ1wYHrIqR7GzfdSyGezP8HCa9JXWQX%252FNmR4vo%252BO01LRMJXt8glw%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A49%26version%3D1.0", "payRequestId": "SN202107072036496283745335188044"}, "success": true}</t>
         </is>
       </c>
       <c r="F15" s="10" t="n">
@@ -6399,12 +6399,12 @@
       </c>
       <c r="D16" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "M12IxbL5ZGm3VBtKN098eac4QzAuElkq", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "wxpay", "processToken": "HwGxyPHpfQCj4ApdChPiAT", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 99999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "2759c974ccd652e944914f6ce16f910d", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "kw5N3jiXahcy2PBtrm0SuDxqUIfvoYdO", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "wxpay", "processToken": "QfKcTYkUkTLfHSn6z6468B", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 99999999, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "cca6b79e207c337737f8971d9a8724bb", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "0MkvNzVRUJhqCL67lPmdo12O4nSKZTpw"}</t>
         </is>
       </c>
       <c r="E16" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "282cc7b30b00d08dec9869fabb6790d3117be73f3bd60e123d473bac21a0fde51623896105YD2WAajVQo6Z6cj95A0rbxTgPMA4dDxm", "payRequestId": "SN202106171015057111362128624121"}, "success": true}</t>
+          <t>{"data": {"channelData": "5d44005d063acac96638d3a3e55b320755daf6637bd7f2e9a214d188ecf40dd116256614107kJZVzQlOQ8FpwW8DMghOwOhA85N3U3a", "payRequestId": "SN202107072036503311415428240533"}, "success": true}</t>
         </is>
       </c>
       <c r="F16" s="10" t="n">
@@ -6442,12 +6442,12 @@
       </c>
       <c r="D17" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "M12IxbL5ZGm3VBtKN098eac4QzAuElkq", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "alipay", "processToken": "5tyqPsYX5i6MNXX4Mvnwhf", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "37aff68fda1aab354cf1bde1adcb9519", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "vFtVXQ6rxMSuNR25CqnhW9g8lPmOeGAE", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGN", "payType": "alipay", "processToken": "DqDxn1mpio6qTvrV7bifCw", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "a1c7b3b301025e25af0577d09e4acce6", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "maUeGYQ7rHTtsBF6Mx8WnyCRfVPE1kpL"}</t>
         </is>
       </c>
       <c r="E17" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=60000157&amp;appClearTop=false&amp;startMultApp=YES&amp;sign_params=alipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522access_params%2522%253A%257B%2522channel%2522%253A%2522ALIPAYAPP%2522%257D%252C%2522external_agreement_no%2522%253A%2522SN202106171015050101404686282887%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.user.agreement.page.sign%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidnotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DKEkoy8Zu243K%252BZoxaTYHGO0mzhGU0sUTdkeldTFFTE4hRsoOwuXG4A8KN3jmNcSsbWHNqz29byR8QHnfHib%252F1PGTeYegQ2wYGC%252BQ%252FsX83IWw8fhrp2%252FuJlcxoE6B3Ljau%252F%252BOIZY9e3KGbqevjQRwTLLSeXtNfwvDTNheXaf2pV3VcGME1P%252Ffu7BfWuKQS0h7ZS%252BeGYzgU2pmTHhQCIEEpSPf4q2XUyAQU44s7hceufm7YP6FNcuv%252FXQO%252FnaqoYkDDHiDK2xEdVE4HSgF6Dqygh1OgBjpB15p7dEA4Wx8G52YI9SpBsWRCt9KeNuXQh8ImEN3upo3S8JOAnJuKNDf2g%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A05%26version%3D1.0", "payRequestId": "SN202106171015050622465326102816"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=60000157&amp;appClearTop=false&amp;startMultApp=YES&amp;sign_params=alipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522access_params%2522%253A%257B%2522channel%2522%253A%2522ALIPAYAPP%2522%257D%252C%2522external_agreement_no%2522%253A%2522SN202107072036503421706758688208%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.user.agreement.page.sign%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidnotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3Detj4oTyRE%252F%252FIL2du3XToKuS2xjVLaCwciNZr821a%252FoSDcp35%252BKaF6nqcYulbQ%252BHtqLG8VY%252FbJ%252FCPV%252Fg3MhGVXvdmbNu4Gihj5%252BgUyYl6%252F4v8m%252FOG%252BPQ%252F0mQ3unxF8IXg6Wow23hbcI8btqJkfrm6rs0%252FFr5D4bWeHKwoTl488YNSW9ExwwJPnFCmzMJICD1IbrNfB6UWWmbQ9GuU598qVMF0HJEV%252BvH701JmITNuW7LoREUfMXWmwi3Bd%252BzHVCCvym1F9ZHMWhx9y4FRqPYDaexS26fcBjFhWXEWq6%252B8nun%252F32g1SFlkD2QJR%252B4tkqlcVUorKl37EbUBIrT1olhlnA%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A50%26version%3D1.0", "payRequestId": "SN202107072036506703572587554548"}, "success": true}</t>
         </is>
       </c>
       <c r="F17" s="10" t="n">
@@ -6485,7 +6485,7 @@
       </c>
       <c r="D18" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "TeCQziMm54vbRwyfVXo0DdGN92SEKIJY", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "1", "processToken": "S7QGbhTsg5VzKdGS2yAE6D", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "fa2de70ee5a0cfc4e615bc0ce869250f", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "q9jZsikfDGJ0UaXmHb37KcLtuTg1NMYo", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "1", "processToken": "UwH9nHZkrMKT6GxfUgYGs9", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "ACROSS", "appKey": "2033", "sign": "1714070d27c3003710f7024644dd525a", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "HtqKwYWjASGdI5C84eZx9RvLEkToi6bB"}</t>
         </is>
       </c>
       <c r="E18" s="7" t="inlineStr">
@@ -6526,12 +6526,12 @@
       </c>
       <c r="D19" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "IG9LkhcoizPCbZWj1MOg4w38BmV5SHt6", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "UzkBJ2bByNyWf4JGfLEzVv", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "1a4481d43bb450d7fcbcf4b8ac87dadd", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "RkP1XVox9ArQ2w6aEudfCOqYG43jNzDc", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "BhQW9LA54rAC95aBhRZXQA", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "2398814bec9845e2cb14ed6fc5d7448f", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "xBAHN2zOe0ZrS1dnJMEFipKu5YgLDaTQ"}</t>
         </is>
       </c>
       <c r="E19" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "璇锋眰澶辫触,璇锋崲鍏朵粬鏀粯鏂瑰紡", "payRequestId": "RM20210617101506208677696951007t"}, "success": true}</t>
+          <t>{"data": {"channelData": "璇锋眰澶辫触,璇锋崲鍏朵粬鏀粯鏂瑰紡", "payRequestId": "RM20210707203651208677696935842t"}, "success": true}</t>
         </is>
       </c>
       <c r="F19" s="10" t="n">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="D20" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "IWPyz5oOCixtg3lDuAH4h2nXLNBradcv", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "Vhr4hSV8mcrJ4Gd8rjR7kV", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "7254e893060e368f61f31731e1437fe2", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "wSlodHtRVI0DK6Uc1ANC3MBhmbea2EGz", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "9tLRjmADNfQMpaYhXsTW9f", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "d2b1937feeb0e3aba755546231a330a4", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "WcxZ34oliFqO9Pg2wSYf7zLQbMXDe5It"}</t>
         </is>
       </c>
       <c r="E20" s="7" t="inlineStr">
@@ -6608,7 +6608,7 @@
       </c>
       <c r="D21" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "IWPyz5oOCixtg3lDuAH4h2nXLNBradcv", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "2mqyUDfvEZyRrDcEJn4Tyh", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "a155f0cc90ea386d19351290a6d9af66", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Jeho45cWqPS8f2Tyk3BlKdY9vQrtxMHs", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "wxpay", "processToken": "ViR6oZcc9bzeXT8WEq5vAA", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "", "desc": "test product description", "screenInfo": "HALF", "appKey": "2033", "sign": "1e00b9a8d1cc1dfab703734bad86cca5", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "G9lX46Egqj1WAxF3PUboeHwsLBQ7yTiZ"}</t>
         </is>
       </c>
       <c r="E21" s="7" t="inlineStr">
@@ -6649,12 +6649,12 @@
       </c>
       <c r="D22" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "3cYSNVxDgUdJ9WvXQfhs72PiM4A5Baty", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "GidkE39pXiu6thH1iCv6Do", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "aaaaaaaaaa", "appKey": "2033", "sign": "bddc681430957278cc533032188520be", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "PAVhI6psLeg53c4CQ1OZykGvqwfrHSBX", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "NfAu9ThuZ1HkDEUmmyGz4G", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "aaaaaaaaaa", "appKey": "2033", "sign": "074e314206d7ac555b9b26d6b33135e3", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "7w9mdNc2PWv5QgLx3nA0XhUEf8GeVTFq"}</t>
         </is>
       </c>
       <c r="E22" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202106171015075006470184483761%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210617094331208677696970708t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DHhEq9fCYXp4bkwy1AMEirr4infq65IgCS2wyCBs%252FWN%252FujtEQk%252F%252FTA29L5iTDaYbunoYSTY%252Bv5as1MDjFqy3O08HXk74XEneatSZNPfsulyLqB28Cg6o4CvJIb%252Bo9M4Lw8myad4U9CcR814UoCltnPTajOqI6HTQkW5COKcyzqIo1DwMnL2xTZnuwihC5muvsfjVBurfb2zLyDv5GpBZMCq8UwpKurnMFyZ7%252B9pS%252FUED24i8y8LNdy5xxh9T%252Bp9VyRa8qr2Oa2DI4JOMF2EUUTwZoWulOBzrV7jlHpMXViB6Q4ApFZDKO3ZPylUPQ1doDjb6lIzrBlRwilqbAMUwe6g%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A07%26version%3D1.0", "payRequestId": "RM20210617094331208677696970708t"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202107072036526422158053676615%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210707203652208677696983686t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DCBICW%252FBQN4t73EHbGcnP4lgmastmXIBxUaumXT%252FQ8Va8J9%252B%252Bt17fRGdWPXaO2ur5V45vtGio6bILNC3N%252FENs0ikVqnoUKpfL6fEwUhfHSFtWQU8lGEa374NVdU5BAzO9W9dg%252FAqaBWWzje9CObTIB6i7vM%252Fj4V%252BJ3MfZvKm0CM859ul4Gl14cCtcUE%252BEer8UwgGwogN4%252FIiNAbO3cVP3rlzlNf%252FloX%252BB6p1E%252FMARMIyQ13YHjQ36cFwE1neGQ5J85XlpxoLXjIRe55sUj%252Bp%252Fxmh%252FNCXj7sRlE8%252BpZUikGeEQk1HEhydX%252BA0D8qCIlxtu8GaHssCcktt4hDYSOw3Q%252BA%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A52%26version%3D1.0", "payRequestId": "RM20210707203652208677696983686t"}, "success": true}</t>
         </is>
       </c>
       <c r="F22" s="10" t="n">
@@ -6690,7 +6690,7 @@
       </c>
       <c r="D23" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "6sZotJEuq9GFapHZVmkgYb", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "585160377187360a418651303d65d441", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "", "partnerCode": "2031", "signPartnerOrder": "YuwArj2WctN5FapQ0TgoGl6UdBKPOfZ7", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "T2hN4ihb4VsGbb2wnSkvgL", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "9aaae6023486a640113e19541b6f51d1", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "o3RNO5zSJriKAML2lQ76enHY8hUqak4C"}</t>
         </is>
       </c>
       <c r="E23" s="7" t="inlineStr">
@@ -6731,7 +6731,7 @@
       </c>
       <c r="D24" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "4nJ4FBj5Bj5oDTiBHPb8fV", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "b9363b1f379abe84d3a719070e714229", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "", "signPartnerOrder": "I1WPOeRyht2MFSrJVGzbXBCilu3wdE7Z", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "2usBf8UyvdXLRf2k1R4q2k", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "b70399ecf86d960b5d2d995a058dc5c2", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "ako0Vv5m4NEcUAQCp6LtXSTM8D7y9RWs"}</t>
         </is>
       </c>
       <c r="E24" s="7" t="inlineStr">
@@ -6772,12 +6772,12 @@
       </c>
       <c r="D25" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "Tpq6BtKp2NvtGtMxwWiqoW", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "b30433acc6b68228a1836d3bf4be1c76", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "ZM5Hf2XVQGT8ayqwdkDImKUpPRovAWS9", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "PdaJ7wsH2u4wbsn5SNQVTf", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "16e34a17b757098e8000428506f1c576", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "IJnychtSOXxda5CHRwBU9AYFozG2e14W"}</t>
         </is>
       </c>
       <c r="E25" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "signPartnerOrder must not be empty"}, "success": false}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202107072036526084360765018406%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210707203652208677696936835t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.00%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DhdMFK49CViZ%252F%252FmrpkPoL%252B%252Bqovt9Bx%252F%252Fa%252BJgsKGxQoRz%252B5jdYGpP%252FPQ2kOTKsG3jlO%252B0SCWgGmOl6Lgv7cS0n7Y3DEtlVZR43sWCNNDiZyH3juJmcOgyTMebUxL%252FOVIgErSm8QoHk0qFwEcn5%252BKMVC00gTPFOD1oPvP7jsBzAC%252FouK1KxEr8LhW4X8BG1V2h0VleK9vNWHCndbZgNs68wlfG54Im3U0we1kHe1KHibElNe6o5LoV83oNJ3FhYkUIv3m5LZV%252FQ%252Fx9eM9m2L1o34rzFM7YB2u6Uq91M4cS8ym06T5fleSNSVm9DPK%252FmYHJhvGZUceQgP8aJd3zRuIwsSA%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A52%26version%3D1.0", "payRequestId": "RM20210707203652208677696936835t"}, "success": true}</t>
         </is>
       </c>
       <c r="F25" s="10" t="n">
@@ -6813,7 +6813,7 @@
       </c>
       <c r="D26" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "LR9M4Pq1BvkTFM9JgkuJsy", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "dd850253ad2e423c4019043461f1b0a8", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "sn4LC8uzfErbO1FyBoaN3iMIe7jmchQg", "appPackage": "", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "XgqCLRBNXt11rFiwCWeqbk", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "726e57201cd7b131ec9206a7e0f542e6", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "gh7v2njUpLxNXAkwCdeZfcW6Hmor1OqM"}</t>
         </is>
       </c>
       <c r="E26" s="7" t="inlineStr">
@@ -6854,7 +6854,7 @@
       </c>
       <c r="D27" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "U22pY9ZL69KM5P85m31MSt", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "a435977a110f3d8a1d5e3df04cd4a798", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "TaDV1RO2hJoGywlZvzLcPSt6u079B8M3", "appPackage": "com.example.pay_demo", "notifyUrl": "", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "HXLhmt1jCrjsBYiDxa22Sk", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "64bab175f8f2b4a4c0892466315d56b4", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "G6itrVOMCqzwfSvnW4Fu9y2eYU1DAlgb"}</t>
         </is>
       </c>
       <c r="E27" s="7" t="inlineStr">
@@ -6895,7 +6895,7 @@
       </c>
       <c r="D28" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "RLXEURnM7LzuVnkCYaCbQP", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "13dbdbc47fd6b19875a05e90d5aaab7d", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Jk0s4l6KBz1DZFGc5r3NbtYnpLQSa2my", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "E3NgJKQ8oXcvtVb8i91ASt", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "33c429c79c955924cfdf4b883d8b6570", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "x3kGFsplD5nOQrzRPgd8T2ucaSwqCIN4"}</t>
         </is>
       </c>
       <c r="E28" s="7" t="inlineStr">
@@ -6936,7 +6936,7 @@
       </c>
       <c r="D29" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "8SDL647kfzth4YX7tYtuf3", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "b38c4f87f8b2a3a56e90fc8cc8793409", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "P0X2SF8xtHnQyfIWdKeVbwiazugrJ5h6", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "L15ReCSanWiafXXJ62tFj4", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "137129617f024a005874775a09653f06", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "3HFYetmcX9pS7hQIJsC2O4blxyvawVBP"}</t>
         </is>
       </c>
       <c r="E29" s="7" t="inlineStr">
@@ -6977,12 +6977,12 @@
       </c>
       <c r="D30" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "Xe6t4HxyAgQ2dPwCJoaFuS1pT0biVlrn", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "1", "payType": "alipay", "processToken": "KULyWS5WjHBfNndthtzrsm", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "4ae4640286fa68fbc8b634469ce36a57", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "G7U3SZ9MpFt1IfJ4niDLTBbuaxAkPdyK", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "1", "payType": "alipay", "processToken": "HRmav8Wr8NV5GoGF34GkRM", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 0, "subject": "test product subject", "desc": "test product description", "screenInfo": "FULL", "appKey": "2033", "sign": "4e7c74434c9412dd4fb84c0e97b2eff6", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "WnrSK1ysd3kA4MjOVl8JiT9B6qoQNu7m"}</t>
         </is>
       </c>
       <c r="E30" s="7" t="inlineStr">
         <is>
-          <t>{"error": {"code": "101", "message": "PARAM_ERROR:%s"}, "success": false}</t>
+          <t>{"error": {"code": "101", "message": "PARAM_ERROR:invalid transtype"}, "success": false}</t>
         </is>
       </c>
       <c r="F30" s="10" t="n">
@@ -7018,12 +7018,12 @@
       </c>
       <c r="D31" s="13" t="inlineStr">
         <is>
-          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "3cYSNVxDgUdJ9WvXQfhs72PiM4A5Baty", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "YGwTFjYDuruPSsmgvFdmJ7", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "aaaaaaaaaa", "appKey": "2033", "sign": "c4b761e963ca4d5d83ef068a01118904", "timestamp": "1623896102036", "nonce": "eAXREQjL"}</t>
+          <t>{"renewProductCode": "20310001", "partnerCode": "2031", "signPartnerOrder": "8PiaLyEGNXUz3bj0dkBqu7QoZxfO261T", "appPackage": "com.example.pay_demo", "notifyUrl": "http://secure.pay-test3.wanyol.com/notify/receiver", "country": "CN", "currency": "CNY", "transType": "SIGNANDPAY", "payType": "alipay", "processToken": "QBJ4LRo3pP7hDExza4FLnd", "thirdPartId": "", "appVersion": "", "subUserId": "", "subUserName": "", "amount": 1, "subject": "test product subject", "desc": "test product description", "screenInfo": "aaaaaaaaaa", "appKey": "2033", "sign": "d0100298002204d545862d34960cfd44", "timestamp": "1625661404973", "nonce": "tDkOPzwV", "partnerOrder": "leDSNTbhguvPYwXqKBc324mVAZyRrL9Q"}</t>
         </is>
       </c>
       <c r="E31" s="7" t="inlineStr">
         <is>
-          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202106171015057347631760868882%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210617094331208677696970708t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DdHP0iSdAL%252FgyGeuOZPTPhqBFlg9NhJLfkhsd7itTQCxDZ3rPQs%252F1rsxzqcUz25Ei2H8QWJc2UBBck2SChtZjFC%252FRWQZZcE23u2RbdVr%252F5finK12SnbTJnlFWQI1i0YbU%252BUxL%252FmaEr3u67ZgAgIl5ZTN%252F8ZS6hJJf0k93NZS7UVFbFxJ0rHekRHpeQlomUiL9kEW9P83hPyLUxJYpzqZmaw1nr3imuECZCK5AxLr8XUe3%252FiTMx8Yuf0bIwdNSsjU4J3emtqkol4e6F5Ue97Jk7v2RCDtrt0MKifMY86ezcTZHVCKEA2aAAaANUTYwZDiioU2o5WdBNdPn8VvsR6GNog%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-06-17%2B10%253A15%253A05%26version%3D1.0", "payRequestId": "RM20210617094331208677696970708t"}, "success": true}</t>
+          <t>{"data": {"channelData": "alipays://platformapi/startapp?appId=20000067&amp;url=https%3A%2F%2Fopenapi.alipay.com%2Fgateway.do%3Falipay_sdk%3Dalipay-sdk-java-dynamicVersionNo%26app_id%3D2016120904060189%26biz_content%3D%257B%2522agreement_sign_params%2522%253A%257B%2522external_agreement_no%2522%253A%2522SN202107072036503215860113231512%2522%252C%2522personal_product_code%2522%253A%2522GENERAL_WITHHOLDING_P%2522%252C%2522sign_scene%2522%253A%2522INDUSTRY%257CGAME_CHARGE%2522%257D%252C%2522body%2522%253A%2522test%2Bproduct%2Bdescription%2522%252C%2522integration_type%2522%253A%2522ALIAPP%2522%252C%2522out_trade_no%2522%253A%2522RM20210707203650208677696934474t%2522%252C%2522product_code%2522%253A%2522GENERAL_WITHHOLDING%2522%252C%2522subject%2522%253A%2522test%2Bproduct%2Bsubject%2522%252C%2522total_amount%2522%253A%25220.01%2522%257D%26charset%3DUTF-8%26format%3Djson%26method%3Dalipay.trade.page.pay%26notify_url%3Dhttp%253A%252F%252Fopaycenter-secure-test3.wanyol.com%252Fopaycenter%252Falipayavoidpaynotifynew%26return_url%3Dkekepay%253A%252F%252Fcallback%252Faliautorenew%26sign%3DOar5XKsebbt7QlYRO4wppoCYkKGvmfv5H3lE7A2k%252Bkj2ojzJ0sOKSN42b1wKQbYjrHLKefGwN%252FUSaw27fgOuAHXgGlCi6HTeVSI6z7xLvq9j%252BxkBulHVy53QP7y%252B9yyNBWMh3kMLx9LGTtYnrAY6dYSxDRb8xxVMPa2FV%252FVSgMFVJY0m193CviWezAG3o4lfSbUh%252BFSSuuZqKiqpRwmWX9yL%252BJ%252F130knCMZPtQREkPdV8kisS%252FDzK7K4jtqNcBEWaE%252BJe%252Bo5i%252BNAYQW4S0Pkdog1px1gUnq12RjiHKSRxm%252B2pURZw7N4RZwlme%252BMf4FSJFz93DVZtAk4M%252Bc5lrnArA%253D%253D%26sign_type%3DRSA2%26timestamp%3D2021-07-07%2B20%253A36%253A50%26version%3D1.0", "payRequestId": "RM20210707203650208677696934474t"}, "success": true}</t>
         </is>
       </c>
       <c r="F31" s="10" t="n">
@@ -10602,21 +10602,21 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col width="20.5" customWidth="1" style="1" min="1" max="1"/>
-    <col width="19" customWidth="1" style="1" min="2" max="2"/>
-    <col width="13.4416666666667" customWidth="1" style="1" min="3" max="3"/>
-    <col width="50" customWidth="1" style="1" min="4" max="4"/>
-    <col width="45.6666666666667" customWidth="1" style="1" min="5" max="5"/>
-    <col width="13.775" customWidth="1" style="1" min="6" max="6"/>
-    <col width="25.375" customWidth="1" style="1" min="7" max="7"/>
+    <col width="33.5" customWidth="1" style="1" min="1" max="1"/>
+    <col width="18.5" customWidth="1" style="1" min="2" max="2"/>
+    <col width="9.625" customWidth="1" style="1" min="3" max="3"/>
+    <col width="63.625" customWidth="1" style="1" min="4" max="4"/>
+    <col width="43.375" customWidth="1" style="1" min="5" max="5"/>
+    <col width="11.875" customWidth="1" style="1" min="6" max="6"/>
+    <col width="18.625" customWidth="1" style="1" min="7" max="7"/>
     <col width="15.6666666666667" customWidth="1" style="1" min="8" max="8"/>
     <col width="21.1083333333333" customWidth="1" style="1" min="9" max="9"/>
   </cols>
@@ -10720,10 +10720,10 @@
         </is>
       </c>
     </row>
-    <row r="7" ht="50" customHeight="1" s="1">
+    <row r="7" ht="54" customHeight="1" s="1">
       <c r="A7" s="7" t="inlineStr">
         <is>
-          <t>支付apk获取凭证</t>
+          <t>有账号支付apk获取凭证</t>
         </is>
       </c>
       <c r="B7" s="18" t="inlineStr">
@@ -10738,12 +10738,12 @@
       </c>
       <c r="D7" s="19" t="inlineStr">
         <is>
-          <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
+          <t>{"token": "TOKEN_7t5kusT0owaYVytvYSs24PqfTvPRfYTSqbeurVd0X+rI8Kyt08nE1Ih5lgZHhNtr","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
       <c r="E7" s="20" t="inlineStr">
         <is>
-          <t>{"data": {"expireTime": 1622535182059, "processToken": "R8xpwHnvizRZwCMEZvtn8f"}, "success": true}</t>
+          <t>{"data": {"expireTime": 1625741400336, "processToken": "SzyEphsdNHSRKWbaRUcPH7"}, "success": true}</t>
         </is>
       </c>
       <c r="F7" s="10" t="n">
@@ -10761,10 +10761,10 @@
       </c>
       <c r="I7" s="11" t="n"/>
     </row>
-    <row r="8" ht="50" customHeight="1" s="1">
+    <row r="8" ht="54" customHeight="1" s="1">
       <c r="A8" s="7" t="inlineStr">
         <is>
-          <t>msp获取凭证</t>
+          <t>有账号msp获取凭证</t>
         </is>
       </c>
       <c r="B8" s="18" t="inlineStr">
@@ -10779,12 +10779,12 @@
       </c>
       <c r="D8" s="19" t="inlineStr">
         <is>
-          <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
+          <t>{"token": "TOKEN_7t5kusT0owaYVytvYSs24PqfTvPRfYTSqbeurVd0X+rI8Kyt08nE1Ih5lgZHhNtr","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
         </is>
       </c>
       <c r="E8" s="20" t="inlineStr">
         <is>
-          <t>{"data": {"expireTime": 1622535182343, "processToken": "6y3QWma3bUuysLdJy3tydC"}, "success": true}</t>
+          <t>{"error": {"code": "100", "message": "SYSTEM_ERROR"}, "success": false}</t>
         </is>
       </c>
       <c r="F8" s="10" t="n">
@@ -10797,256 +10797,338 @@
       </c>
       <c r="H8" s="22" t="inlineStr">
         <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="I8" s="11" t="n"/>
+    </row>
+    <row r="9" ht="40.5" customHeight="1" s="1">
+      <c r="A9" s="7" t="inlineStr">
+        <is>
+          <t>掌阅无账号获取凭证</t>
+        </is>
+      </c>
+      <c r="B9" s="18" t="inlineStr">
+        <is>
+          <t>smoke</t>
+        </is>
+      </c>
+      <c r="C9" s="8" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="D9" s="19" t="inlineStr">
+        <is>
+          <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "20242209","platform": "ATLAS"}</t>
+        </is>
+      </c>
+      <c r="E9" s="20" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1625741400394, "processToken": "CcwDZshqdPt97Dbtt8YWUa"}, "success": true}</t>
+        </is>
+      </c>
+      <c r="F9" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G9" s="21" t="inlineStr">
+        <is>
+          <t>{"success": true}</t>
+        </is>
+      </c>
+      <c r="H9" s="22" t="inlineStr">
+        <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I8" s="11" t="n"/>
-    </row>
-    <row r="9" ht="50" customHeight="1" s="1">
-      <c r="A9" s="7" t="inlineStr">
-        <is>
-          <t>apk无账号获取凭证</t>
-        </is>
-      </c>
-      <c r="B9" s="18" t="inlineStr">
+      <c r="I9" s="11" t="n"/>
+    </row>
+    <row r="10" ht="40.5" customHeight="1" s="1">
+      <c r="A10" s="7" t="inlineStr">
+        <is>
+          <t>单机游戏无账号获取凭证</t>
+        </is>
+      </c>
+      <c r="B10" s="18" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
       </c>
-      <c r="C9" s="8" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="D9" s="19" t="inlineStr">
-        <is>
-          <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
-        </is>
-      </c>
-      <c r="E9" s="20" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1622535182383, "processToken": "PQ81y37GJtXs7TzvY48Vr6"}, "success": true}</t>
-        </is>
-      </c>
-      <c r="F9" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G9" s="21" t="inlineStr">
+      <c r="C10" s="8" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="D10" s="19" t="inlineStr">
+        <is>
+          <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "5456937","platform": "ALTAS"}</t>
+        </is>
+      </c>
+      <c r="E10" s="20" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1625741400436, "processToken": "5ugy8QLaH5urxcuLQUQarc"}, "success": true}</t>
+        </is>
+      </c>
+      <c r="F10" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G10" s="21" t="inlineStr">
         <is>
           <t>{"success": true}</t>
         </is>
       </c>
-      <c r="H9" s="22" t="inlineStr">
+      <c r="H10" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I9" s="11" t="n"/>
-    </row>
-    <row r="10" ht="50" customHeight="1" s="1">
-      <c r="A10" s="7" t="inlineStr">
-        <is>
-          <t>msp无账号获取凭证</t>
-        </is>
-      </c>
-      <c r="B10" s="18" t="inlineStr">
+      <c r="I10" s="11" t="n"/>
+    </row>
+    <row r="11" ht="40.5" customHeight="1" s="1">
+      <c r="A11" s="7" t="inlineStr">
+        <is>
+          <t>MSP-TVPay 无账号获取凭证</t>
+        </is>
+      </c>
+      <c r="B11" s="18" t="inlineStr">
         <is>
           <t>smoke</t>
         </is>
       </c>
-      <c r="C10" s="8" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="D10" s="19" t="inlineStr">
-        <is>
-          <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
-        </is>
-      </c>
-      <c r="E10" s="20" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1622535182420, "processToken": "KPEHTZjGfBUJcNzyAew8Lk"}, "success": true}</t>
-        </is>
-      </c>
-      <c r="F10" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G10" s="21" t="inlineStr">
+      <c r="C11" s="8" t="inlineStr">
+        <is>
+          <t>+</t>
+        </is>
+      </c>
+      <c r="D11" s="19" t="inlineStr">
+        <is>
+          <t>{"token": "","appId": "2031","appPackage": "com.oppo.usercenter", "partnerCode": "2032","platform": "MSP"}</t>
+        </is>
+      </c>
+      <c r="E11" s="20" t="inlineStr">
+        <is>
+          <t>{"error": {"code": "100", "message": "SYSTEM_ERROR"}, "success": false}</t>
+        </is>
+      </c>
+      <c r="F11" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G11" s="21" t="inlineStr">
         <is>
           <t>{"success": true}</t>
         </is>
       </c>
-      <c r="H10" s="22" t="inlineStr">
+      <c r="H11" s="22" t="inlineStr">
+        <is>
+          <t>failed</t>
+        </is>
+      </c>
+      <c r="I11" s="11" t="n"/>
+    </row>
+    <row r="12" ht="54" customHeight="1" s="1">
+      <c r="A12" s="7" t="inlineStr">
+        <is>
+          <t>msp获取凭证不传appId</t>
+        </is>
+      </c>
+      <c r="B12" s="18" t="inlineStr">
+        <is>
+          <t>smoke</t>
+        </is>
+      </c>
+      <c r="C12" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D12" s="19" t="inlineStr">
+        <is>
+          <t>{"token": "TOKEN_7t5kusT0owaYVytvYSs24PqfTvPRfYTSqbeurVd0X+rI8Kyt08nE1Ih5lgZHhNtr","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
+        </is>
+      </c>
+      <c r="E12" s="20" t="inlineStr">
+        <is>
+          <t>{"error": {"code": "100", "message": "SYSTEM_ERROR"}, "success": false}</t>
+        </is>
+      </c>
+      <c r="F12" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G12" s="21" t="inlineStr">
+        <is>
+          <t>{"success": true}</t>
+        </is>
+      </c>
+      <c r="H12" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I10" s="11" t="n"/>
-    </row>
-    <row r="11" ht="50" customHeight="1" s="1">
-      <c r="A11" s="7" t="inlineStr">
-        <is>
-          <t>msp获取凭证不传appId</t>
-        </is>
-      </c>
-      <c r="B11" s="18" t="inlineStr">
-        <is>
-          <t>smoke</t>
-        </is>
-      </c>
-      <c r="C11" s="8" t="inlineStr">
-        <is>
-          <t>+</t>
-        </is>
-      </c>
-      <c r="D11" s="19" t="inlineStr">
-        <is>
-          <t>{"token": "","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "MSP"}</t>
-        </is>
-      </c>
-      <c r="E11" s="20" t="inlineStr">
-        <is>
-          <t>{"data": {"expireTime": 1622535182455, "processToken": "UWYXyAVCQPzJiK3YXMUhxr"}, "success": true}</t>
-        </is>
-      </c>
-      <c r="F11" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G11" s="21" t="inlineStr">
+      <c r="I12" s="11" t="n"/>
+    </row>
+    <row r="13" ht="54" customHeight="1" s="1">
+      <c r="A13" s="7" t="inlineStr">
+        <is>
+          <t>MSP_测试获取凭证，platform=ALTAS</t>
+        </is>
+      </c>
+      <c r="B13" s="18" t="inlineStr">
+        <is>
+          <t>full</t>
+        </is>
+      </c>
+      <c r="C13" s="8" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="D13" s="19" t="inlineStr">
+        <is>
+          <t>{"token": "TOKEN_7t5kusT0owaYVytvYSs24PqfTvPRfYTSqbeurVd0X+rI8Kyt08nE1Ih5lgZHhNtr","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "72724322","platform": "ALTAS"}</t>
+        </is>
+      </c>
+      <c r="E13" s="20" t="inlineStr">
+        <is>
+          <t>{"data": {"expireTime": 1625741402742, "processToken": "SZ2UL6t8m2ur2LjRZmqbvr"}, "success": true}</t>
+        </is>
+      </c>
+      <c r="F13" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G13" s="21" t="inlineStr">
         <is>
           <t>{"success": true}</t>
         </is>
       </c>
-      <c r="H11" s="22" t="inlineStr">
+      <c r="H13" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I11" s="11" t="n"/>
-    </row>
-    <row r="12" ht="50" customHeight="1" s="1">
-      <c r="A12" s="7" t="inlineStr">
+      <c r="I13" s="11" t="n"/>
+    </row>
+    <row r="14" ht="40.5" customHeight="1" s="1">
+      <c r="A14" s="7" t="inlineStr">
         <is>
           <t>token传入不正确</t>
         </is>
       </c>
-      <c r="B12" s="18" t="inlineStr">
+      <c r="B14" s="18" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="C12" s="8" t="inlineStr">
+      <c r="C14" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D12" s="19" t="inlineStr">
+      <c r="D14" s="19" t="inlineStr">
         <is>
           <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E12" s="20" t="inlineStr">
+      <c r="E14" s="20" t="inlineStr">
         <is>
           <t>{"error": {"code": "20000", "message": "鉴权失败"}, "success": false}</t>
         </is>
       </c>
-      <c r="F12" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G12" s="21" t="inlineStr">
+      <c r="F14" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G14" s="21" t="inlineStr">
         <is>
           <t>{"success": false}</t>
         </is>
       </c>
-      <c r="H12" s="22" t="inlineStr">
+      <c r="H14" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I12" s="11" t="n"/>
-    </row>
-    <row r="13" ht="50" customHeight="1" s="1">
-      <c r="A13" s="7" t="inlineStr">
+      <c r="I14" s="11" t="n"/>
+    </row>
+    <row r="15" ht="27" customHeight="1" s="1">
+      <c r="A15" s="7" t="inlineStr">
         <is>
           <t>partnerCode不传</t>
         </is>
       </c>
-      <c r="B13" s="18" t="inlineStr">
+      <c r="B15" s="18" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="C13" s="8" t="inlineStr">
+      <c r="C15" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D13" s="19" t="inlineStr">
+      <c r="D15" s="19" t="inlineStr">
         <is>
           <t>{"token": "error_token","appId": "","appPackage": "com.oppo.usercenter", "partnerCode": "","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E13" s="20" t="inlineStr">
+      <c r="E15" s="20" t="inlineStr">
         <is>
           <t>{"error": {"code": "101", "message": "must not be blank"}, "success": false}</t>
         </is>
       </c>
-      <c r="F13" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G13" s="21" t="inlineStr">
+      <c r="F15" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G15" s="21" t="inlineStr">
         <is>
           <t>{"success": false}</t>
         </is>
       </c>
-      <c r="H13" s="22" t="inlineStr">
+      <c r="H15" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I13" s="11" t="n"/>
-    </row>
-    <row r="14" ht="50" customHeight="1" s="1">
-      <c r="A14" s="7" t="inlineStr">
+      <c r="I15" s="11" t="n"/>
+    </row>
+    <row r="16" ht="27" customHeight="1" s="1">
+      <c r="A16" s="7" t="inlineStr">
         <is>
           <t>appPackage不传</t>
         </is>
       </c>
-      <c r="B14" s="18" t="inlineStr">
+      <c r="B16" s="18" t="inlineStr">
         <is>
           <t>full</t>
         </is>
       </c>
-      <c r="C14" s="8" t="inlineStr">
+      <c r="C16" s="8" t="inlineStr">
         <is>
           <t>-</t>
         </is>
       </c>
-      <c r="D14" s="20" t="inlineStr">
+      <c r="D16" s="20" t="inlineStr">
         <is>
           <t>{"token": "","appId": "","appPackage": "", "partnerCode": "2031","platform": "ATLAS"}</t>
         </is>
       </c>
-      <c r="E14" s="20" t="inlineStr">
+      <c r="E16" s="20" t="inlineStr">
         <is>
           <t>{"error": {"code": "101", "message": "must not be blank"}, "success": false}</t>
         </is>
       </c>
-      <c r="F14" s="10" t="n">
-        <v>200</v>
-      </c>
-      <c r="G14" s="21" t="inlineStr">
+      <c r="F16" s="10" t="n">
+        <v>200</v>
+      </c>
+      <c r="G16" s="21" t="inlineStr">
         <is>
           <t>{"success": false}</t>
         </is>
       </c>
-      <c r="H14" s="22" t="inlineStr">
+      <c r="H16" s="22" t="inlineStr">
         <is>
           <t>passed</t>
         </is>
       </c>
-      <c r="I14" s="11" t="n"/>
+      <c r="I16" s="11" t="n"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>

</xml_diff>